<commit_message>
Forgot the migration file, updated monsters
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="198">
   <si>
     <t>name</t>
   </si>
@@ -451,6 +451,141 @@
   </si>
   <si>
     <t>4200-4500</t>
+  </si>
+  <si>
+    <t>Adult Red Dragon</t>
+  </si>
+  <si>
+    <t>9000-14000</t>
+  </si>
+  <si>
+    <t>4500-6000</t>
+  </si>
+  <si>
+    <t>Litch Lord of the Labyrinth</t>
+  </si>
+  <si>
+    <t>14000-17000</t>
+  </si>
+  <si>
+    <t>6200-8000</t>
+  </si>
+  <si>
+    <t>Whisper of Fate</t>
+  </si>
+  <si>
+    <t>19000-25000</t>
+  </si>
+  <si>
+    <t>9000-12000</t>
+  </si>
+  <si>
+    <t>Demonic Angel</t>
+  </si>
+  <si>
+    <t>25000-30000</t>
+  </si>
+  <si>
+    <t>12300-14500</t>
+  </si>
+  <si>
+    <t>Virgin Priestess Zombie</t>
+  </si>
+  <si>
+    <t>32000-35000</t>
+  </si>
+  <si>
+    <t>15300-18900</t>
+  </si>
+  <si>
+    <t>Hells Paladin</t>
+  </si>
+  <si>
+    <t>35000-41000</t>
+  </si>
+  <si>
+    <t>19000-22500</t>
+  </si>
+  <si>
+    <t>Ancient Gold Dragon</t>
+  </si>
+  <si>
+    <t>41500-4700</t>
+  </si>
+  <si>
+    <t>23000-25000</t>
+  </si>
+  <si>
+    <t>Broken Hearted Banshee</t>
+  </si>
+  <si>
+    <t>47000-50000</t>
+  </si>
+  <si>
+    <t>25500-27000</t>
+  </si>
+  <si>
+    <t>Red Wizard of Krull</t>
+  </si>
+  <si>
+    <t>50000-54000</t>
+  </si>
+  <si>
+    <t>28000-31500</t>
+  </si>
+  <si>
+    <t>Devils Lover</t>
+  </si>
+  <si>
+    <t>55000-59500</t>
+  </si>
+  <si>
+    <t>34000-40000</t>
+  </si>
+  <si>
+    <t>Fabled Princess</t>
+  </si>
+  <si>
+    <t>60400-65700</t>
+  </si>
+  <si>
+    <t>43000-50000</t>
+  </si>
+  <si>
+    <t>Demon Hunter</t>
+  </si>
+  <si>
+    <t>66700-69800</t>
+  </si>
+  <si>
+    <t>66000-70000</t>
+  </si>
+  <si>
+    <t>Cyclops Bat</t>
+  </si>
+  <si>
+    <t>70000-76000</t>
+  </si>
+  <si>
+    <t>75000-83000</t>
+  </si>
+  <si>
+    <t>Water Fiend</t>
+  </si>
+  <si>
+    <t>79500-86700</t>
+  </si>
+  <si>
+    <t>84500-87000</t>
+  </si>
+  <si>
+    <t>Labyrinth Hound</t>
+  </si>
+  <si>
+    <t>89000-94000</t>
+  </si>
+  <si>
+    <t>90000-120000</t>
   </si>
   <si>
     <t>monster_id</t>
@@ -813,7 +948,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -821,13 +956,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="4" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="32" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="6" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="5" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="3" bestFit="true" customWidth="true" style="0"/>
@@ -2998,6 +3133,768 @@
         <v>1</v>
       </c>
       <c r="R42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43">
+        <v>4500</v>
+      </c>
+      <c r="C43">
+        <v>6000</v>
+      </c>
+      <c r="D43">
+        <v>500</v>
+      </c>
+      <c r="E43">
+        <v>6300</v>
+      </c>
+      <c r="F43">
+        <v>6400</v>
+      </c>
+      <c r="G43">
+        <v>450</v>
+      </c>
+      <c r="H43">
+        <v>110</v>
+      </c>
+      <c r="I43" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>10</v>
+      </c>
+      <c r="K43">
+        <v>0.02</v>
+      </c>
+      <c r="L43">
+        <v>1000</v>
+      </c>
+      <c r="M43" t="s">
+        <v>146</v>
+      </c>
+      <c r="N43" t="s">
+        <v>147</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="R43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44">
+        <v>8000</v>
+      </c>
+      <c r="C44">
+        <v>9000</v>
+      </c>
+      <c r="D44">
+        <v>7560</v>
+      </c>
+      <c r="E44">
+        <v>9700</v>
+      </c>
+      <c r="F44">
+        <v>9100</v>
+      </c>
+      <c r="G44">
+        <v>475</v>
+      </c>
+      <c r="H44">
+        <v>160</v>
+      </c>
+      <c r="I44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+      <c r="K44">
+        <v>0.03</v>
+      </c>
+      <c r="L44">
+        <v>1200</v>
+      </c>
+      <c r="M44" t="s">
+        <v>149</v>
+      </c>
+      <c r="N44" t="s">
+        <v>150</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="R44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45">
+        <v>10000</v>
+      </c>
+      <c r="C45">
+        <v>10600</v>
+      </c>
+      <c r="D45">
+        <v>11000</v>
+      </c>
+      <c r="E45">
+        <v>10870</v>
+      </c>
+      <c r="F45">
+        <v>12000</v>
+      </c>
+      <c r="G45">
+        <v>500</v>
+      </c>
+      <c r="H45">
+        <v>200</v>
+      </c>
+      <c r="I45" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>10</v>
+      </c>
+      <c r="K45">
+        <v>0.05</v>
+      </c>
+      <c r="L45">
+        <v>1300</v>
+      </c>
+      <c r="M45" t="s">
+        <v>152</v>
+      </c>
+      <c r="N45" t="s">
+        <v>153</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46">
+        <v>14900</v>
+      </c>
+      <c r="C46">
+        <v>13000</v>
+      </c>
+      <c r="D46">
+        <v>14999</v>
+      </c>
+      <c r="E46">
+        <v>14670</v>
+      </c>
+      <c r="F46">
+        <v>14500</v>
+      </c>
+      <c r="G46">
+        <v>560</v>
+      </c>
+      <c r="H46">
+        <v>253</v>
+      </c>
+      <c r="I46" t="s">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+      <c r="K46">
+        <v>0.03</v>
+      </c>
+      <c r="L46">
+        <v>1600</v>
+      </c>
+      <c r="M46" t="s">
+        <v>155</v>
+      </c>
+      <c r="N46" t="s">
+        <v>156</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="R46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47">
+        <v>16000</v>
+      </c>
+      <c r="C47">
+        <v>14600</v>
+      </c>
+      <c r="D47">
+        <v>15999</v>
+      </c>
+      <c r="E47">
+        <v>16000</v>
+      </c>
+      <c r="F47">
+        <v>16000</v>
+      </c>
+      <c r="G47">
+        <v>620</v>
+      </c>
+      <c r="H47">
+        <v>275</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>10</v>
+      </c>
+      <c r="K47">
+        <v>0.04</v>
+      </c>
+      <c r="L47">
+        <v>1800</v>
+      </c>
+      <c r="M47" t="s">
+        <v>158</v>
+      </c>
+      <c r="N47" t="s">
+        <v>159</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="R47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48">
+        <v>18750</v>
+      </c>
+      <c r="C48">
+        <v>18500</v>
+      </c>
+      <c r="D48">
+        <v>19000</v>
+      </c>
+      <c r="E48">
+        <v>18900</v>
+      </c>
+      <c r="F48">
+        <v>18950</v>
+      </c>
+      <c r="G48">
+        <v>660</v>
+      </c>
+      <c r="H48">
+        <v>325</v>
+      </c>
+      <c r="I48" t="s">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>10</v>
+      </c>
+      <c r="K48">
+        <v>0.01</v>
+      </c>
+      <c r="L48">
+        <v>2000</v>
+      </c>
+      <c r="M48" t="s">
+        <v>161</v>
+      </c>
+      <c r="N48" t="s">
+        <v>162</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="R48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49">
+        <v>22000</v>
+      </c>
+      <c r="C49">
+        <v>22040</v>
+      </c>
+      <c r="D49">
+        <v>21000</v>
+      </c>
+      <c r="E49">
+        <v>21000</v>
+      </c>
+      <c r="F49">
+        <v>2100</v>
+      </c>
+      <c r="G49">
+        <v>690</v>
+      </c>
+      <c r="H49">
+        <v>375</v>
+      </c>
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <v>10</v>
+      </c>
+      <c r="K49">
+        <v>0.04</v>
+      </c>
+      <c r="L49">
+        <v>2200</v>
+      </c>
+      <c r="M49" t="s">
+        <v>164</v>
+      </c>
+      <c r="N49" t="s">
+        <v>165</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50">
+        <v>23000</v>
+      </c>
+      <c r="C50">
+        <v>21000</v>
+      </c>
+      <c r="D50">
+        <v>22000</v>
+      </c>
+      <c r="E50">
+        <v>24000</v>
+      </c>
+      <c r="F50">
+        <v>20000</v>
+      </c>
+      <c r="G50">
+        <v>715</v>
+      </c>
+      <c r="H50">
+        <v>400</v>
+      </c>
+      <c r="I50" t="s">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>10</v>
+      </c>
+      <c r="K50">
+        <v>0.03</v>
+      </c>
+      <c r="L50">
+        <v>2400</v>
+      </c>
+      <c r="M50" t="s">
+        <v>167</v>
+      </c>
+      <c r="N50" t="s">
+        <v>168</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51">
+        <v>24000</v>
+      </c>
+      <c r="C51">
+        <v>23400</v>
+      </c>
+      <c r="D51">
+        <v>25000</v>
+      </c>
+      <c r="E51">
+        <v>24500</v>
+      </c>
+      <c r="F51">
+        <v>2500</v>
+      </c>
+      <c r="G51">
+        <v>745</v>
+      </c>
+      <c r="H51">
+        <v>440</v>
+      </c>
+      <c r="I51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>10</v>
+      </c>
+      <c r="K51">
+        <v>0.01</v>
+      </c>
+      <c r="L51">
+        <v>2600</v>
+      </c>
+      <c r="M51" t="s">
+        <v>170</v>
+      </c>
+      <c r="N51" t="s">
+        <v>171</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="R51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52">
+        <v>25000</v>
+      </c>
+      <c r="C52">
+        <v>27000</v>
+      </c>
+      <c r="D52">
+        <v>26000</v>
+      </c>
+      <c r="E52">
+        <v>25000</v>
+      </c>
+      <c r="F52">
+        <v>28600</v>
+      </c>
+      <c r="G52">
+        <v>800</v>
+      </c>
+      <c r="H52">
+        <v>490</v>
+      </c>
+      <c r="I52" t="s">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>10</v>
+      </c>
+      <c r="K52">
+        <v>0.04</v>
+      </c>
+      <c r="L52">
+        <v>2800</v>
+      </c>
+      <c r="M52" t="s">
+        <v>173</v>
+      </c>
+      <c r="N52" t="s">
+        <v>174</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="R52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53">
+        <v>29000</v>
+      </c>
+      <c r="C53">
+        <v>28000</v>
+      </c>
+      <c r="D53">
+        <v>30600</v>
+      </c>
+      <c r="E53">
+        <v>27000</v>
+      </c>
+      <c r="F53">
+        <v>30000</v>
+      </c>
+      <c r="G53">
+        <v>850</v>
+      </c>
+      <c r="H53">
+        <v>525</v>
+      </c>
+      <c r="I53" t="s">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>15</v>
+      </c>
+      <c r="K53">
+        <v>0.01</v>
+      </c>
+      <c r="L53">
+        <v>3000</v>
+      </c>
+      <c r="M53" t="s">
+        <v>176</v>
+      </c>
+      <c r="N53" t="s">
+        <v>177</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q53">
+        <v>0.15</v>
+      </c>
+      <c r="R53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54">
+        <v>29800</v>
+      </c>
+      <c r="C54">
+        <v>31000</v>
+      </c>
+      <c r="D54">
+        <v>30500</v>
+      </c>
+      <c r="E54">
+        <v>29800</v>
+      </c>
+      <c r="F54">
+        <v>2870</v>
+      </c>
+      <c r="G54">
+        <v>900</v>
+      </c>
+      <c r="H54">
+        <v>550</v>
+      </c>
+      <c r="I54" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>15</v>
+      </c>
+      <c r="K54">
+        <v>0.04</v>
+      </c>
+      <c r="L54">
+        <v>3400</v>
+      </c>
+      <c r="M54" t="s">
+        <v>179</v>
+      </c>
+      <c r="N54" t="s">
+        <v>180</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="R54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55">
+        <v>34000</v>
+      </c>
+      <c r="C55">
+        <v>35000</v>
+      </c>
+      <c r="D55">
+        <v>36000</v>
+      </c>
+      <c r="E55">
+        <v>32000</v>
+      </c>
+      <c r="F55">
+        <v>31000</v>
+      </c>
+      <c r="G55">
+        <v>930</v>
+      </c>
+      <c r="H55">
+        <v>625</v>
+      </c>
+      <c r="I55" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>15</v>
+      </c>
+      <c r="K55">
+        <v>0.03</v>
+      </c>
+      <c r="L55">
+        <v>3500</v>
+      </c>
+      <c r="M55" t="s">
+        <v>182</v>
+      </c>
+      <c r="N55" t="s">
+        <v>183</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="R55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56">
+        <v>36000</v>
+      </c>
+      <c r="C56">
+        <v>35000</v>
+      </c>
+      <c r="D56">
+        <v>38300</v>
+      </c>
+      <c r="E56">
+        <v>34000</v>
+      </c>
+      <c r="F56">
+        <v>34000</v>
+      </c>
+      <c r="G56">
+        <v>950</v>
+      </c>
+      <c r="H56">
+        <v>660</v>
+      </c>
+      <c r="I56" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>15</v>
+      </c>
+      <c r="K56">
+        <v>0.03</v>
+      </c>
+      <c r="L56">
+        <v>3800</v>
+      </c>
+      <c r="M56" t="s">
+        <v>185</v>
+      </c>
+      <c r="N56" t="s">
+        <v>186</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q56">
+        <v>0.15</v>
+      </c>
+      <c r="R56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" t="s">
+        <v>187</v>
+      </c>
+      <c r="B57">
+        <v>38000</v>
+      </c>
+      <c r="C57">
+        <v>40000</v>
+      </c>
+      <c r="D57">
+        <v>39000</v>
+      </c>
+      <c r="E57">
+        <v>43000</v>
+      </c>
+      <c r="F57">
+        <v>43400</v>
+      </c>
+      <c r="G57">
+        <v>1000</v>
+      </c>
+      <c r="H57">
+        <v>750</v>
+      </c>
+      <c r="I57" t="s">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <v>20</v>
+      </c>
+      <c r="K57">
+        <v>0.04</v>
+      </c>
+      <c r="L57">
+        <v>4000</v>
+      </c>
+      <c r="M57" t="s">
+        <v>188</v>
+      </c>
+      <c r="N57" t="s">
+        <v>189</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="R57" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3022,7 +3919,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -3030,7 +3927,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="32" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="22" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="6" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="3" bestFit="true" customWidth="true" style="0"/>
@@ -3041,25 +3938,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>191</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3073,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3087,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3101,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3115,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3129,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3143,7 +4040,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3157,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3171,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3185,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3199,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3213,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3227,7 +4124,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3241,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3255,7 +4152,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3269,7 +4166,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3283,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3297,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3311,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3325,7 +4222,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3339,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3353,7 +4250,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3367,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3381,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3395,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3409,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3423,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3437,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3451,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3465,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -3479,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3493,7 +4390,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3507,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3521,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3535,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3549,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3563,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3577,7 +4474,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3591,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3605,7 +4502,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3619,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3633,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3647,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3661,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3675,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3689,7 +4586,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3703,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3717,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3731,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3745,7 +4642,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3759,7 +4656,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3773,7 +4670,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3787,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3801,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3815,7 +4712,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3829,7 +4726,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3843,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3857,7 +4754,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3871,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3885,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3899,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3913,7 +4810,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3927,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3941,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3955,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3969,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3983,7 +4880,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3997,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -4011,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -4025,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -4039,7 +4936,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -4053,7 +4950,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -4067,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -4081,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -4095,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -4109,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -4123,7 +5020,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -4137,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -4151,7 +5048,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4165,7 +5062,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4179,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4193,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4207,7 +5104,427 @@
         <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>152</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84">
+        <v>17</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85">
+        <v>16</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>148</v>
+      </c>
+      <c r="C86">
+        <v>16</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87">
+        <v>18</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="C88">
+        <v>19</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89">
+        <v>17</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="C90">
+        <v>20</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>154</v>
+      </c>
+      <c r="C91">
+        <v>17</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92">
+        <v>21</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>157</v>
+      </c>
+      <c r="C93">
+        <v>21</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>160</v>
+      </c>
+      <c r="C94">
+        <v>20</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="G94" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>160</v>
+      </c>
+      <c r="C95">
+        <v>20</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="G95" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>163</v>
+      </c>
+      <c r="C96">
+        <v>17</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="G96" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>163</v>
+      </c>
+      <c r="C97">
+        <v>19</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98">
+        <v>24</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="G98" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>166</v>
+      </c>
+      <c r="C99">
+        <v>23</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>169</v>
+      </c>
+      <c r="C100">
+        <v>21</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>169</v>
+      </c>
+      <c r="C101">
+        <v>23</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="G101" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>172</v>
+      </c>
+      <c r="C102">
+        <v>23</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="G102" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>172</v>
+      </c>
+      <c r="C103">
+        <v>22</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="G103" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>175</v>
+      </c>
+      <c r="C104">
+        <v>26</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="G104" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>175</v>
+      </c>
+      <c r="C105">
+        <v>26</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="G105" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>178</v>
+      </c>
+      <c r="C106">
+        <v>24</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="G106" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>178</v>
+      </c>
+      <c r="C107">
+        <v>23</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="G107" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>181</v>
+      </c>
+      <c r="C108">
+        <v>20</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="G108" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>181</v>
+      </c>
+      <c r="C109">
+        <v>25</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110">
+        <v>28</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>184</v>
+      </c>
+      <c r="C111">
+        <v>25</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>187</v>
+      </c>
+      <c r="C112">
+        <v>25</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>187</v>
+      </c>
+      <c r="C113">
+        <v>24</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempting to fix battle formula.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -684,7 +684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -705,12 +705,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -761,7 +755,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,16 +779,16 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11"/>
@@ -1505,19 +1499,19 @@
         <v>57</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>8000</v>
+        <v>3500</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>46</v>
@@ -1555,19 +1549,19 @@
         <v>60</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>25000</v>
+        <v>4580</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>25000</v>
+        <v>4580</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>25000</v>
+        <v>4580</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>25000</v>
+        <v>4580</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>25000</v>
+        <v>4580</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>50</v>
@@ -1611,19 +1605,19 @@
         <v>63</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>75</v>
@@ -1667,19 +1661,19 @@
         <v>66</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>75000</v>
+        <v>16000</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>75000</v>
+        <v>16000</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>75000</v>
+        <v>16000</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>75000</v>
+        <v>16000</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>75000</v>
+        <v>16000</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>90</v>
@@ -1717,19 +1711,19 @@
         <v>69</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>110000</v>
+        <v>32000</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>100</v>
@@ -1767,19 +1761,19 @@
         <v>72</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>157000</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>157000</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>157000</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>157000</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>157000</v>
+        <v>35000</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>35000</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>35000</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>35000</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>110</v>
@@ -1817,19 +1811,19 @@
         <v>75</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>430000</v>
+        <v>37000</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>430000</v>
+        <v>37000</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>430000</v>
+        <v>37000</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>430000</v>
+        <v>37000</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>430000</v>
+        <v>37000</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>120</v>
@@ -1867,19 +1861,19 @@
         <v>78</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>550000</v>
+        <v>55000</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>550000</v>
+        <v>55000</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>550000</v>
+        <v>55000</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>550000</v>
+        <v>55000</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>550000</v>
+        <v>55000</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>140</v>
@@ -1917,19 +1911,19 @@
         <v>81</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>750000</v>
+        <v>59000</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>750000</v>
+        <v>59000</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>750000</v>
+        <v>59000</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>750000</v>
+        <v>59000</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>750000</v>
+        <v>59000</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>130</v>
@@ -1967,19 +1961,19 @@
         <v>84</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>825000</v>
+        <v>68000</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>825000</v>
+        <v>68000</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>825000</v>
+        <v>68000</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>825000</v>
+        <v>68000</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>825000</v>
+        <v>68000</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>140</v>
@@ -2023,19 +2017,19 @@
         <v>88</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>850000</v>
+        <v>72000</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>850000</v>
+        <v>72000</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>850000</v>
+        <v>72000</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>850000</v>
+        <v>72000</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>850000</v>
+        <v>72000</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>145</v>
@@ -2073,19 +2067,19 @@
         <v>91</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>935000</v>
+        <v>75000</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>935000</v>
+        <v>75000</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>935000</v>
+        <v>75000</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>935000</v>
+        <v>75000</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>935000</v>
+        <v>75000</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>155</v>
@@ -2123,19 +2117,19 @@
         <v>94</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>958000</v>
+        <v>120000</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>958000</v>
+        <v>120000</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>958000</v>
+        <v>120000</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>958000</v>
+        <v>120000</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>958000</v>
+        <v>120000</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>160</v>
@@ -2173,19 +2167,19 @@
         <v>97</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>975000</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>975000</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>975000</v>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>975000</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>975000</v>
+        <v>130000</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>130000</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>130000</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>130000</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>130000</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>200</v>
@@ -2223,19 +2217,19 @@
         <v>100</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1000000</v>
+        <v>150000</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>1000000</v>
+        <v>150000</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>1000000</v>
+        <v>150000</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>1000000</v>
+        <v>150000</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>1000000</v>
+        <v>150000</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>230</v>
@@ -2273,19 +2267,19 @@
         <v>103</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2000000</v>
+        <v>180000</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>2000000</v>
+        <v>180000</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>2000000</v>
+        <v>180000</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>2000000</v>
+        <v>180000</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>2000000</v>
+        <v>180000</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>260</v>
@@ -2323,19 +2317,19 @@
         <v>106</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>300</v>
@@ -2373,19 +2367,19 @@
         <v>109</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>3750000</v>
+        <v>5000</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>3750000</v>
+        <v>5000</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>3750000</v>
+        <v>5000</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>3750000</v>
+        <v>5000</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>3750000</v>
+        <v>5000</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>75</v>
@@ -2423,19 +2417,19 @@
         <v>112</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>4000000</v>
+        <v>15000</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>4000000</v>
+        <v>15000</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>4000000</v>
+        <v>15000</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>4000000</v>
+        <v>15000</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>4000000</v>
+        <v>15000</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>85</v>
@@ -2473,19 +2467,19 @@
         <v>115</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>4150000</v>
+        <v>45000</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>4150000</v>
+        <v>45000</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>4150000</v>
+        <v>45000</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>4150000</v>
+        <v>45000</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>4150000</v>
+        <v>45000</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>95</v>
@@ -2523,19 +2517,19 @@
         <v>118</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>4300000</v>
+        <v>49000</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>4300000</v>
+        <v>49000</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>4300000</v>
+        <v>49000</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>4300000</v>
+        <v>49000</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>4300000</v>
+        <v>49000</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>125</v>
@@ -2573,19 +2567,19 @@
         <v>121</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>4580000</v>
+        <v>60000</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>4580000</v>
+        <v>60000</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>4580000</v>
+        <v>60000</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>4580000</v>
+        <v>60000</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>4580000</v>
+        <v>60000</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>150</v>
@@ -2623,19 +2617,19 @@
         <v>124</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>4850000</v>
+        <v>63000</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>4850000</v>
+        <v>63000</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>4850000</v>
+        <v>63000</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>4850000</v>
+        <v>63000</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>4850000</v>
+        <v>63000</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>175</v>
@@ -2673,19 +2667,19 @@
         <v>127</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>5180000</v>
+        <v>75000</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>5180000</v>
+        <v>75000</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>5180000</v>
+        <v>75000</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>5180000</v>
+        <v>75000</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>5180000</v>
+        <v>75000</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>200</v>
@@ -2723,19 +2717,19 @@
         <v>130</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>5300000</v>
+        <v>85000</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>5300000</v>
+        <v>85000</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>5300000</v>
+        <v>85000</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>5300000</v>
+        <v>85000</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>5300000</v>
+        <v>85000</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>260</v>
@@ -2773,19 +2767,19 @@
         <v>133</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>5580000</v>
+        <v>93000</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>5580000</v>
+        <v>93000</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>5580000</v>
+        <v>93000</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>5580000</v>
+        <v>93000</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>5580000</v>
+        <v>93000</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>320</v>
@@ -2823,19 +2817,19 @@
         <v>136</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>5680000</v>
+        <v>125000</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>5680000</v>
+        <v>125000</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>5680000</v>
+        <v>125000</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>5680000</v>
+        <v>125000</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>5680000</v>
+        <v>125000</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>350</v>
@@ -2873,19 +2867,19 @@
         <v>139</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>5835000</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>5835000</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>5835000</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>5835000</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>5835000</v>
+        <v>150000</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>150000</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>150000</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>150000</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>150000</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>375</v>
@@ -2923,19 +2917,19 @@
         <v>142</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>6325800</v>
+        <v>160000</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>6325800</v>
+        <v>160000</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>6325800</v>
+        <v>160000</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>6325800</v>
+        <v>160000</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>6325800</v>
+        <v>160000</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>400</v>
@@ -2973,19 +2967,19 @@
         <v>145</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>6500000</v>
+        <v>170000</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>6500000</v>
+        <v>170000</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>6500000</v>
+        <v>170000</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>6500000</v>
+        <v>170000</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>6500000</v>
+        <v>170000</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>450</v>
@@ -3023,19 +3017,19 @@
         <v>148</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>6850000</v>
+        <v>180000</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>6850000</v>
+        <v>180000</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>6850000</v>
+        <v>180000</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>6850000</v>
+        <v>180000</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>6850000</v>
+        <v>180000</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>475</v>
@@ -3073,19 +3067,19 @@
         <v>151</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>6985000</v>
+        <v>190000</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>6985000</v>
+        <v>190000</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>6985000</v>
+        <v>190000</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>6985000</v>
+        <v>190000</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>6985000</v>
+        <v>190000</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>500</v>
@@ -3123,19 +3117,19 @@
         <v>154</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>7158000</v>
+        <v>225000</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>7158000</v>
+        <v>225000</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>7158000</v>
+        <v>225000</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>7158000</v>
+        <v>225000</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>7158000</v>
+        <v>225000</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>560</v>
@@ -3173,19 +3167,19 @@
         <v>157</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>7485000</v>
+        <v>235000</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>7485000</v>
+        <v>235000</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>7485000</v>
+        <v>235000</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>7485000</v>
+        <v>235000</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>7485000</v>
+        <v>235000</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>620</v>
@@ -3223,19 +3217,19 @@
         <v>160</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>7580000</v>
+        <v>260000</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>7580000</v>
+        <v>260000</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>7580000</v>
+        <v>260000</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>7580000</v>
+        <v>260000</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>7580000</v>
+        <v>260000</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>660</v>
@@ -3272,20 +3266,20 @@
       <c r="A49" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>7950000</v>
+      <c r="B49" s="1" t="n">
+        <v>275000</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>7950000</v>
+        <v>275000</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>7950000</v>
+        <v>275000</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>7950000</v>
+        <v>275000</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>7950000</v>
+        <v>275000</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>690</v>
@@ -3323,19 +3317,19 @@
         <v>166</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>8350000</v>
+        <v>283000</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>8350000</v>
+        <v>283000</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>8350000</v>
+        <v>283000</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>8350000</v>
+        <v>283000</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>8350000</v>
+        <v>283000</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>715</v>
@@ -3373,19 +3367,19 @@
         <v>169</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>8590000</v>
+        <v>285000</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>8590000</v>
+        <v>285000</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>8590000</v>
+        <v>285000</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>8590000</v>
+        <v>285000</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>8590000</v>
+        <v>285000</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>745</v>
@@ -3423,19 +3417,19 @@
         <v>172</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>9158000</v>
+        <v>290000</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>9158000</v>
+        <v>290000</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>9158000</v>
+        <v>290000</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>9158000</v>
+        <v>290000</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>9158000</v>
+        <v>290000</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>800</v>
@@ -3473,19 +3467,19 @@
         <v>175</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>9358000</v>
+        <v>295000</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>9358000</v>
+        <v>295000</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>9358000</v>
+        <v>295000</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>9358000</v>
+        <v>295000</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>9358000</v>
+        <v>295000</v>
       </c>
       <c r="G53" s="0" t="n">
         <v>850</v>
@@ -3529,19 +3523,19 @@
         <v>178</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>9586000</v>
+        <v>300000</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>9586000</v>
+        <v>300000</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>9586000</v>
+        <v>300000</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>9586000</v>
+        <v>300000</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>9586000</v>
+        <v>300000</v>
       </c>
       <c r="G54" s="0" t="n">
         <v>900</v>
@@ -3579,19 +3573,19 @@
         <v>181</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>10250000</v>
+        <v>310000</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>10250000</v>
+        <v>310000</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>10250000</v>
+        <v>310000</v>
       </c>
       <c r="E55" s="1" t="n">
-        <v>10250000</v>
+        <v>310000</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>10250000</v>
+        <v>310000</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>930</v>
@@ -3629,19 +3623,19 @@
         <v>184</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>10500000</v>
+        <v>320000</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>10500000</v>
+        <v>320000</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>10500000</v>
+        <v>320000</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>10500000</v>
+        <v>320000</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>10500000</v>
+        <v>320000</v>
       </c>
       <c r="G56" s="0" t="n">
         <v>950</v>
@@ -3685,19 +3679,19 @@
         <v>187</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>10856000</v>
+        <v>330000</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>10856000</v>
+        <v>330000</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>10856000</v>
+        <v>330000</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>10856000</v>
+        <v>330000</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>10856000</v>
+        <v>330000</v>
       </c>
       <c r="G57" s="0" t="n">
         <v>1000</v>
@@ -3735,19 +3729,19 @@
         <v>190</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>11500000</v>
+        <v>345000</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>11500000</v>
+        <v>345000</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>11500000</v>
+        <v>345000</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>11500000</v>
+        <v>345000</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>11500000</v>
+        <v>345000</v>
       </c>
       <c r="G58" s="0" t="n">
         <v>1050</v>
@@ -3785,19 +3779,19 @@
         <v>193</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>11999999</v>
+        <v>350000</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>11999999</v>
+        <v>350000</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>11999999</v>
+        <v>350000</v>
       </c>
       <c r="E59" s="1" t="n">
-        <v>11999999</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <v>10000000</v>
+        <v>350000</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>350000</v>
       </c>
       <c r="G59" s="0" t="n">
         <v>1120</v>
@@ -3835,19 +3829,19 @@
         <v>196</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>12000000</v>
+        <v>360000</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>12000000</v>
+        <v>360000</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>12000000</v>
+        <v>360000</v>
       </c>
       <c r="E60" s="1" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="F60" s="0" t="n">
-        <v>12000000</v>
+        <v>360000</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>360000</v>
       </c>
       <c r="G60" s="0" t="n">
         <v>1150</v>
@@ -3885,19 +3879,19 @@
         <v>199</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>13000000</v>
+        <v>370000</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>13000000</v>
+        <v>370000</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>13000000</v>
+        <v>370000</v>
       </c>
       <c r="E61" s="1" t="n">
-        <v>13000000</v>
+        <v>370000</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>12999999</v>
+        <v>370000</v>
       </c>
       <c r="G61" s="0" t="n">
         <v>1200</v>
@@ -3935,19 +3929,19 @@
         <v>202</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>14000000</v>
+        <v>380000</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>14000000</v>
+        <v>380000</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>14000000</v>
+        <v>380000</v>
       </c>
       <c r="E62" s="1" t="n">
-        <v>14000000</v>
+        <v>380000</v>
       </c>
       <c r="F62" s="1" t="n">
-        <v>14000000</v>
+        <v>380000</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>1260</v>
@@ -3985,19 +3979,19 @@
         <v>205</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>16000000</v>
+        <v>390000</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>16000000</v>
+        <v>390000</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>16000000</v>
+        <v>390000</v>
       </c>
       <c r="E63" s="1" t="n">
-        <v>16000000</v>
+        <v>390000</v>
       </c>
       <c r="F63" s="1" t="n">
-        <v>16000000</v>
+        <v>390000</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>1300</v>
@@ -4035,19 +4029,19 @@
         <v>208</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>17000000</v>
+        <v>400000</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>17000000</v>
+        <v>400000</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>17000000</v>
+        <v>400000</v>
       </c>
       <c r="E64" s="1" t="n">
-        <v>17000000</v>
+        <v>400000</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>17000000</v>
+        <v>400000</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>1500</v>
@@ -4102,7 +4096,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22"/>

</xml_diff>

<commit_message>
Started fixed the monsters
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -1,22 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C5846A-8D8A-554F-9164-1274CB8BD441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Monsters" sheetId="1" r:id="rId4"/>
-    <sheet name="Monsters Skills" sheetId="2" r:id="rId5"/>
+    <sheet name="Monsters" sheetId="1" r:id="rId1"/>
+    <sheet name="Monsters Skills" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="218">
   <si>
     <t>name</t>
   </si>
@@ -675,14 +691,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -693,28 +704,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1004,39 +1024,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="3" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1092,21 +1103,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>6</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -1148,24 +1159,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>18</v>
@@ -1198,30 +1209,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>12</v>
       </c>
       <c r="H4">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -1248,7 +1259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1298,7 +1309,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1410,7 +1421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1566,7 +1577,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1622,7 +1633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1728,7 +1739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1834,7 +1845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1890,7 +1901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1940,7 +1951,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1990,7 +2001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2040,7 +2051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2090,7 +2101,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -2140,7 +2151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -2190,7 +2201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2246,7 +2257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -2346,7 +2357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -2396,7 +2407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -2446,7 +2457,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2496,7 +2507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -2546,7 +2557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -2596,7 +2607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>109</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2696,7 +2707,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -2796,7 +2807,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -2846,7 +2857,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -2896,7 +2907,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -2946,7 +2957,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -2996,7 +3007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -3046,7 +3057,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -3096,7 +3107,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -3146,7 +3157,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>142</v>
       </c>
@@ -3196,7 +3207,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -3246,7 +3257,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>148</v>
       </c>
@@ -3296,7 +3307,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>151</v>
       </c>
@@ -3346,7 +3357,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>154</v>
       </c>
@@ -3396,7 +3407,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>157</v>
       </c>
@@ -3446,7 +3457,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>160</v>
       </c>
@@ -3496,7 +3507,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>163</v>
       </c>
@@ -3546,7 +3557,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>166</v>
       </c>
@@ -3596,7 +3607,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -3646,7 +3657,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>172</v>
       </c>
@@ -3696,7 +3707,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>175</v>
       </c>
@@ -3752,7 +3763,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>178</v>
       </c>
@@ -3802,7 +3813,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>181</v>
       </c>
@@ -3852,7 +3863,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>184</v>
       </c>
@@ -3908,7 +3919,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -3958,7 +3969,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -4008,7 +4019,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -4058,7 +4069,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>196</v>
       </c>
@@ -4108,7 +4119,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>199</v>
       </c>
@@ -4158,7 +4169,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>202</v>
       </c>
@@ -4208,7 +4219,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>205</v>
       </c>
@@ -4258,7 +4269,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>208</v>
       </c>
@@ -4309,44 +4320,30 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="6" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="3" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -4369,7 +4366,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -4383,7 +4380,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4397,7 +4394,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -4411,7 +4408,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -4425,7 +4422,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4439,7 +4436,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -4453,7 +4450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -4467,7 +4464,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -4481,7 +4478,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -4495,7 +4492,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -4523,7 +4520,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -4537,7 +4534,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -4551,7 +4548,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -4565,7 +4562,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -4579,7 +4576,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -4593,7 +4590,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -4607,7 +4604,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -4621,7 +4618,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -4635,7 +4632,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -4649,7 +4646,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -4663,7 +4660,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -4677,7 +4674,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -4691,7 +4688,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -4705,7 +4702,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -4719,7 +4716,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -4733,7 +4730,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -4747,7 +4744,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -4761,7 +4758,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -4775,7 +4772,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4789,7 +4786,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>66</v>
       </c>
@@ -4803,7 +4800,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -4817,7 +4814,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -4831,7 +4828,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -4845,7 +4842,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -4859,7 +4856,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -4873,7 +4870,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -4887,7 +4884,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -4901,7 +4898,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -4915,7 +4912,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -4929,7 +4926,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -4943,7 +4940,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -4957,7 +4954,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -4971,7 +4968,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -4985,7 +4982,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -4999,7 +4996,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -5013,7 +5010,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -5027,7 +5024,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -5041,7 +5038,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -5055,7 +5052,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -5069,7 +5066,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -5083,7 +5080,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -5097,7 +5094,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -5111,7 +5108,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -5125,7 +5122,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -5139,7 +5136,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -5153,7 +5150,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -5167,7 +5164,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -5181,7 +5178,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -5195,7 +5192,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>109</v>
       </c>
@@ -5209,7 +5206,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -5223,7 +5220,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -5237,7 +5234,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -5251,7 +5248,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>115</v>
       </c>
@@ -5265,7 +5262,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>118</v>
       </c>
@@ -5279,7 +5276,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -5293,7 +5290,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>121</v>
       </c>
@@ -5307,7 +5304,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -5321,7 +5318,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -5335,7 +5332,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>124</v>
       </c>
@@ -5349,7 +5346,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>127</v>
       </c>
@@ -5363,7 +5360,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>127</v>
       </c>
@@ -5377,7 +5374,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>130</v>
       </c>
@@ -5391,7 +5388,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>130</v>
       </c>
@@ -5405,7 +5402,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>133</v>
       </c>
@@ -5419,7 +5416,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>133</v>
       </c>
@@ -5433,7 +5430,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>136</v>
       </c>
@@ -5447,7 +5444,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>136</v>
       </c>
@@ -5461,7 +5458,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>139</v>
       </c>
@@ -5475,7 +5472,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>139</v>
       </c>
@@ -5489,7 +5486,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>142</v>
       </c>
@@ -5503,7 +5500,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>142</v>
       </c>
@@ -5517,7 +5514,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>145</v>
       </c>
@@ -5531,7 +5528,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>145</v>
       </c>
@@ -5545,7 +5542,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>148</v>
       </c>
@@ -5559,7 +5556,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>148</v>
       </c>
@@ -5573,7 +5570,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>151</v>
       </c>
@@ -5587,7 +5584,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>151</v>
       </c>
@@ -5601,7 +5598,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>154</v>
       </c>
@@ -5615,7 +5612,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>154</v>
       </c>
@@ -5629,7 +5626,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>157</v>
       </c>
@@ -5643,7 +5640,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -5657,7 +5654,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>160</v>
       </c>
@@ -5671,7 +5668,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>160</v>
       </c>
@@ -5685,7 +5682,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>163</v>
       </c>
@@ -5699,7 +5696,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>163</v>
       </c>
@@ -5713,7 +5710,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>166</v>
       </c>
@@ -5727,7 +5724,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>166</v>
       </c>
@@ -5741,7 +5738,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>169</v>
       </c>
@@ -5755,7 +5752,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>169</v>
       </c>
@@ -5769,7 +5766,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>172</v>
       </c>
@@ -5783,7 +5780,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>172</v>
       </c>
@@ -5797,7 +5794,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>175</v>
       </c>
@@ -5811,7 +5808,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>175</v>
       </c>
@@ -5825,7 +5822,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>178</v>
       </c>
@@ -5839,7 +5836,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>178</v>
       </c>
@@ -5853,7 +5850,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>181</v>
       </c>
@@ -5867,7 +5864,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>181</v>
       </c>
@@ -5881,7 +5878,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>184</v>
       </c>
@@ -5895,7 +5892,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>184</v>
       </c>
@@ -5909,7 +5906,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>187</v>
       </c>
@@ -5923,7 +5920,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>187</v>
       </c>
@@ -5937,7 +5934,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>190</v>
       </c>
@@ -5951,7 +5948,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>190</v>
       </c>
@@ -5965,7 +5962,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>193</v>
       </c>
@@ -5979,7 +5976,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>193</v>
       </c>
@@ -5993,7 +5990,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>196</v>
       </c>
@@ -6007,7 +6004,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>196</v>
       </c>
@@ -6021,7 +6018,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>199</v>
       </c>
@@ -6035,7 +6032,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>199</v>
       </c>
@@ -6049,7 +6046,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>202</v>
       </c>
@@ -6063,7 +6060,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>202</v>
       </c>
@@ -6077,7 +6074,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>205</v>
       </c>
@@ -6091,7 +6088,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>205</v>
       </c>
@@ -6105,7 +6102,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -6119,7 +6116,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>208</v>
       </c>
@@ -6134,17 +6131,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed upgrade buildings. Brought over new attack formula from 1.1.0
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -778,7 +778,7 @@
   <dimension ref="A1:R64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="K59" activeCellId="0" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1203,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>80</v>
@@ -1471,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>500</v>
@@ -1539,7 +1539,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>61</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>64</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>67</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>70</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>20</v>
       </c>
       <c r="K59" s="0" t="n">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="L59" s="0" t="n">
         <v>4400</v>

</xml_diff>

<commit_message>
Lots of little fixes for fights and celestial fights.
- Slight changes, adjustments and bug fixes.
- We now do the shop processing for buying in a seperate job.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163E2A38-6BBC-3F43-8B7F-F8EC04AAC984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E9E933-9282-1F4B-874F-0C4F12648F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N70" workbookViewId="0">
-      <selection activeCell="Z103" sqref="Z103"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1276,6 +1276,12 @@
       <c r="I2">
         <v>8</v>
       </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
       <c r="O2">
         <v>3</v>
       </c>
@@ -1356,6 +1362,12 @@
       <c r="I3">
         <v>9</v>
       </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
       <c r="O3">
         <v>5</v>
       </c>
@@ -1430,6 +1442,12 @@
       <c r="I4">
         <v>11</v>
       </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
       <c r="O4">
         <v>9</v>
       </c>
@@ -1504,6 +1522,12 @@
       <c r="I5">
         <v>16</v>
       </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
       <c r="O5">
         <v>8</v>
       </c>
@@ -1578,6 +1602,12 @@
       <c r="I6">
         <v>24</v>
       </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
       <c r="O6">
         <v>14</v>
       </c>
@@ -1658,6 +1688,12 @@
       <c r="I7">
         <v>30</v>
       </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
       <c r="O7">
         <v>25</v>
       </c>
@@ -1738,6 +1774,12 @@
       <c r="I8">
         <v>48</v>
       </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
       <c r="O8">
         <v>40</v>
       </c>
@@ -1818,6 +1860,12 @@
       <c r="I9">
         <v>50</v>
       </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
       <c r="O9">
         <v>60</v>
       </c>
@@ -1892,6 +1940,12 @@
       <c r="I10">
         <v>96</v>
       </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
       <c r="O10">
         <v>100</v>
       </c>
@@ -1972,6 +2026,12 @@
       <c r="I11">
         <v>145</v>
       </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
       <c r="O11">
         <v>140</v>
       </c>
@@ -2052,6 +2112,12 @@
       <c r="I12">
         <v>208</v>
       </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
       <c r="O12">
         <v>200</v>
       </c>
@@ -2132,6 +2198,12 @@
       <c r="I13">
         <v>600</v>
       </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
       <c r="O13">
         <v>260</v>
       </c>
@@ -2206,6 +2278,12 @@
       <c r="I14">
         <v>1000</v>
       </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
       <c r="O14">
         <v>300</v>
       </c>
@@ -2280,6 +2358,12 @@
       <c r="I15">
         <v>2300</v>
       </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
       <c r="O15">
         <v>425</v>
       </c>
@@ -2360,6 +2444,12 @@
       <c r="I16">
         <v>5000</v>
       </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
       <c r="O16">
         <v>490</v>
       </c>
@@ -2434,6 +2524,12 @@
       <c r="I17">
         <v>8000</v>
       </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
       <c r="O17">
         <v>545</v>
       </c>
@@ -2508,6 +2604,12 @@
       <c r="I18">
         <v>12000</v>
       </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
       <c r="O18">
         <v>570</v>
       </c>
@@ -2582,6 +2684,12 @@
       <c r="I19">
         <v>14000</v>
       </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
       <c r="O19">
         <v>610</v>
       </c>
@@ -2656,6 +2764,12 @@
       <c r="I20">
         <v>18000</v>
       </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
       <c r="O20">
         <v>650</v>
       </c>
@@ -2730,6 +2844,12 @@
       <c r="I21">
         <v>24000</v>
       </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
       <c r="O21">
         <v>710</v>
       </c>
@@ -2804,6 +2924,12 @@
       <c r="I22">
         <v>28000</v>
       </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
       <c r="O22">
         <v>750</v>
       </c>
@@ -2884,6 +3010,12 @@
       <c r="I23">
         <v>32000</v>
       </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
       <c r="O23">
         <v>790</v>
       </c>
@@ -2958,6 +3090,12 @@
       <c r="I24">
         <v>38000</v>
       </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
       <c r="O24">
         <v>840</v>
       </c>
@@ -3032,6 +3170,12 @@
       <c r="I25">
         <v>40000</v>
       </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
       <c r="O25">
         <v>870</v>
       </c>
@@ -3106,6 +3250,12 @@
       <c r="I26">
         <v>44000</v>
       </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
       <c r="O26">
         <v>920</v>
       </c>
@@ -3180,6 +3330,12 @@
       <c r="I27">
         <v>45000</v>
       </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
       <c r="O27">
         <v>950</v>
       </c>
@@ -3254,6 +3410,12 @@
       <c r="I28">
         <v>50000</v>
       </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
       <c r="O28">
         <v>970</v>
       </c>
@@ -3328,6 +3490,12 @@
       <c r="I29">
         <v>65000</v>
       </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
       <c r="O29">
         <v>99999</v>
       </c>
@@ -3402,6 +3570,12 @@
       <c r="I30">
         <v>8</v>
       </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
       <c r="O30">
         <v>3</v>
       </c>
@@ -3476,6 +3650,12 @@
       <c r="I31">
         <v>9</v>
       </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
       <c r="O31">
         <v>5</v>
       </c>
@@ -3550,6 +3730,12 @@
       <c r="I32">
         <v>11</v>
       </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
       <c r="O32">
         <v>9</v>
       </c>
@@ -3624,6 +3810,12 @@
       <c r="I33">
         <v>16</v>
       </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
       <c r="O33">
         <v>8</v>
       </c>
@@ -3698,6 +3890,12 @@
       <c r="I34">
         <v>24</v>
       </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
       <c r="O34">
         <v>14</v>
       </c>
@@ -3772,6 +3970,12 @@
       <c r="I35">
         <v>30</v>
       </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
       <c r="O35">
         <v>25</v>
       </c>
@@ -3846,6 +4050,12 @@
       <c r="I36">
         <v>48</v>
       </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
       <c r="O36">
         <v>40</v>
       </c>
@@ -3920,6 +4130,12 @@
       <c r="I37">
         <v>50</v>
       </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
       <c r="O37">
         <v>60</v>
       </c>
@@ -3994,6 +4210,12 @@
       <c r="I38">
         <v>96</v>
       </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
       <c r="O38">
         <v>100</v>
       </c>
@@ -4068,6 +4290,12 @@
       <c r="I39">
         <v>145</v>
       </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
       <c r="O39">
         <v>140</v>
       </c>
@@ -4142,6 +4370,12 @@
       <c r="I40">
         <v>208</v>
       </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
       <c r="O40">
         <v>200</v>
       </c>
@@ -4216,6 +4450,12 @@
       <c r="I41">
         <v>600</v>
       </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
       <c r="O41">
         <v>260</v>
       </c>
@@ -4290,6 +4530,12 @@
       <c r="I42">
         <v>1000</v>
       </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
       <c r="O42">
         <v>300</v>
       </c>
@@ -4364,6 +4610,12 @@
       <c r="I43">
         <v>2300</v>
       </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
       <c r="O43">
         <v>425</v>
       </c>
@@ -4438,6 +4690,12 @@
       <c r="I44">
         <v>2500</v>
       </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
       <c r="O44">
         <v>470</v>
       </c>
@@ -4512,6 +4770,12 @@
       <c r="I45">
         <v>5000</v>
       </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
       <c r="O45">
         <v>490</v>
       </c>
@@ -4586,6 +4850,12 @@
       <c r="I46">
         <v>8000</v>
       </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
       <c r="O46">
         <v>545</v>
       </c>
@@ -4660,6 +4930,12 @@
       <c r="I47">
         <v>12000</v>
       </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
       <c r="O47">
         <v>570</v>
       </c>
@@ -4734,6 +5010,12 @@
       <c r="I48">
         <v>14000</v>
       </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
       <c r="O48">
         <v>610</v>
       </c>
@@ -4808,6 +5090,12 @@
       <c r="I49">
         <v>18000</v>
       </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
       <c r="O49">
         <v>650</v>
       </c>
@@ -4882,6 +5170,12 @@
       <c r="I50">
         <v>24000</v>
       </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
       <c r="O50">
         <v>710</v>
       </c>
@@ -4956,6 +5250,12 @@
       <c r="I51">
         <v>28000</v>
       </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
       <c r="O51">
         <v>750</v>
       </c>
@@ -5030,6 +5330,12 @@
       <c r="I52">
         <v>32000</v>
       </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
       <c r="O52">
         <v>790</v>
       </c>
@@ -5110,6 +5416,12 @@
       <c r="I53">
         <v>38000</v>
       </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
       <c r="O53">
         <v>840</v>
       </c>
@@ -5184,6 +5496,12 @@
       <c r="I54">
         <v>40000</v>
       </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
       <c r="O54">
         <v>870</v>
       </c>
@@ -5258,6 +5576,12 @@
       <c r="I55">
         <v>44000</v>
       </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
       <c r="O55">
         <v>920</v>
       </c>
@@ -5338,6 +5662,12 @@
       <c r="I56">
         <v>45000</v>
       </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
       <c r="O56">
         <v>950</v>
       </c>
@@ -5412,6 +5742,12 @@
       <c r="I57">
         <v>50000</v>
       </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
       <c r="O57">
         <v>970</v>
       </c>
@@ -5486,6 +5822,12 @@
       <c r="I58">
         <v>65000</v>
       </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
       <c r="O58">
         <v>990</v>
       </c>
@@ -5560,6 +5902,12 @@
       <c r="I59">
         <v>68000</v>
       </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
       <c r="O59">
         <v>999</v>
       </c>
@@ -5634,6 +5982,12 @@
       <c r="I60">
         <v>70000</v>
       </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
       <c r="O60">
         <v>99999</v>
       </c>
@@ -5708,6 +6062,12 @@
       <c r="I61">
         <v>80000</v>
       </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
       <c r="O61">
         <v>99999</v>
       </c>
@@ -5782,6 +6142,12 @@
       <c r="I62">
         <v>90000</v>
       </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
       <c r="O62">
         <v>99999</v>
       </c>
@@ -5856,6 +6222,12 @@
       <c r="I63">
         <v>100000</v>
       </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
       <c r="O63">
         <v>99999</v>
       </c>
@@ -6755,6 +7127,12 @@
       <c r="I73">
         <v>8</v>
       </c>
+      <c r="M73">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>1</v>
+      </c>
       <c r="O73">
         <v>3</v>
       </c>
@@ -6829,6 +7207,12 @@
       <c r="I74">
         <v>9</v>
       </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+      <c r="N74">
+        <v>1</v>
+      </c>
       <c r="O74">
         <v>5</v>
       </c>
@@ -6903,6 +7287,12 @@
       <c r="I75">
         <v>11</v>
       </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
       <c r="O75">
         <v>9</v>
       </c>
@@ -6977,6 +7367,12 @@
       <c r="I76">
         <v>16</v>
       </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
       <c r="O76">
         <v>8</v>
       </c>
@@ -7051,6 +7447,12 @@
       <c r="I77">
         <v>24</v>
       </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
       <c r="O77">
         <v>14</v>
       </c>
@@ -7125,6 +7527,12 @@
       <c r="I78">
         <v>30</v>
       </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <v>1</v>
+      </c>
       <c r="O78">
         <v>25</v>
       </c>
@@ -7199,6 +7607,12 @@
       <c r="I79">
         <v>48</v>
       </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
       <c r="O79">
         <v>40</v>
       </c>
@@ -7273,6 +7687,12 @@
       <c r="I80">
         <v>50</v>
       </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>1</v>
+      </c>
       <c r="O80">
         <v>60</v>
       </c>
@@ -7347,6 +7767,12 @@
       <c r="I81">
         <v>96</v>
       </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
       <c r="O81">
         <v>100</v>
       </c>
@@ -7421,6 +7847,12 @@
       <c r="I82">
         <v>145</v>
       </c>
+      <c r="M82">
+        <v>1</v>
+      </c>
+      <c r="N82">
+        <v>1</v>
+      </c>
       <c r="O82">
         <v>140</v>
       </c>
@@ -7495,6 +7927,12 @@
       <c r="I83">
         <v>208</v>
       </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <v>1</v>
+      </c>
       <c r="O83">
         <v>200</v>
       </c>
@@ -7575,6 +8013,12 @@
       <c r="I84">
         <v>600</v>
       </c>
+      <c r="M84">
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
       <c r="O84">
         <v>260</v>
       </c>
@@ -7649,6 +8093,12 @@
       <c r="I85">
         <v>1000</v>
       </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+      <c r="N85">
+        <v>1</v>
+      </c>
       <c r="O85">
         <v>300</v>
       </c>
@@ -7723,6 +8173,12 @@
       <c r="I86">
         <v>2300</v>
       </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
       <c r="O86">
         <v>425</v>
       </c>
@@ -7797,6 +8253,12 @@
       <c r="I87">
         <v>2500</v>
       </c>
+      <c r="M87">
+        <v>1</v>
+      </c>
+      <c r="N87">
+        <v>1</v>
+      </c>
       <c r="O87">
         <v>470</v>
       </c>
@@ -7871,6 +8333,12 @@
       <c r="I88">
         <v>5000</v>
       </c>
+      <c r="M88">
+        <v>1</v>
+      </c>
+      <c r="N88">
+        <v>1</v>
+      </c>
       <c r="O88">
         <v>490</v>
       </c>
@@ -7945,6 +8413,12 @@
       <c r="I89">
         <v>8000</v>
       </c>
+      <c r="M89">
+        <v>1</v>
+      </c>
+      <c r="N89">
+        <v>1</v>
+      </c>
       <c r="O89">
         <v>545</v>
       </c>
@@ -8019,6 +8493,12 @@
       <c r="I90">
         <v>12000</v>
       </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <v>1</v>
+      </c>
       <c r="O90">
         <v>570</v>
       </c>
@@ -8099,6 +8579,12 @@
       <c r="I91">
         <v>14000</v>
       </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
       <c r="O91">
         <v>610</v>
       </c>
@@ -8173,6 +8659,12 @@
       <c r="I92">
         <v>18000</v>
       </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+      <c r="N92">
+        <v>1</v>
+      </c>
       <c r="O92">
         <v>650</v>
       </c>
@@ -8247,6 +8739,12 @@
       <c r="I93">
         <v>24000</v>
       </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
       <c r="O93">
         <v>710</v>
       </c>
@@ -8321,6 +8819,12 @@
       <c r="I94">
         <v>28000</v>
       </c>
+      <c r="M94">
+        <v>1</v>
+      </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
       <c r="O94">
         <v>750</v>
       </c>
@@ -8395,6 +8899,12 @@
       <c r="I95">
         <v>32000</v>
       </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+      <c r="N95">
+        <v>1</v>
+      </c>
       <c r="O95">
         <v>790</v>
       </c>
@@ -8469,6 +8979,12 @@
       <c r="I96">
         <v>38000</v>
       </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <v>1</v>
+      </c>
       <c r="O96">
         <v>840</v>
       </c>
@@ -8543,6 +9059,12 @@
       <c r="I97">
         <v>40000</v>
       </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
       <c r="O97">
         <v>870</v>
       </c>
@@ -8617,6 +9139,12 @@
       <c r="I98">
         <v>44000</v>
       </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
       <c r="O98">
         <v>920</v>
       </c>
@@ -8691,6 +9219,12 @@
       <c r="I99">
         <v>45000</v>
       </c>
+      <c r="M99">
+        <v>1</v>
+      </c>
+      <c r="N99">
+        <v>1</v>
+      </c>
       <c r="O99">
         <v>950</v>
       </c>
@@ -8765,6 +9299,12 @@
       <c r="I100">
         <v>50000</v>
       </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <v>1</v>
+      </c>
       <c r="O100">
         <v>970</v>
       </c>
@@ -8839,6 +9379,12 @@
       <c r="I101">
         <v>65000</v>
       </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <v>1</v>
+      </c>
       <c r="O101">
         <v>990</v>
       </c>
@@ -8913,6 +9459,12 @@
       <c r="I102">
         <v>68000</v>
       </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
       <c r="O102">
         <v>999</v>
       </c>
@@ -8987,6 +9539,12 @@
       <c r="I103">
         <v>70000</v>
       </c>
+      <c r="M103">
+        <v>1</v>
+      </c>
+      <c r="N103">
+        <v>1</v>
+      </c>
       <c r="O103">
         <v>99999</v>
       </c>
@@ -9061,6 +9619,12 @@
       <c r="I104">
         <v>80000</v>
       </c>
+      <c r="M104">
+        <v>1</v>
+      </c>
+      <c r="N104">
+        <v>1</v>
+      </c>
       <c r="O104">
         <v>99999</v>
       </c>
@@ -9135,6 +9699,12 @@
       <c r="I105">
         <v>90000</v>
       </c>
+      <c r="M105">
+        <v>1</v>
+      </c>
+      <c r="N105">
+        <v>1</v>
+      </c>
       <c r="O105">
         <v>99999</v>
       </c>
@@ -9208,6 +9778,12 @@
       </c>
       <c r="I106">
         <v>100000</v>
+      </c>
+      <c r="M106">
+        <v>1</v>
+      </c>
+      <c r="N106">
+        <v>1</v>
       </c>
       <c r="O106">
         <v>99999</v>

</xml_diff>

<commit_message>
Front end can now cast for their attack
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99661DD7-A529-6343-B728-A9B0DD7FC59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556A4BB4-F3AD-CB4D-AD22-F0C24511AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="337">
   <si>
     <t>name</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Demon Imp</t>
-  </si>
-  <si>
-    <t>fous</t>
   </si>
   <si>
     <t>10-20</t>
@@ -1386,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="S104" sqref="S104"/>
+    <sheetView tabSelected="1" topLeftCell="M25" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="T5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="U5">
         <v>3</v>
@@ -1924,10 +1921,10 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AA5">
         <v>3</v>
@@ -1965,7 +1962,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>24</v>
@@ -2028,10 +2025,10 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z6" t="s">
         <v>54</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>55</v>
       </c>
       <c r="AA6">
         <v>5</v>
@@ -2064,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="AK6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AL6">
         <v>0.1</v>
@@ -2075,7 +2072,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -2138,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA7">
         <v>8</v>
@@ -2174,7 +2171,7 @@
         <v>1</v>
       </c>
       <c r="AK7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL7">
         <v>0.15</v>
@@ -2185,7 +2182,7 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>48</v>
@@ -2248,10 +2245,10 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z8" t="s">
         <v>61</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>62</v>
       </c>
       <c r="AA8">
         <v>10</v>
@@ -2284,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="AK8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL8">
         <v>0.18</v>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -2358,10 +2355,10 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z9" t="s">
         <v>65</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>66</v>
       </c>
       <c r="AA9">
         <v>12</v>
@@ -2399,7 +2396,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>96</v>
@@ -2462,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" t="s">
         <v>68</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>69</v>
       </c>
       <c r="AA10">
         <v>14</v>
@@ -2498,7 +2495,7 @@
         <v>1</v>
       </c>
       <c r="AK10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL10">
         <v>0.01</v>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>145</v>
@@ -2572,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z11" t="s">
         <v>72</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>73</v>
       </c>
       <c r="AA11">
         <v>18</v>
@@ -2608,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="AK11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL11">
         <v>0.15</v>
@@ -2619,7 +2616,7 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>208</v>
@@ -2682,10 +2679,10 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z12" t="s">
         <v>75</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>76</v>
       </c>
       <c r="AA12">
         <v>20</v>
@@ -2718,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="AK12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL12">
         <v>0.15</v>
@@ -2729,7 +2726,7 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>600</v>
@@ -2792,10 +2789,10 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z13" t="s">
         <v>79</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>80</v>
       </c>
       <c r="AA13">
         <v>25</v>
@@ -2833,7 +2830,7 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14">
         <v>1000</v>
@@ -2896,10 +2893,10 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z14" t="s">
         <v>82</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>83</v>
       </c>
       <c r="AA14">
         <v>30</v>
@@ -2937,7 +2934,7 @@
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>2300</v>
@@ -3000,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z15" t="s">
         <v>85</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>86</v>
       </c>
       <c r="AA15">
         <v>50</v>
@@ -3036,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="AK15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL15">
         <v>0.16</v>
@@ -3047,7 +3044,7 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>5000</v>
@@ -3110,10 +3107,10 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z16" t="s">
         <v>92</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>93</v>
       </c>
       <c r="AA16">
         <v>60</v>
@@ -3151,7 +3148,7 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17">
         <v>8000</v>
@@ -3214,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="Y17" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z17" t="s">
         <v>95</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>96</v>
       </c>
       <c r="AA17">
         <v>100</v>
@@ -3255,7 +3252,7 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18">
         <v>12000</v>
@@ -3318,10 +3315,10 @@
         <v>0</v>
       </c>
       <c r="Y18" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z18" t="s">
         <v>88</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>89</v>
       </c>
       <c r="AA18">
         <v>200</v>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19">
         <v>14000</v>
@@ -3422,10 +3419,10 @@
         <v>0</v>
       </c>
       <c r="Y19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z19" t="s">
         <v>99</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>100</v>
       </c>
       <c r="AA19">
         <v>400</v>
@@ -3463,7 +3460,7 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20">
         <v>18000</v>
@@ -3526,10 +3523,10 @@
         <v>0</v>
       </c>
       <c r="Y20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z20" t="s">
         <v>102</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>103</v>
       </c>
       <c r="AA20">
         <v>500</v>
@@ -3567,7 +3564,7 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21">
         <v>24000</v>
@@ -3630,10 +3627,10 @@
         <v>0</v>
       </c>
       <c r="Y21" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z21" t="s">
         <v>105</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>106</v>
       </c>
       <c r="AA21">
         <v>1000</v>
@@ -3671,7 +3668,7 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22">
         <v>28000</v>
@@ -3734,10 +3731,10 @@
         <v>0</v>
       </c>
       <c r="Y22" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z22" t="s">
         <v>108</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>109</v>
       </c>
       <c r="AA22">
         <v>1500</v>
@@ -3770,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="AK22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AL22">
         <v>0.01</v>
@@ -3781,7 +3778,7 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23">
         <v>32000</v>
@@ -3844,10 +3841,10 @@
         <v>0</v>
       </c>
       <c r="Y23" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z23" t="s">
         <v>112</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>113</v>
       </c>
       <c r="AA23">
         <v>3000</v>
@@ -3885,7 +3882,7 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24">
         <v>38000</v>
@@ -3948,10 +3945,10 @@
         <v>0</v>
       </c>
       <c r="Y24" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z24" t="s">
         <v>115</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>116</v>
       </c>
       <c r="AA24">
         <v>5000</v>
@@ -3989,7 +3986,7 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25">
         <v>40000</v>
@@ -4052,10 +4049,10 @@
         <v>0</v>
       </c>
       <c r="Y25" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z25" t="s">
         <v>118</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>119</v>
       </c>
       <c r="AA25">
         <v>10000</v>
@@ -4093,7 +4090,7 @@
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B26">
         <v>44000</v>
@@ -4156,10 +4153,10 @@
         <v>0</v>
       </c>
       <c r="Y26" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z26" t="s">
         <v>121</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>122</v>
       </c>
       <c r="AA26">
         <v>15000</v>
@@ -4197,7 +4194,7 @@
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27">
         <v>45000</v>
@@ -4260,10 +4257,10 @@
         <v>0</v>
       </c>
       <c r="Y27" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z27" t="s">
         <v>124</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>125</v>
       </c>
       <c r="AA27">
         <v>20000</v>
@@ -4301,7 +4298,7 @@
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28">
         <v>50000</v>
@@ -4364,10 +4361,10 @@
         <v>0</v>
       </c>
       <c r="Y28" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z28" t="s">
         <v>127</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>128</v>
       </c>
       <c r="AA28">
         <v>40000</v>
@@ -4405,7 +4402,7 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29">
         <v>65000</v>
@@ -4468,10 +4465,10 @@
         <v>0</v>
       </c>
       <c r="Y29" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z29" t="s">
         <v>130</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>131</v>
       </c>
       <c r="AA29">
         <v>50000</v>
@@ -4504,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="AK29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL29">
         <v>1E-3</v>
@@ -4515,7 +4512,7 @@
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -4614,12 +4611,12 @@
         <v>1</v>
       </c>
       <c r="AM30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -4718,12 +4715,12 @@
         <v>1</v>
       </c>
       <c r="AM31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B32">
         <v>11</v>
@@ -4822,12 +4819,12 @@
         <v>1</v>
       </c>
       <c r="AM32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33">
         <v>16</v>
@@ -4890,10 +4887,10 @@
         <v>0</v>
       </c>
       <c r="Y33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AA33">
         <v>3</v>
@@ -4926,12 +4923,12 @@
         <v>1</v>
       </c>
       <c r="AM33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B34">
         <v>24</v>
@@ -4994,10 +4991,10 @@
         <v>0</v>
       </c>
       <c r="Y34" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z34" t="s">
         <v>54</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>55</v>
       </c>
       <c r="AA34">
         <v>5</v>
@@ -5030,12 +5027,12 @@
         <v>1</v>
       </c>
       <c r="AM34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35">
         <v>30</v>
@@ -5098,10 +5095,10 @@
         <v>0</v>
       </c>
       <c r="Y35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA35">
         <v>8</v>
@@ -5134,12 +5131,12 @@
         <v>1</v>
       </c>
       <c r="AM35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B36">
         <v>48</v>
@@ -5202,10 +5199,10 @@
         <v>0</v>
       </c>
       <c r="Y36" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z36" t="s">
         <v>61</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>62</v>
       </c>
       <c r="AA36">
         <v>10</v>
@@ -5238,12 +5235,12 @@
         <v>1</v>
       </c>
       <c r="AM36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B37">
         <v>50</v>
@@ -5306,10 +5303,10 @@
         <v>0</v>
       </c>
       <c r="Y37" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z37" t="s">
         <v>65</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>66</v>
       </c>
       <c r="AA37">
         <v>12</v>
@@ -5342,12 +5339,12 @@
         <v>1</v>
       </c>
       <c r="AM37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38">
         <v>96</v>
@@ -5410,10 +5407,10 @@
         <v>0</v>
       </c>
       <c r="Y38" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z38" t="s">
         <v>68</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>69</v>
       </c>
       <c r="AA38">
         <v>14</v>
@@ -5446,12 +5443,12 @@
         <v>1</v>
       </c>
       <c r="AM38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B39">
         <v>145</v>
@@ -5514,10 +5511,10 @@
         <v>0</v>
       </c>
       <c r="Y39" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z39" t="s">
         <v>72</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>73</v>
       </c>
       <c r="AA39">
         <v>18</v>
@@ -5550,12 +5547,12 @@
         <v>1</v>
       </c>
       <c r="AM39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B40">
         <v>208</v>
@@ -5618,10 +5615,10 @@
         <v>0</v>
       </c>
       <c r="Y40" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z40" t="s">
         <v>75</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>76</v>
       </c>
       <c r="AA40">
         <v>20</v>
@@ -5654,12 +5651,12 @@
         <v>1</v>
       </c>
       <c r="AM40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41">
         <v>600</v>
@@ -5722,10 +5719,10 @@
         <v>0</v>
       </c>
       <c r="Y41" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z41" t="s">
         <v>79</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>80</v>
       </c>
       <c r="AA41">
         <v>25</v>
@@ -5758,12 +5755,12 @@
         <v>1</v>
       </c>
       <c r="AM41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42">
         <v>1000</v>
@@ -5826,10 +5823,10 @@
         <v>0</v>
       </c>
       <c r="Y42" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z42" t="s">
         <v>82</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>83</v>
       </c>
       <c r="AA42">
         <v>30</v>
@@ -5862,12 +5859,12 @@
         <v>1</v>
       </c>
       <c r="AM42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B43">
         <v>2300</v>
@@ -5930,10 +5927,10 @@
         <v>0</v>
       </c>
       <c r="Y43" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z43" t="s">
         <v>85</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>86</v>
       </c>
       <c r="AA43">
         <v>50</v>
@@ -5966,12 +5963,12 @@
         <v>1</v>
       </c>
       <c r="AM43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B44">
         <v>2500</v>
@@ -6034,10 +6031,10 @@
         <v>0</v>
       </c>
       <c r="Y44" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z44" t="s">
         <v>149</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>150</v>
       </c>
       <c r="AA44">
         <v>60</v>
@@ -6070,12 +6067,12 @@
         <v>1</v>
       </c>
       <c r="AM44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45">
         <v>5000</v>
@@ -6138,10 +6135,10 @@
         <v>0</v>
       </c>
       <c r="Y45" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z45" t="s">
         <v>92</v>
-      </c>
-      <c r="Z45" t="s">
-        <v>93</v>
       </c>
       <c r="AA45">
         <v>100</v>
@@ -6174,12 +6171,12 @@
         <v>1</v>
       </c>
       <c r="AM45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46">
         <v>8000</v>
@@ -6242,10 +6239,10 @@
         <v>0</v>
       </c>
       <c r="Y46" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z46" t="s">
         <v>95</v>
-      </c>
-      <c r="Z46" t="s">
-        <v>96</v>
       </c>
       <c r="AA46">
         <v>200</v>
@@ -6278,12 +6275,12 @@
         <v>1</v>
       </c>
       <c r="AM46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47">
         <v>12000</v>
@@ -6346,10 +6343,10 @@
         <v>0</v>
       </c>
       <c r="Y47" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z47" t="s">
         <v>88</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>89</v>
       </c>
       <c r="AA47">
         <v>400</v>
@@ -6382,12 +6379,12 @@
         <v>1</v>
       </c>
       <c r="AM47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48">
         <v>14000</v>
@@ -6450,10 +6447,10 @@
         <v>0</v>
       </c>
       <c r="Y48" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z48" t="s">
         <v>99</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>100</v>
       </c>
       <c r="AA48">
         <v>500</v>
@@ -6486,12 +6483,12 @@
         <v>1</v>
       </c>
       <c r="AM48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49">
         <v>18000</v>
@@ -6554,10 +6551,10 @@
         <v>0</v>
       </c>
       <c r="Y49" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z49" t="s">
         <v>102</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>103</v>
       </c>
       <c r="AA49">
         <v>1000</v>
@@ -6590,18 +6587,18 @@
         <v>1</v>
       </c>
       <c r="AK49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AL49">
         <v>0.01</v>
       </c>
       <c r="AM49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50">
         <v>24000</v>
@@ -6664,10 +6661,10 @@
         <v>0</v>
       </c>
       <c r="Y50" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z50" t="s">
         <v>105</v>
-      </c>
-      <c r="Z50" t="s">
-        <v>106</v>
       </c>
       <c r="AA50">
         <v>1500</v>
@@ -6700,12 +6697,12 @@
         <v>1</v>
       </c>
       <c r="AM50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B51">
         <v>28000</v>
@@ -6768,10 +6765,10 @@
         <v>0</v>
       </c>
       <c r="Y51" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z51" t="s">
         <v>108</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>109</v>
       </c>
       <c r="AA51">
         <v>3000</v>
@@ -6804,12 +6801,12 @@
         <v>1</v>
       </c>
       <c r="AM51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52">
         <v>32000</v>
@@ -6872,10 +6869,10 @@
         <v>0</v>
       </c>
       <c r="Y52" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z52" t="s">
         <v>112</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>113</v>
       </c>
       <c r="AA52">
         <v>5000</v>
@@ -6908,18 +6905,18 @@
         <v>1</v>
       </c>
       <c r="AK52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AL52">
         <v>0.15</v>
       </c>
       <c r="AM52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B53">
         <v>38000</v>
@@ -6982,10 +6979,10 @@
         <v>0</v>
       </c>
       <c r="Y53" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z53" t="s">
         <v>115</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>116</v>
       </c>
       <c r="AA53">
         <v>10000</v>
@@ -7018,12 +7015,12 @@
         <v>1</v>
       </c>
       <c r="AM53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B54">
         <v>40000</v>
@@ -7086,10 +7083,10 @@
         <v>0</v>
       </c>
       <c r="Y54" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z54" t="s">
         <v>118</v>
-      </c>
-      <c r="Z54" t="s">
-        <v>119</v>
       </c>
       <c r="AA54">
         <v>15000</v>
@@ -7122,12 +7119,12 @@
         <v>1</v>
       </c>
       <c r="AM54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B55">
         <v>44000</v>
@@ -7190,10 +7187,10 @@
         <v>0</v>
       </c>
       <c r="Y55" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z55" t="s">
         <v>121</v>
-      </c>
-      <c r="Z55" t="s">
-        <v>122</v>
       </c>
       <c r="AA55">
         <v>20000</v>
@@ -7226,18 +7223,18 @@
         <v>1</v>
       </c>
       <c r="AK55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL55">
         <v>0.15</v>
       </c>
       <c r="AM55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B56">
         <v>45000</v>
@@ -7300,10 +7297,10 @@
         <v>0</v>
       </c>
       <c r="Y56" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z56" t="s">
         <v>124</v>
-      </c>
-      <c r="Z56" t="s">
-        <v>125</v>
       </c>
       <c r="AA56">
         <v>40000</v>
@@ -7336,12 +7333,12 @@
         <v>1</v>
       </c>
       <c r="AM56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B57">
         <v>50000</v>
@@ -7404,10 +7401,10 @@
         <v>0</v>
       </c>
       <c r="Y57" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z57" t="s">
         <v>127</v>
-      </c>
-      <c r="Z57" t="s">
-        <v>128</v>
       </c>
       <c r="AA57">
         <v>50000</v>
@@ -7440,12 +7437,12 @@
         <v>1</v>
       </c>
       <c r="AM57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B58">
         <v>65000</v>
@@ -7508,10 +7505,10 @@
         <v>0</v>
       </c>
       <c r="Y58" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z58" t="s">
         <v>130</v>
-      </c>
-      <c r="Z58" t="s">
-        <v>131</v>
       </c>
       <c r="AA58">
         <v>60000</v>
@@ -7544,12 +7541,12 @@
         <v>1</v>
       </c>
       <c r="AM58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B59">
         <v>68000</v>
@@ -7612,10 +7609,10 @@
         <v>0</v>
       </c>
       <c r="Y59" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z59" t="s">
         <v>167</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>168</v>
       </c>
       <c r="AA59">
         <v>75000</v>
@@ -7648,12 +7645,12 @@
         <v>1</v>
       </c>
       <c r="AM59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60">
         <v>70000</v>
@@ -7716,10 +7713,10 @@
         <v>0</v>
       </c>
       <c r="Y60" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z60" t="s">
         <v>170</v>
-      </c>
-      <c r="Z60" t="s">
-        <v>171</v>
       </c>
       <c r="AA60">
         <v>100000</v>
@@ -7752,12 +7749,12 @@
         <v>1</v>
       </c>
       <c r="AM60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B61">
         <v>80000</v>
@@ -7820,10 +7817,10 @@
         <v>0</v>
       </c>
       <c r="Y61" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z61" t="s">
         <v>173</v>
-      </c>
-      <c r="Z61" t="s">
-        <v>174</v>
       </c>
       <c r="AA61">
         <v>120000</v>
@@ -7856,12 +7853,12 @@
         <v>1</v>
       </c>
       <c r="AM61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62">
         <v>90000</v>
@@ -7924,10 +7921,10 @@
         <v>0</v>
       </c>
       <c r="Y62" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z62" t="s">
         <v>176</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>177</v>
       </c>
       <c r="AA62">
         <v>130000</v>
@@ -7960,12 +7957,12 @@
         <v>1</v>
       </c>
       <c r="AM62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63">
         <v>100000</v>
@@ -8028,10 +8025,10 @@
         <v>0</v>
       </c>
       <c r="Y63" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z63" t="s">
         <v>179</v>
-      </c>
-      <c r="Z63" t="s">
-        <v>180</v>
       </c>
       <c r="AA63">
         <v>150000</v>
@@ -8064,18 +8061,18 @@
         <v>1</v>
       </c>
       <c r="AK63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AL63">
         <v>0.01</v>
       </c>
       <c r="AM63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64">
         <v>200000</v>
@@ -8147,10 +8144,10 @@
         <v>8</v>
       </c>
       <c r="Y64" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z64" t="s">
         <v>183</v>
-      </c>
-      <c r="Z64" t="s">
-        <v>184</v>
       </c>
       <c r="AA64">
         <v>400000</v>
@@ -8183,7 +8180,7 @@
         <v>1</v>
       </c>
       <c r="AK64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AL64">
         <v>0.25</v>
@@ -8194,7 +8191,7 @@
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65">
         <v>300000</v>
@@ -8266,10 +8263,10 @@
         <v>10</v>
       </c>
       <c r="Y65" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z65" t="s">
         <v>186</v>
-      </c>
-      <c r="Z65" t="s">
-        <v>187</v>
       </c>
       <c r="AA65">
         <v>450000</v>
@@ -8302,7 +8299,7 @@
         <v>1</v>
       </c>
       <c r="AK65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AL65">
         <v>0.01</v>
@@ -8313,7 +8310,7 @@
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66">
         <v>500000</v>
@@ -8385,10 +8382,10 @@
         <v>16</v>
       </c>
       <c r="Y66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Z66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA66">
         <v>500000</v>
@@ -8421,7 +8418,7 @@
         <v>1</v>
       </c>
       <c r="AK66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AL66">
         <v>0.01</v>
@@ -8432,7 +8429,7 @@
     </row>
     <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B67">
         <v>600000</v>
@@ -8504,10 +8501,10 @@
         <v>24</v>
       </c>
       <c r="Y67" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z67" t="s">
         <v>191</v>
-      </c>
-      <c r="Z67" t="s">
-        <v>192</v>
       </c>
       <c r="AA67">
         <v>600000</v>
@@ -8545,7 +8542,7 @@
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B68">
         <v>750000</v>
@@ -8617,10 +8614,10 @@
         <v>36</v>
       </c>
       <c r="Y68" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z68" t="s">
         <v>194</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>195</v>
       </c>
       <c r="AA68">
         <v>1000000</v>
@@ -8653,12 +8650,12 @@
         <v>1</v>
       </c>
       <c r="AM68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B69">
         <v>800000</v>
@@ -8730,10 +8727,10 @@
         <v>16</v>
       </c>
       <c r="Y69" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z69" t="s">
         <v>197</v>
-      </c>
-      <c r="Z69" t="s">
-        <v>198</v>
       </c>
       <c r="AA69">
         <v>2000000</v>
@@ -8766,12 +8763,12 @@
         <v>1</v>
       </c>
       <c r="AM69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B70">
         <v>950000</v>
@@ -8843,10 +8840,10 @@
         <v>24</v>
       </c>
       <c r="Y70" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z70" t="s">
         <v>200</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>201</v>
       </c>
       <c r="AA70">
         <v>3000000</v>
@@ -8879,18 +8876,18 @@
         <v>1</v>
       </c>
       <c r="AK70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AL70">
         <v>0.2</v>
       </c>
       <c r="AM70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71">
         <v>1000000</v>
@@ -8962,10 +8959,10 @@
         <v>28</v>
       </c>
       <c r="Y71" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z71" t="s">
         <v>204</v>
-      </c>
-      <c r="Z71" t="s">
-        <v>205</v>
       </c>
       <c r="AA71">
         <v>4000000</v>
@@ -8998,12 +8995,12 @@
         <v>1</v>
       </c>
       <c r="AM71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B72">
         <v>2000000</v>
@@ -9075,10 +9072,10 @@
         <v>32</v>
       </c>
       <c r="Y72" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z72" t="s">
         <v>207</v>
-      </c>
-      <c r="Z72" t="s">
-        <v>208</v>
       </c>
       <c r="AA72">
         <v>5000000</v>
@@ -9111,12 +9108,12 @@
         <v>1</v>
       </c>
       <c r="AM72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -9215,12 +9212,12 @@
         <v>1</v>
       </c>
       <c r="AM73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74">
         <v>9</v>
@@ -9319,12 +9316,12 @@
         <v>1</v>
       </c>
       <c r="AM74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B75">
         <v>11</v>
@@ -9423,12 +9420,12 @@
         <v>1</v>
       </c>
       <c r="AM75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B76">
         <v>16</v>
@@ -9491,10 +9488,10 @@
         <v>0</v>
       </c>
       <c r="Y76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AA76">
         <v>3</v>
@@ -9527,12 +9524,12 @@
         <v>1</v>
       </c>
       <c r="AM76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B77">
         <v>24</v>
@@ -9595,10 +9592,10 @@
         <v>0</v>
       </c>
       <c r="Y77" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z77" t="s">
         <v>54</v>
-      </c>
-      <c r="Z77" t="s">
-        <v>55</v>
       </c>
       <c r="AA77">
         <v>5</v>
@@ -9631,12 +9628,12 @@
         <v>1</v>
       </c>
       <c r="AM77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B78">
         <v>30</v>
@@ -9699,10 +9696,10 @@
         <v>0</v>
       </c>
       <c r="Y78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA78">
         <v>8</v>
@@ -9735,12 +9732,12 @@
         <v>1</v>
       </c>
       <c r="AM78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B79">
         <v>48</v>
@@ -9803,10 +9800,10 @@
         <v>0</v>
       </c>
       <c r="Y79" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z79" t="s">
         <v>61</v>
-      </c>
-      <c r="Z79" t="s">
-        <v>62</v>
       </c>
       <c r="AA79">
         <v>10</v>
@@ -9839,12 +9836,12 @@
         <v>1</v>
       </c>
       <c r="AM79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B80">
         <v>50</v>
@@ -9907,10 +9904,10 @@
         <v>0</v>
       </c>
       <c r="Y80" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z80" t="s">
         <v>65</v>
-      </c>
-      <c r="Z80" t="s">
-        <v>66</v>
       </c>
       <c r="AA80">
         <v>12</v>
@@ -9943,12 +9940,12 @@
         <v>1</v>
       </c>
       <c r="AM80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B81">
         <v>96</v>
@@ -10011,10 +10008,10 @@
         <v>0</v>
       </c>
       <c r="Y81" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z81" t="s">
         <v>68</v>
-      </c>
-      <c r="Z81" t="s">
-        <v>69</v>
       </c>
       <c r="AA81">
         <v>14</v>
@@ -10047,12 +10044,12 @@
         <v>1</v>
       </c>
       <c r="AM81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B82">
         <v>145</v>
@@ -10115,10 +10112,10 @@
         <v>0</v>
       </c>
       <c r="Y82" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z82" t="s">
         <v>72</v>
-      </c>
-      <c r="Z82" t="s">
-        <v>73</v>
       </c>
       <c r="AA82">
         <v>18</v>
@@ -10151,12 +10148,12 @@
         <v>1</v>
       </c>
       <c r="AM82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B83">
         <v>208</v>
@@ -10219,10 +10216,10 @@
         <v>0</v>
       </c>
       <c r="Y83" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z83" t="s">
         <v>75</v>
-      </c>
-      <c r="Z83" t="s">
-        <v>76</v>
       </c>
       <c r="AA83">
         <v>20</v>
@@ -10255,18 +10252,18 @@
         <v>1</v>
       </c>
       <c r="AK83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AL83">
         <v>0.01</v>
       </c>
       <c r="AM83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B84">
         <v>600</v>
@@ -10329,10 +10326,10 @@
         <v>0</v>
       </c>
       <c r="Y84" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z84" t="s">
         <v>79</v>
-      </c>
-      <c r="Z84" t="s">
-        <v>80</v>
       </c>
       <c r="AA84">
         <v>25</v>
@@ -10365,12 +10362,12 @@
         <v>1</v>
       </c>
       <c r="AM84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B85">
         <v>1000</v>
@@ -10433,10 +10430,10 @@
         <v>0</v>
       </c>
       <c r="Y85" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z85" t="s">
         <v>82</v>
-      </c>
-      <c r="Z85" t="s">
-        <v>83</v>
       </c>
       <c r="AA85">
         <v>30</v>
@@ -10469,12 +10466,12 @@
         <v>1</v>
       </c>
       <c r="AM85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B86">
         <v>2300</v>
@@ -10537,10 +10534,10 @@
         <v>0</v>
       </c>
       <c r="Y86" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z86" t="s">
         <v>85</v>
-      </c>
-      <c r="Z86" t="s">
-        <v>86</v>
       </c>
       <c r="AA86">
         <v>50</v>
@@ -10573,12 +10570,12 @@
         <v>1</v>
       </c>
       <c r="AM86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B87">
         <v>2500</v>
@@ -10641,10 +10638,10 @@
         <v>0</v>
       </c>
       <c r="Y87" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z87" t="s">
         <v>149</v>
-      </c>
-      <c r="Z87" t="s">
-        <v>150</v>
       </c>
       <c r="AA87">
         <v>60</v>
@@ -10677,12 +10674,12 @@
         <v>1</v>
       </c>
       <c r="AM87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B88">
         <v>5000</v>
@@ -10745,10 +10742,10 @@
         <v>0</v>
       </c>
       <c r="Y88" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z88" t="s">
         <v>92</v>
-      </c>
-      <c r="Z88" t="s">
-        <v>93</v>
       </c>
       <c r="AA88">
         <v>100</v>
@@ -10781,12 +10778,12 @@
         <v>1</v>
       </c>
       <c r="AM88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B89">
         <v>8000</v>
@@ -10849,10 +10846,10 @@
         <v>0</v>
       </c>
       <c r="Y89" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z89" t="s">
         <v>95</v>
-      </c>
-      <c r="Z89" t="s">
-        <v>96</v>
       </c>
       <c r="AA89">
         <v>200</v>
@@ -10885,12 +10882,12 @@
         <v>1</v>
       </c>
       <c r="AM89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B90">
         <v>14000</v>
@@ -10953,10 +10950,10 @@
         <v>0</v>
       </c>
       <c r="Y90" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z90" t="s">
         <v>99</v>
-      </c>
-      <c r="Z90" t="s">
-        <v>100</v>
       </c>
       <c r="AA90">
         <v>500</v>
@@ -10989,12 +10986,12 @@
         <v>1</v>
       </c>
       <c r="AM90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91">
         <v>12000</v>
@@ -11057,10 +11054,10 @@
         <v>0</v>
       </c>
       <c r="Y91" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z91" t="s">
         <v>88</v>
-      </c>
-      <c r="Z91" t="s">
-        <v>89</v>
       </c>
       <c r="AA91">
         <v>400</v>
@@ -11093,18 +11090,18 @@
         <v>1</v>
       </c>
       <c r="AK91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AL91">
         <v>0.2</v>
       </c>
       <c r="AM91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B92">
         <v>18000</v>
@@ -11167,10 +11164,10 @@
         <v>0</v>
       </c>
       <c r="Y92" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z92" t="s">
         <v>102</v>
-      </c>
-      <c r="Z92" t="s">
-        <v>103</v>
       </c>
       <c r="AA92">
         <v>1000</v>
@@ -11203,12 +11200,12 @@
         <v>1</v>
       </c>
       <c r="AM92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B93">
         <v>24000</v>
@@ -11271,10 +11268,10 @@
         <v>0</v>
       </c>
       <c r="Y93" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z93" t="s">
         <v>105</v>
-      </c>
-      <c r="Z93" t="s">
-        <v>106</v>
       </c>
       <c r="AA93">
         <v>1500</v>
@@ -11307,12 +11304,12 @@
         <v>1</v>
       </c>
       <c r="AM93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B94">
         <v>28000</v>
@@ -11375,10 +11372,10 @@
         <v>0</v>
       </c>
       <c r="Y94" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z94" t="s">
         <v>108</v>
-      </c>
-      <c r="Z94" t="s">
-        <v>109</v>
       </c>
       <c r="AA94">
         <v>3000</v>
@@ -11411,12 +11408,12 @@
         <v>1</v>
       </c>
       <c r="AM94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B95">
         <v>32000</v>
@@ -11479,10 +11476,10 @@
         <v>0</v>
       </c>
       <c r="Y95" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z95" t="s">
         <v>112</v>
-      </c>
-      <c r="Z95" t="s">
-        <v>113</v>
       </c>
       <c r="AA95">
         <v>5000</v>
@@ -11515,12 +11512,12 @@
         <v>1</v>
       </c>
       <c r="AM95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B96">
         <v>38000</v>
@@ -11583,10 +11580,10 @@
         <v>0</v>
       </c>
       <c r="Y96" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z96" t="s">
         <v>115</v>
-      </c>
-      <c r="Z96" t="s">
-        <v>116</v>
       </c>
       <c r="AA96">
         <v>10000</v>
@@ -11619,12 +11616,12 @@
         <v>1</v>
       </c>
       <c r="AM96" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B97">
         <v>40000</v>
@@ -11687,10 +11684,10 @@
         <v>0</v>
       </c>
       <c r="Y97" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z97" t="s">
         <v>118</v>
-      </c>
-      <c r="Z97" t="s">
-        <v>119</v>
       </c>
       <c r="AA97">
         <v>15000</v>
@@ -11723,12 +11720,12 @@
         <v>1</v>
       </c>
       <c r="AM97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B98">
         <v>44000</v>
@@ -11791,10 +11788,10 @@
         <v>0</v>
       </c>
       <c r="Y98" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z98" t="s">
         <v>121</v>
-      </c>
-      <c r="Z98" t="s">
-        <v>122</v>
       </c>
       <c r="AA98">
         <v>20000</v>
@@ -11827,12 +11824,12 @@
         <v>1</v>
       </c>
       <c r="AM98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="99" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B99">
         <v>45000</v>
@@ -11895,10 +11892,10 @@
         <v>0</v>
       </c>
       <c r="Y99" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z99" t="s">
         <v>124</v>
-      </c>
-      <c r="Z99" t="s">
-        <v>125</v>
       </c>
       <c r="AA99">
         <v>40000</v>
@@ -11931,12 +11928,12 @@
         <v>1</v>
       </c>
       <c r="AM99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B100">
         <v>50000</v>
@@ -11999,10 +11996,10 @@
         <v>0</v>
       </c>
       <c r="Y100" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z100" t="s">
         <v>127</v>
-      </c>
-      <c r="Z100" t="s">
-        <v>128</v>
       </c>
       <c r="AA100">
         <v>50000</v>
@@ -12035,12 +12032,12 @@
         <v>1</v>
       </c>
       <c r="AM100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B101">
         <v>65000</v>
@@ -12103,10 +12100,10 @@
         <v>0</v>
       </c>
       <c r="Y101" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z101" t="s">
         <v>130</v>
-      </c>
-      <c r="Z101" t="s">
-        <v>131</v>
       </c>
       <c r="AA101">
         <v>60000</v>
@@ -12139,12 +12136,12 @@
         <v>1</v>
       </c>
       <c r="AM101" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B102">
         <v>68000</v>
@@ -12207,10 +12204,10 @@
         <v>0</v>
       </c>
       <c r="Y102" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z102" t="s">
         <v>167</v>
-      </c>
-      <c r="Z102" t="s">
-        <v>168</v>
       </c>
       <c r="AA102">
         <v>75000</v>
@@ -12243,12 +12240,12 @@
         <v>1</v>
       </c>
       <c r="AM102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B103">
         <v>70000</v>
@@ -12311,10 +12308,10 @@
         <v>0</v>
       </c>
       <c r="Y103" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z103" t="s">
         <v>170</v>
-      </c>
-      <c r="Z103" t="s">
-        <v>171</v>
       </c>
       <c r="AA103">
         <v>100000</v>
@@ -12347,12 +12344,12 @@
         <v>1</v>
       </c>
       <c r="AM103" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B104">
         <v>80000</v>
@@ -12415,10 +12412,10 @@
         <v>0</v>
       </c>
       <c r="Y104" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z104" t="s">
         <v>173</v>
-      </c>
-      <c r="Z104" t="s">
-        <v>174</v>
       </c>
       <c r="AA104">
         <v>120000</v>
@@ -12451,12 +12448,12 @@
         <v>1</v>
       </c>
       <c r="AM104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="105" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B105">
         <v>90000</v>
@@ -12519,10 +12516,10 @@
         <v>0</v>
       </c>
       <c r="Y105" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z105" t="s">
         <v>176</v>
-      </c>
-      <c r="Z105" t="s">
-        <v>177</v>
       </c>
       <c r="AA105">
         <v>130000</v>
@@ -12555,12 +12552,12 @@
         <v>1</v>
       </c>
       <c r="AM105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B106">
         <v>100000</v>
@@ -12623,10 +12620,10 @@
         <v>0</v>
       </c>
       <c r="Y106" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z106" t="s">
         <v>179</v>
-      </c>
-      <c r="Z106" t="s">
-        <v>180</v>
       </c>
       <c r="AA106">
         <v>150000</v>
@@ -12659,12 +12656,12 @@
         <v>1</v>
       </c>
       <c r="AM106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="107" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B107">
         <v>3000000</v>
@@ -12736,10 +12733,10 @@
         <v>40</v>
       </c>
       <c r="Y107" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z107" t="s">
         <v>243</v>
-      </c>
-      <c r="Z107" t="s">
-        <v>244</v>
       </c>
       <c r="AA107">
         <v>1000000</v>
@@ -12772,12 +12769,12 @@
         <v>1</v>
       </c>
       <c r="AM107" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B108">
         <v>4000000</v>
@@ -12849,10 +12846,10 @@
         <v>45</v>
       </c>
       <c r="Y108" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z108" t="s">
         <v>246</v>
-      </c>
-      <c r="Z108" t="s">
-        <v>247</v>
       </c>
       <c r="AA108">
         <v>2000000</v>
@@ -12885,12 +12882,12 @@
         <v>1</v>
       </c>
       <c r="AM108" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B109">
         <v>5000000</v>
@@ -12962,10 +12959,10 @@
         <v>50</v>
       </c>
       <c r="Y109" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z109" t="s">
         <v>249</v>
-      </c>
-      <c r="Z109" t="s">
-        <v>250</v>
       </c>
       <c r="AA109">
         <v>3000000</v>
@@ -12998,12 +12995,12 @@
         <v>1</v>
       </c>
       <c r="AM109" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B110">
         <v>10000000</v>
@@ -13075,10 +13072,10 @@
         <v>75</v>
       </c>
       <c r="Y110" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z110" t="s">
         <v>252</v>
-      </c>
-      <c r="Z110" t="s">
-        <v>253</v>
       </c>
       <c r="AA110">
         <v>4000000</v>
@@ -13111,12 +13108,12 @@
         <v>1</v>
       </c>
       <c r="AM110" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="111" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B111">
         <v>20000000</v>
@@ -13188,10 +13185,10 @@
         <v>100</v>
       </c>
       <c r="Y111" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z111" t="s">
         <v>255</v>
-      </c>
-      <c r="Z111" t="s">
-        <v>256</v>
       </c>
       <c r="AA111">
         <v>5000000</v>
@@ -13224,12 +13221,12 @@
         <v>1</v>
       </c>
       <c r="AM111" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="112" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B112">
         <v>80000</v>
@@ -13292,10 +13289,10 @@
         <v>0</v>
       </c>
       <c r="Y112" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z112" t="s">
         <v>258</v>
-      </c>
-      <c r="Z112" t="s">
-        <v>259</v>
       </c>
       <c r="AA112">
         <v>10000</v>
@@ -13333,7 +13330,7 @@
     </row>
     <row r="113" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B113">
         <v>120000</v>
@@ -13396,10 +13393,10 @@
         <v>0</v>
       </c>
       <c r="Y113" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z113" t="s">
         <v>261</v>
-      </c>
-      <c r="Z113" t="s">
-        <v>262</v>
       </c>
       <c r="AA113">
         <v>15000</v>
@@ -13437,7 +13434,7 @@
     </row>
     <row r="114" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B114">
         <v>130000</v>
@@ -13500,10 +13497,10 @@
         <v>0</v>
       </c>
       <c r="Y114" t="s">
+        <v>263</v>
+      </c>
+      <c r="Z114" t="s">
         <v>264</v>
-      </c>
-      <c r="Z114" t="s">
-        <v>265</v>
       </c>
       <c r="AA114">
         <v>30000</v>
@@ -13541,7 +13538,7 @@
     </row>
     <row r="115" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B115">
         <v>150000</v>
@@ -13604,10 +13601,10 @@
         <v>0</v>
       </c>
       <c r="Y115" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z115" t="s">
         <v>267</v>
-      </c>
-      <c r="Z115" t="s">
-        <v>268</v>
       </c>
       <c r="AA115">
         <v>50000</v>
@@ -13645,7 +13642,7 @@
     </row>
     <row r="116" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B116">
         <v>180000</v>
@@ -13708,10 +13705,10 @@
         <v>0</v>
       </c>
       <c r="Y116" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z116" t="s">
         <v>270</v>
-      </c>
-      <c r="Z116" t="s">
-        <v>271</v>
       </c>
       <c r="AA116">
         <v>60000</v>
@@ -13749,7 +13746,7 @@
     </row>
     <row r="117" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B117">
         <v>220000</v>
@@ -13812,10 +13809,10 @@
         <v>0</v>
       </c>
       <c r="Y117" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z117" t="s">
         <v>273</v>
-      </c>
-      <c r="Z117" t="s">
-        <v>274</v>
       </c>
       <c r="AA117">
         <v>75000</v>
@@ -13853,7 +13850,7 @@
     </row>
     <row r="118" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B118">
         <v>250000</v>
@@ -13916,10 +13913,10 @@
         <v>0</v>
       </c>
       <c r="Y118" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z118" t="s">
         <v>276</v>
-      </c>
-      <c r="Z118" t="s">
-        <v>277</v>
       </c>
       <c r="AA118">
         <v>100000</v>
@@ -13957,7 +13954,7 @@
     </row>
     <row r="119" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B119">
         <v>280000</v>
@@ -14020,10 +14017,10 @@
         <v>0</v>
       </c>
       <c r="Y119" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z119" t="s">
         <v>279</v>
-      </c>
-      <c r="Z119" t="s">
-        <v>280</v>
       </c>
       <c r="AA119">
         <v>110000</v>
@@ -14061,7 +14058,7 @@
     </row>
     <row r="120" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B120">
         <v>290000</v>
@@ -14124,10 +14121,10 @@
         <v>0</v>
       </c>
       <c r="Y120" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z120" t="s">
         <v>282</v>
-      </c>
-      <c r="Z120" t="s">
-        <v>283</v>
       </c>
       <c r="AA120">
         <v>130000</v>
@@ -14165,7 +14162,7 @@
     </row>
     <row r="121" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B121">
         <v>340000</v>
@@ -14228,10 +14225,10 @@
         <v>0</v>
       </c>
       <c r="Y121" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z121" t="s">
         <v>285</v>
-      </c>
-      <c r="Z121" t="s">
-        <v>286</v>
       </c>
       <c r="AA121">
         <v>150000</v>
@@ -14269,7 +14266,7 @@
     </row>
     <row r="122" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B122">
         <v>350000</v>
@@ -14332,10 +14329,10 @@
         <v>0</v>
       </c>
       <c r="Y122" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z122" t="s">
         <v>288</v>
-      </c>
-      <c r="Z122" t="s">
-        <v>289</v>
       </c>
       <c r="AA122">
         <v>180000</v>
@@ -14373,7 +14370,7 @@
     </row>
     <row r="123" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B123">
         <v>400000</v>
@@ -14436,10 +14433,10 @@
         <v>0</v>
       </c>
       <c r="Y123" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z123" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AA123">
         <v>250000</v>
@@ -14477,7 +14474,7 @@
     </row>
     <row r="124" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B124">
         <v>420000</v>
@@ -14540,10 +14537,10 @@
         <v>0</v>
       </c>
       <c r="Y124" t="s">
+        <v>292</v>
+      </c>
+      <c r="Z124" t="s">
         <v>293</v>
-      </c>
-      <c r="Z124" t="s">
-        <v>294</v>
       </c>
       <c r="AA124">
         <v>275000</v>
@@ -14581,7 +14578,7 @@
     </row>
     <row r="125" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B125">
         <v>450000</v>
@@ -14644,10 +14641,10 @@
         <v>0</v>
       </c>
       <c r="Y125" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z125" t="s">
         <v>296</v>
-      </c>
-      <c r="Z125" t="s">
-        <v>297</v>
       </c>
       <c r="AA125">
         <v>300000</v>
@@ -14685,7 +14682,7 @@
     </row>
     <row r="126" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B126">
         <v>475000</v>
@@ -14748,10 +14745,10 @@
         <v>0</v>
       </c>
       <c r="Y126" t="s">
+        <v>298</v>
+      </c>
+      <c r="Z126" t="s">
         <v>299</v>
-      </c>
-      <c r="Z126" t="s">
-        <v>300</v>
       </c>
       <c r="AA126">
         <v>345000</v>
@@ -14789,7 +14786,7 @@
     </row>
     <row r="127" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B127">
         <v>490000</v>
@@ -14852,10 +14849,10 @@
         <v>0</v>
       </c>
       <c r="Y127" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z127" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AA127">
         <v>368000</v>
@@ -14893,7 +14890,7 @@
     </row>
     <row r="128" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B128">
         <v>250000</v>
@@ -14956,10 +14953,10 @@
         <v>0</v>
       </c>
       <c r="Y128" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z128" t="s">
         <v>258</v>
-      </c>
-      <c r="Z128" t="s">
-        <v>259</v>
       </c>
       <c r="AA128">
         <v>10000</v>
@@ -14992,12 +14989,12 @@
         <v>1</v>
       </c>
       <c r="AM128" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="129" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B129">
         <v>300000</v>
@@ -15060,10 +15057,10 @@
         <v>0</v>
       </c>
       <c r="Y129" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z129" t="s">
         <v>261</v>
-      </c>
-      <c r="Z129" t="s">
-        <v>262</v>
       </c>
       <c r="AA129">
         <v>15000</v>
@@ -15096,12 +15093,12 @@
         <v>1</v>
       </c>
       <c r="AM129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B130">
         <v>325000</v>
@@ -15164,10 +15161,10 @@
         <v>0</v>
       </c>
       <c r="Y130" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z130" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AA130">
         <v>30000</v>
@@ -15200,12 +15197,12 @@
         <v>1</v>
       </c>
       <c r="AM130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B131">
         <v>450000</v>
@@ -15268,10 +15265,10 @@
         <v>0</v>
       </c>
       <c r="Y131" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z131" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AA131">
         <v>50000</v>
@@ -15304,12 +15301,12 @@
         <v>1</v>
       </c>
       <c r="AM131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="132" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B132">
         <v>475000</v>
@@ -15372,10 +15369,10 @@
         <v>0</v>
       </c>
       <c r="Y132" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z132" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA132">
         <v>60000</v>
@@ -15408,12 +15405,12 @@
         <v>1</v>
       </c>
       <c r="AM132" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B133">
         <v>500000</v>
@@ -15476,10 +15473,10 @@
         <v>0</v>
       </c>
       <c r="Y133" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z133" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AA133">
         <v>75000</v>
@@ -15512,12 +15509,12 @@
         <v>1</v>
       </c>
       <c r="AM133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B134">
         <v>560000</v>
@@ -15580,10 +15577,10 @@
         <v>0</v>
       </c>
       <c r="Y134" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z134" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA134">
         <v>100000</v>
@@ -15616,12 +15613,12 @@
         <v>1</v>
       </c>
       <c r="AM134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B135">
         <v>600000</v>
@@ -15684,10 +15681,10 @@
         <v>0</v>
       </c>
       <c r="Y135" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z135" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AA135">
         <v>110000</v>
@@ -15720,12 +15717,12 @@
         <v>1</v>
       </c>
       <c r="AM135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B136">
         <v>670000</v>
@@ -15788,10 +15785,10 @@
         <v>0</v>
       </c>
       <c r="Y136" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AA136">
         <v>130000</v>
@@ -15824,12 +15821,12 @@
         <v>1</v>
       </c>
       <c r="AM136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B137">
         <v>720000</v>
@@ -15892,10 +15889,10 @@
         <v>0</v>
       </c>
       <c r="Y137" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Z137" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA137">
         <v>150000</v>
@@ -15928,12 +15925,12 @@
         <v>1</v>
       </c>
       <c r="AM137" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B138">
         <v>750000</v>
@@ -15996,10 +15993,10 @@
         <v>0</v>
       </c>
       <c r="Y138" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z138" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AA138">
         <v>180000</v>
@@ -16032,12 +16029,12 @@
         <v>1</v>
       </c>
       <c r="AM138" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B139">
         <v>775000</v>
@@ -16100,10 +16097,10 @@
         <v>0</v>
       </c>
       <c r="Y139" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z139" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AA139">
         <v>250000</v>
@@ -16136,12 +16133,12 @@
         <v>1</v>
       </c>
       <c r="AM139" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B140">
         <v>800000</v>
@@ -16204,10 +16201,10 @@
         <v>0</v>
       </c>
       <c r="Y140" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Z140" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AA140">
         <v>275000</v>
@@ -16240,12 +16237,12 @@
         <v>1</v>
       </c>
       <c r="AM140" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B141">
         <v>825000</v>
@@ -16308,10 +16305,10 @@
         <v>0</v>
       </c>
       <c r="Y141" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Z141" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA141">
         <v>300000</v>
@@ -16344,12 +16341,12 @@
         <v>1</v>
       </c>
       <c r="AM141" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="142" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B142">
         <v>850000</v>
@@ -16412,10 +16409,10 @@
         <v>0</v>
       </c>
       <c r="Y142" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA142">
         <v>345000</v>
@@ -16448,12 +16445,12 @@
         <v>1</v>
       </c>
       <c r="AM142" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="143" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B143">
         <v>875000</v>
@@ -16516,10 +16513,10 @@
         <v>0</v>
       </c>
       <c r="Y143" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z143" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA143">
         <v>368000</v>
@@ -16552,12 +16549,12 @@
         <v>1</v>
       </c>
       <c r="AM143" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="144" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B144">
         <v>250000</v>
@@ -16620,10 +16617,10 @@
         <v>0</v>
       </c>
       <c r="Y144" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z144" t="s">
         <v>258</v>
-      </c>
-      <c r="Z144" t="s">
-        <v>259</v>
       </c>
       <c r="AA144">
         <v>10000</v>
@@ -16656,12 +16653,12 @@
         <v>1</v>
       </c>
       <c r="AM144" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="145" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B145">
         <v>300000</v>
@@ -16724,10 +16721,10 @@
         <v>0</v>
       </c>
       <c r="Y145" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z145" t="s">
         <v>261</v>
-      </c>
-      <c r="Z145" t="s">
-        <v>262</v>
       </c>
       <c r="AA145">
         <v>15000</v>
@@ -16760,12 +16757,12 @@
         <v>1</v>
       </c>
       <c r="AM145" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="146" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B146">
         <v>325000</v>
@@ -16828,10 +16825,10 @@
         <v>0</v>
       </c>
       <c r="Y146" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z146" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AA146">
         <v>30000</v>
@@ -16864,12 +16861,12 @@
         <v>1</v>
       </c>
       <c r="AM146" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="147" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B147">
         <v>450000</v>
@@ -16932,10 +16929,10 @@
         <v>0</v>
       </c>
       <c r="Y147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z147" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AA147">
         <v>50000</v>
@@ -16968,12 +16965,12 @@
         <v>1</v>
       </c>
       <c r="AM147" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="148" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B148">
         <v>475000</v>
@@ -17036,10 +17033,10 @@
         <v>0</v>
       </c>
       <c r="Y148" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA148">
         <v>60000</v>
@@ -17072,12 +17069,12 @@
         <v>1</v>
       </c>
       <c r="AM148" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="149" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B149">
         <v>500000</v>
@@ -17140,10 +17137,10 @@
         <v>0</v>
       </c>
       <c r="Y149" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z149" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AA149">
         <v>75000</v>
@@ -17176,12 +17173,12 @@
         <v>1</v>
       </c>
       <c r="AM149" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="150" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B150">
         <v>560000</v>
@@ -17244,10 +17241,10 @@
         <v>0</v>
       </c>
       <c r="Y150" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z150" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA150">
         <v>100000</v>
@@ -17280,12 +17277,12 @@
         <v>1</v>
       </c>
       <c r="AM150" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="151" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B151">
         <v>600000</v>
@@ -17348,10 +17345,10 @@
         <v>0</v>
       </c>
       <c r="Y151" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z151" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AA151">
         <v>110000</v>
@@ -17384,12 +17381,12 @@
         <v>1</v>
       </c>
       <c r="AM151" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B152">
         <v>670000</v>
@@ -17452,10 +17449,10 @@
         <v>0</v>
       </c>
       <c r="Y152" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z152" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AA152">
         <v>130000</v>
@@ -17488,12 +17485,12 @@
         <v>1</v>
       </c>
       <c r="AM152" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="153" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B153">
         <v>720000</v>
@@ -17556,10 +17553,10 @@
         <v>0</v>
       </c>
       <c r="Y153" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Z153" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA153">
         <v>150000</v>
@@ -17592,12 +17589,12 @@
         <v>1</v>
       </c>
       <c r="AM153" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="154" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B154">
         <v>750000</v>
@@ -17660,10 +17657,10 @@
         <v>0</v>
       </c>
       <c r="Y154" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z154" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AA154">
         <v>180000</v>
@@ -17696,12 +17693,12 @@
         <v>1</v>
       </c>
       <c r="AM154" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="155" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B155">
         <v>775000</v>
@@ -17764,10 +17761,10 @@
         <v>0</v>
       </c>
       <c r="Y155" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Z155" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AA155">
         <v>250000</v>
@@ -17800,12 +17797,12 @@
         <v>1</v>
       </c>
       <c r="AM155" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B156">
         <v>800000</v>
@@ -17868,10 +17865,10 @@
         <v>0</v>
       </c>
       <c r="Y156" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Z156" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AA156">
         <v>275000</v>
@@ -17904,12 +17901,12 @@
         <v>1</v>
       </c>
       <c r="AM156" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="157" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B157">
         <v>825000</v>
@@ -17972,10 +17969,10 @@
         <v>0</v>
       </c>
       <c r="Y157" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Z157" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AA157">
         <v>300000</v>
@@ -18008,12 +18005,12 @@
         <v>1</v>
       </c>
       <c r="AM157" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="158" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B158">
         <v>850000</v>
@@ -18076,10 +18073,10 @@
         <v>0</v>
       </c>
       <c r="Y158" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z158" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AA158">
         <v>345000</v>
@@ -18112,12 +18109,12 @@
         <v>1</v>
       </c>
       <c r="AM158" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="159" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B159">
         <v>875000</v>
@@ -18180,10 +18177,10 @@
         <v>0</v>
       </c>
       <c r="Y159" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z159" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AA159">
         <v>368000</v>
@@ -18216,7 +18213,7 @@
         <v>1</v>
       </c>
       <c r="AM159" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of little changes.
- Game is now in feature freeze, lets finish the current features, clean
  up the tests and launch.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD8C18E-24F0-214B-98C9-00161D21A8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Monsters" sheetId="1" r:id="rId1"/>
+    <sheet name="Monsters" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="338">
   <si>
     <t>name</t>
   </si>
@@ -999,7 +983,10 @@
     <t>Queen of the Gloom Wings</t>
   </si>
   <si>
-    <t>Storm Gian</t>
+    <t>Storm Giant</t>
+  </si>
+  <si>
+    <t>Lifes Flail</t>
   </si>
   <si>
     <t>Fire Kin Elemental</t>
@@ -1047,9 +1034,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1060,37 +1052,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -1380,46 +1363,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:AM159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J83" workbookViewId="0">
-      <selection activeCell="O110" sqref="O110"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="21" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="26" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="17" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="10" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="13" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="4" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="8" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="27" max="27" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="28" max="28" width="23" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="30" max="30" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="31" max="31" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="32" max="32" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="33" max="33" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="34" max="34" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="36" max="36" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="37" max="37" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="38" max="38" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="39" max="39" width="13" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1567,16 +1564,16 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="K2">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="L2">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="M2">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -1621,16 +1618,16 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AF2">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AG2">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AH2">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AI2">
         <v>0</v>
@@ -1648,7 +1645,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1677,16 +1674,16 @@
         <v>9</v>
       </c>
       <c r="J3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="K3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="M3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -1728,19 +1725,19 @@
         <v>2</v>
       </c>
       <c r="AD3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AE3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AF3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AG3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AH3">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AI3">
         <v>0</v>
@@ -1752,7 +1749,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1832,19 +1829,19 @@
         <v>2</v>
       </c>
       <c r="AD4">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="AE4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AF4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AG4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AH4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AI4">
         <v>0</v>
@@ -1856,7 +1853,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1936,19 +1933,19 @@
         <v>3</v>
       </c>
       <c r="AD5">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AE5">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AF5">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AG5">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AH5">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AI5">
         <v>0</v>
@@ -1960,7 +1957,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2037,7 @@
         <v>5</v>
       </c>
       <c r="AD6">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AE6">
         <v>0.01</v>
@@ -2070,7 +2067,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2290,7 +2287,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -2394,7 +2391,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2504,7 +2501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2614,7 +2611,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2643,16 +2640,16 @@
         <v>208</v>
       </c>
       <c r="J12">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K12">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="L12">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M12">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -2697,16 +2694,16 @@
         <v>0.15</v>
       </c>
       <c r="AE12">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AF12">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AG12">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AH12">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AI12">
         <v>0</v>
@@ -2724,7 +2721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -2828,7 +2825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -2932,7 +2929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -3042,7 +3039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -3125,16 +3122,16 @@
         <v>0.36</v>
       </c>
       <c r="AE16">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AF16">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AG16">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AH16">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AI16">
         <v>0</v>
@@ -3152,7 +3149,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -3256,7 +3253,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -3360,7 +3357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -3464,7 +3461,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -3547,16 +3544,16 @@
         <v>0.36</v>
       </c>
       <c r="AE20">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AF20">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AG20">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AH20">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AI20">
         <v>0</v>
@@ -3568,7 +3565,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -3672,7 +3669,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3776,7 +3773,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -3886,7 +3883,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -3990,7 +3987,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -4094,7 +4091,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -4198,7 +4195,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -4302,7 +4299,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39">
       <c r="A28" t="s">
         <v>122</v>
       </c>
@@ -4406,7 +4403,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -4510,7 +4507,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39">
       <c r="A30" t="s">
         <v>128</v>
       </c>
@@ -4614,13 +4611,13 @@
         <v>131</v>
       </c>
       <c r="AL30">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AM30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39">
       <c r="A31" t="s">
         <v>132</v>
       </c>
@@ -4649,16 +4646,16 @@
         <v>8</v>
       </c>
       <c r="J31">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="K31">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="L31">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="M31">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="Q31">
         <v>1</v>
@@ -4703,16 +4700,16 @@
         <v>0</v>
       </c>
       <c r="AE31">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AF31">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AG31">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AH31">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AI31">
         <v>0</v>
@@ -4724,7 +4721,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -4753,16 +4750,16 @@
         <v>9</v>
       </c>
       <c r="J32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="K32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="M32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="Q32">
         <v>1</v>
@@ -4804,19 +4801,19 @@
         <v>2</v>
       </c>
       <c r="AD32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AE32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AF32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AG32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AH32">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AI32">
         <v>0</v>
@@ -4828,7 +4825,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -4908,19 +4905,19 @@
         <v>2</v>
       </c>
       <c r="AD33">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="AE33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AF33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AG33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AH33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AI33">
         <v>0</v>
@@ -4932,7 +4929,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>136</v>
       </c>
@@ -5012,19 +5009,19 @@
         <v>3</v>
       </c>
       <c r="AD34">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AE34">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AF34">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AG34">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AH34">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AI34">
         <v>0</v>
@@ -5036,7 +5033,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -5116,7 +5113,7 @@
         <v>5</v>
       </c>
       <c r="AD35">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AE35">
         <v>0.01</v>
@@ -5140,7 +5137,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -5244,7 +5241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -5348,7 +5345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>140</v>
       </c>
@@ -5452,7 +5449,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>141</v>
       </c>
@@ -5556,7 +5553,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -5660,7 +5657,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -5689,16 +5686,16 @@
         <v>208</v>
       </c>
       <c r="J41">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="K41">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="L41">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="M41">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Q41">
         <v>1</v>
@@ -5743,16 +5740,16 @@
         <v>0.15</v>
       </c>
       <c r="AE41">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AF41">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AG41">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AH41">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AI41">
         <v>0</v>
@@ -5764,7 +5761,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39">
       <c r="A42" t="s">
         <v>144</v>
       </c>
@@ -5868,7 +5865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -5972,7 +5969,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -6076,7 +6073,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39">
       <c r="A45" t="s">
         <v>147</v>
       </c>
@@ -6180,7 +6177,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39">
       <c r="A46" t="s">
         <v>150</v>
       </c>
@@ -6284,7 +6281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39">
       <c r="A47" t="s">
         <v>151</v>
       </c>
@@ -6388,7 +6385,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -6471,16 +6468,16 @@
         <v>0.36</v>
       </c>
       <c r="AE48">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AF48">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AG48">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AH48">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="AI48">
         <v>0</v>
@@ -6492,7 +6489,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39">
       <c r="A49" t="s">
         <v>153</v>
       </c>
@@ -6596,7 +6593,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39">
       <c r="A50" t="s">
         <v>154</v>
       </c>
@@ -6706,7 +6703,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -6810,7 +6807,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39">
       <c r="A52" t="s">
         <v>157</v>
       </c>
@@ -6914,7 +6911,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -7024,7 +7021,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -7128,7 +7125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -7232,7 +7229,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -7342,7 +7339,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -7446,7 +7443,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -7550,7 +7547,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -7654,7 +7651,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -7758,7 +7755,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39">
       <c r="A61" t="s">
         <v>168</v>
       </c>
@@ -7862,7 +7859,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:39">
       <c r="A62" t="s">
         <v>171</v>
       </c>
@@ -7945,16 +7942,16 @@
         <v>1</v>
       </c>
       <c r="AE62">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AF62">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AG62">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AH62">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AI62">
         <v>0</v>
@@ -7966,7 +7963,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:39">
       <c r="A63" t="s">
         <v>174</v>
       </c>
@@ -8049,16 +8046,16 @@
         <v>1</v>
       </c>
       <c r="AE63">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AF63">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AG63">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AH63">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AI63">
         <v>0</v>
@@ -8070,7 +8067,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:39">
       <c r="A64" t="s">
         <v>177</v>
       </c>
@@ -8180,7 +8177,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:39">
       <c r="A65" t="s">
         <v>181</v>
       </c>
@@ -8299,7 +8296,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:39">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -8403,10 +8400,13 @@
         <v>1</v>
       </c>
       <c r="AI66">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AJ66">
         <v>1</v>
+      </c>
+      <c r="AK66" t="s">
+        <v>180</v>
       </c>
       <c r="AL66">
         <v>0.01</v>
@@ -8415,7 +8415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:39">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -8519,10 +8519,13 @@
         <v>1</v>
       </c>
       <c r="AI67">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="AJ67">
         <v>1</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>180</v>
       </c>
       <c r="AL67">
         <v>0.01</v>
@@ -8531,7 +8534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:39">
       <c r="A68" t="s">
         <v>189</v>
       </c>
@@ -8644,7 +8647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:39">
       <c r="A69" t="s">
         <v>192</v>
       </c>
@@ -8748,7 +8751,7 @@
         <v>1</v>
       </c>
       <c r="AI69">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AJ69">
         <v>1</v>
@@ -8757,7 +8760,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:39">
       <c r="A70" t="s">
         <v>195</v>
       </c>
@@ -8861,7 +8864,7 @@
         <v>1</v>
       </c>
       <c r="AI70">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="AJ70">
         <v>1</v>
@@ -8870,7 +8873,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:39">
       <c r="A71" t="s">
         <v>198</v>
       </c>
@@ -8979,11 +8982,17 @@
       <c r="AJ71">
         <v>1</v>
       </c>
+      <c r="AK71" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL71">
+        <v>0.2</v>
+      </c>
       <c r="AM71" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:39">
       <c r="A72" t="s">
         <v>202</v>
       </c>
@@ -9096,7 +9105,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:39">
       <c r="A73" t="s">
         <v>205</v>
       </c>
@@ -9209,7 +9218,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:39">
       <c r="A74" t="s">
         <v>208</v>
       </c>
@@ -9292,16 +9301,16 @@
         <v>0</v>
       </c>
       <c r="AE74">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AF74">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AG74">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AH74">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AI74">
         <v>0</v>
@@ -9313,7 +9322,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:39">
       <c r="A75" t="s">
         <v>209</v>
       </c>
@@ -9393,19 +9402,19 @@
         <v>2</v>
       </c>
       <c r="AD75">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AE75">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AF75">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AG75">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AH75">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="AI75">
         <v>0</v>
@@ -9417,7 +9426,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:39">
       <c r="A76" t="s">
         <v>210</v>
       </c>
@@ -9497,19 +9506,19 @@
         <v>2</v>
       </c>
       <c r="AD76">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="AE76">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AF76">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AG76">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AH76">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AI76">
         <v>0</v>
@@ -9521,7 +9530,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:39">
       <c r="A77" t="s">
         <v>211</v>
       </c>
@@ -9601,19 +9610,19 @@
         <v>3</v>
       </c>
       <c r="AD77">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="AE77">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AF77">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AG77">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AH77">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AI77">
         <v>0</v>
@@ -9625,7 +9634,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:39">
       <c r="A78" t="s">
         <v>212</v>
       </c>
@@ -9705,7 +9714,7 @@
         <v>5</v>
       </c>
       <c r="AD78">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AE78">
         <v>0.01</v>
@@ -9729,7 +9738,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:39">
       <c r="A79" t="s">
         <v>213</v>
       </c>
@@ -9833,7 +9842,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:39">
       <c r="A80" t="s">
         <v>214</v>
       </c>
@@ -9937,7 +9946,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:39">
       <c r="A81" t="s">
         <v>215</v>
       </c>
@@ -10041,7 +10050,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:39">
       <c r="A82" t="s">
         <v>216</v>
       </c>
@@ -10151,7 +10160,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:39">
       <c r="A83" t="s">
         <v>217</v>
       </c>
@@ -10255,7 +10264,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:39">
       <c r="A84" t="s">
         <v>218</v>
       </c>
@@ -10338,28 +10347,34 @@
         <v>0.15</v>
       </c>
       <c r="AE84">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AF84">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AG84">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AH84">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="AI84">
         <v>0</v>
       </c>
       <c r="AJ84">
         <v>1</v>
+      </c>
+      <c r="AK84" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL84">
+        <v>0.01</v>
       </c>
       <c r="AM84" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:39">
       <c r="A85" t="s">
         <v>219</v>
       </c>
@@ -10463,7 +10478,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:39">
       <c r="A86" t="s">
         <v>220</v>
       </c>
@@ -10567,7 +10582,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:39">
       <c r="A87" t="s">
         <v>221</v>
       </c>
@@ -10671,7 +10686,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:39">
       <c r="A88" t="s">
         <v>222</v>
       </c>
@@ -10775,7 +10790,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:39">
       <c r="A89" t="s">
         <v>223</v>
       </c>
@@ -10879,7 +10894,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:39">
       <c r="A90" t="s">
         <v>224</v>
       </c>
@@ -10983,7 +10998,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:39">
       <c r="A91" t="s">
         <v>225</v>
       </c>
@@ -11087,7 +11102,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:39">
       <c r="A92" t="s">
         <v>226</v>
       </c>
@@ -11191,7 +11206,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:39">
       <c r="A93" t="s">
         <v>227</v>
       </c>
@@ -11295,7 +11310,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:39">
       <c r="A94" t="s">
         <v>228</v>
       </c>
@@ -11399,7 +11414,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:39">
       <c r="A95" t="s">
         <v>229</v>
       </c>
@@ -11503,7 +11518,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:39">
       <c r="A96" t="s">
         <v>230</v>
       </c>
@@ -11607,7 +11622,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:39">
       <c r="A97" t="s">
         <v>231</v>
       </c>
@@ -11711,7 +11726,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:39">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -11815,7 +11830,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:39">
       <c r="A99" t="s">
         <v>233</v>
       </c>
@@ -11919,7 +11934,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:39">
       <c r="A100" t="s">
         <v>234</v>
       </c>
@@ -12023,7 +12038,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:39">
       <c r="A101" t="s">
         <v>235</v>
       </c>
@@ -12127,7 +12142,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:39">
       <c r="A102" t="s">
         <v>236</v>
       </c>
@@ -12231,7 +12246,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:39">
       <c r="A103" t="s">
         <v>237</v>
       </c>
@@ -12335,7 +12350,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="104" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:39">
       <c r="A104" t="s">
         <v>238</v>
       </c>
@@ -12418,16 +12433,16 @@
         <v>1</v>
       </c>
       <c r="AE104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AF104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AG104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AH104">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="AI104">
         <v>0</v>
@@ -12439,7 +12454,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="105" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:39">
       <c r="A105" t="s">
         <v>239</v>
       </c>
@@ -12522,16 +12537,16 @@
         <v>1</v>
       </c>
       <c r="AE105">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AF105">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AG105">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AH105">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="AI105">
         <v>0</v>
@@ -12543,7 +12558,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="106" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:39">
       <c r="A106" t="s">
         <v>240</v>
       </c>
@@ -12647,7 +12662,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="107" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:39">
       <c r="A107" t="s">
         <v>241</v>
       </c>
@@ -12760,7 +12775,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="108" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:39">
       <c r="A108" t="s">
         <v>244</v>
       </c>
@@ -12873,7 +12888,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="109" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:39">
       <c r="A109" t="s">
         <v>247</v>
       </c>
@@ -12986,7 +13001,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="110" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:39">
       <c r="A110" t="s">
         <v>250</v>
       </c>
@@ -13099,7 +13114,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:39">
       <c r="A111" t="s">
         <v>253</v>
       </c>
@@ -13212,7 +13227,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="112" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:39">
       <c r="A112" t="s">
         <v>256</v>
       </c>
@@ -13316,7 +13331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:39">
       <c r="A113" t="s">
         <v>259</v>
       </c>
@@ -13420,7 +13435,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:39">
       <c r="A114" t="s">
         <v>262</v>
       </c>
@@ -13524,7 +13539,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:39">
       <c r="A115" t="s">
         <v>265</v>
       </c>
@@ -13628,7 +13643,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:39">
       <c r="A116" t="s">
         <v>268</v>
       </c>
@@ -13732,7 +13747,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:39">
       <c r="A117" t="s">
         <v>271</v>
       </c>
@@ -13836,7 +13851,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:39">
       <c r="A118" t="s">
         <v>274</v>
       </c>
@@ -13919,16 +13934,16 @@
         <v>1</v>
       </c>
       <c r="AE118">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AF118">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AG118">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AH118">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AI118">
         <v>0.1</v>
@@ -13940,7 +13955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:39">
       <c r="A119" t="s">
         <v>277</v>
       </c>
@@ -14044,7 +14059,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:39">
       <c r="A120" t="s">
         <v>280</v>
       </c>
@@ -14148,7 +14163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:39">
       <c r="A121" t="s">
         <v>283</v>
       </c>
@@ -14252,7 +14267,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="122" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:39">
       <c r="A122" t="s">
         <v>286</v>
       </c>
@@ -14356,7 +14371,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="123" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:39">
       <c r="A123" t="s">
         <v>289</v>
       </c>
@@ -14460,7 +14475,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:39">
       <c r="A124" t="s">
         <v>291</v>
       </c>
@@ -14564,7 +14579,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:39">
       <c r="A125" t="s">
         <v>294</v>
       </c>
@@ -14668,7 +14683,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:39">
       <c r="A126" t="s">
         <v>297</v>
       </c>
@@ -14772,7 +14787,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:39">
       <c r="A127" t="s">
         <v>300</v>
       </c>
@@ -14876,7 +14891,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:39">
       <c r="A128" t="s">
         <v>302</v>
       </c>
@@ -14980,7 +14995,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:39">
       <c r="A129" t="s">
         <v>303</v>
       </c>
@@ -15084,7 +15099,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:39">
       <c r="A130" t="s">
         <v>304</v>
       </c>
@@ -15188,7 +15203,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="131" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:39">
       <c r="A131" t="s">
         <v>305</v>
       </c>
@@ -15292,7 +15307,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:39">
       <c r="A132" t="s">
         <v>306</v>
       </c>
@@ -15396,7 +15411,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="133" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:39">
       <c r="A133" t="s">
         <v>307</v>
       </c>
@@ -15500,7 +15515,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:39">
       <c r="A134" t="s">
         <v>308</v>
       </c>
@@ -15583,16 +15598,16 @@
         <v>1</v>
       </c>
       <c r="AE134">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AF134">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AG134">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AH134">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AI134">
         <v>0.1</v>
@@ -15604,7 +15619,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:39">
       <c r="A135" t="s">
         <v>309</v>
       </c>
@@ -15708,7 +15723,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:39">
       <c r="A136" t="s">
         <v>310</v>
       </c>
@@ -15812,7 +15827,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:39">
       <c r="A137" t="s">
         <v>311</v>
       </c>
@@ -15916,7 +15931,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="138" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:39">
       <c r="A138" t="s">
         <v>312</v>
       </c>
@@ -16020,7 +16035,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="139" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:39">
       <c r="A139" t="s">
         <v>313</v>
       </c>
@@ -16124,7 +16139,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="140" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:39">
       <c r="A140" t="s">
         <v>314</v>
       </c>
@@ -16228,7 +16243,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:39">
       <c r="A141" t="s">
         <v>315</v>
       </c>
@@ -16332,7 +16347,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="142" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:39">
       <c r="A142" t="s">
         <v>316</v>
       </c>
@@ -16436,7 +16451,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:39">
       <c r="A143" t="s">
         <v>317</v>
       </c>
@@ -16540,7 +16555,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="144" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:39">
       <c r="A144" t="s">
         <v>318</v>
       </c>
@@ -16644,7 +16659,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="145" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:39">
       <c r="A145" t="s">
         <v>319</v>
       </c>
@@ -16748,7 +16763,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="146" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:39">
       <c r="A146" t="s">
         <v>320</v>
       </c>
@@ -16852,7 +16867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="147" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:39">
       <c r="A147" t="s">
         <v>321</v>
       </c>
@@ -16956,7 +16971,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="148" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:39">
       <c r="A148" t="s">
         <v>322</v>
       </c>
@@ -17056,13 +17071,19 @@
       <c r="AJ148">
         <v>1</v>
       </c>
+      <c r="AK148" t="s">
+        <v>323</v>
+      </c>
+      <c r="AL148">
+        <v>0.001</v>
+      </c>
       <c r="AM148" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="149" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:39">
       <c r="A149" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B149">
         <v>500000</v>
@@ -17164,9 +17185,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="150" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:39">
       <c r="A150" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B150">
         <v>560000</v>
@@ -17247,16 +17268,16 @@
         <v>1</v>
       </c>
       <c r="AE150">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AF150">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AG150">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AH150">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AI150">
         <v>0.1</v>
@@ -17268,9 +17289,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="151" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:39">
       <c r="A151" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B151">
         <v>600000</v>
@@ -17372,9 +17393,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="152" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:39">
       <c r="A152" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B152">
         <v>670000</v>
@@ -17476,9 +17497,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="153" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:39">
       <c r="A153" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B153">
         <v>720000</v>
@@ -17580,9 +17601,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="154" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:39">
       <c r="A154" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B154">
         <v>750000</v>
@@ -17684,9 +17705,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="155" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:39">
       <c r="A155" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B155">
         <v>775000</v>
@@ -17788,9 +17809,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:39">
       <c r="A156" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B156">
         <v>800000</v>
@@ -17892,9 +17913,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="157" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:39">
       <c r="A157" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B157">
         <v>825000</v>
@@ -17960,7 +17981,7 @@
         <v>295</v>
       </c>
       <c r="Z157" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AA157">
         <v>300000</v>
@@ -17996,9 +18017,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="158" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:39">
       <c r="A158" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B158">
         <v>850000</v>
@@ -18064,7 +18085,7 @@
         <v>298</v>
       </c>
       <c r="Z158" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AA158">
         <v>345000</v>
@@ -18100,9 +18121,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="159" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:39">
       <c r="A159" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B159">
         <v>875000</v>
@@ -18168,7 +18189,7 @@
         <v>206</v>
       </c>
       <c r="Z159" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AA159">
         <v>368000</v>
@@ -18205,8 +18226,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor fixes and additional monsters
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F0AD22-FEA1-DD4F-AA02-4F64A19BF385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA9B339-6CBA-7F40-9CF4-CF7A4C02BBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="723">
   <si>
     <t>name</t>
   </si>
@@ -2065,6 +2065,141 @@
   </si>
   <si>
     <t>Unholy Sin of Man</t>
+  </si>
+  <si>
+    <t>Minions of Purgatory</t>
+  </si>
+  <si>
+    <t>Prison Gaurd of Kalitar</t>
+  </si>
+  <si>
+    <t>Corrupted Satan Child</t>
+  </si>
+  <si>
+    <t>Cosmic Mage of Doom</t>
+  </si>
+  <si>
+    <t>Clerics Sinful Soul</t>
+  </si>
+  <si>
+    <t>Abominated Eyeball of Fate</t>
+  </si>
+  <si>
+    <t>Cosmic God of All Dragon Kin</t>
+  </si>
+  <si>
+    <t>Fates Skull of Hope</t>
+  </si>
+  <si>
+    <t>Skeleton Lord of the Dungeons</t>
+  </si>
+  <si>
+    <t>Mage of the Labyrinth Experiment</t>
+  </si>
+  <si>
+    <t>Shadow Lands Fate Prophet</t>
+  </si>
+  <si>
+    <t>Fighter of the Seventh Surface Order</t>
+  </si>
+  <si>
+    <t>Hells Chosen Champion of Hate</t>
+  </si>
+  <si>
+    <t>Angelic Celesial Heretic of the Heavens</t>
+  </si>
+  <si>
+    <t>Satanic Wild Hunter of the Rose</t>
+  </si>
+  <si>
+    <t>Wiches Wild Hunt God</t>
+  </si>
+  <si>
+    <t>Pegan God of Festive Canabalistic Feast</t>
+  </si>
+  <si>
+    <t>Demonic Summoning of Kalitar</t>
+  </si>
+  <si>
+    <t>Shadow Demon of Colosus</t>
+  </si>
+  <si>
+    <t>Demonic Baby Soul of Winged Corruption</t>
+  </si>
+  <si>
+    <t>Sun God of Cosmic Rays</t>
+  </si>
+  <si>
+    <t>Faithless Ambomination of Purgatories Heart</t>
+  </si>
+  <si>
+    <t>Purgatories Beating heart</t>
+  </si>
+  <si>
+    <t>125756789900000-128976450900000</t>
+  </si>
+  <si>
+    <t>135987767890000-138967487560000</t>
+  </si>
+  <si>
+    <t>142658798654656-145000000000000</t>
+  </si>
+  <si>
+    <t>148767465687000-153876657690000</t>
+  </si>
+  <si>
+    <t>155978676485000-158977749680000</t>
+  </si>
+  <si>
+    <t>164967490674000-168957355874000</t>
+  </si>
+  <si>
+    <t>173967583650000-175879847657600</t>
+  </si>
+  <si>
+    <t>178746476350000-183757646556000</t>
+  </si>
+  <si>
+    <t>186764565350000-193865764868000</t>
+  </si>
+  <si>
+    <t>195766365452000-198565365456000</t>
+  </si>
+  <si>
+    <t>205765876576600-208564764656000</t>
+  </si>
+  <si>
+    <t>215677576445000-219664763374000</t>
+  </si>
+  <si>
+    <t>223764754330000-228567646476400</t>
+  </si>
+  <si>
+    <t>234746547620000-238347566647000</t>
+  </si>
+  <si>
+    <t>243456627635600-246576476435000</t>
+  </si>
+  <si>
+    <t>253576365474000-258675764560000</t>
+  </si>
+  <si>
+    <t>265345876466000-268385476485000</t>
+  </si>
+  <si>
+    <t>273387456587000-275827466587000</t>
+  </si>
+  <si>
+    <t>278576454454000-285658756376000</t>
+  </si>
+  <si>
+    <t>288576476473740-294476576373000</t>
+  </si>
+  <si>
+    <t>299376465477000-304875864856500</t>
+  </si>
+  <si>
+    <t>308476637656600-312476476445500</t>
   </si>
 </sst>
 </file>
@@ -2404,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM371"/>
+  <dimension ref="A1:AM394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="I371" sqref="I371"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="T393" sqref="T393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40030,7 +40165,7 @@
         <v>1</v>
       </c>
       <c r="U358">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="V358">
         <v>1E-3</v>
@@ -40134,7 +40269,7 @@
         <v>1</v>
       </c>
       <c r="U359">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="V359">
         <v>1E-3</v>
@@ -40238,7 +40373,7 @@
         <v>3</v>
       </c>
       <c r="U360">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="V360">
         <v>1E-3</v>
@@ -40342,7 +40477,7 @@
         <v>7</v>
       </c>
       <c r="U361">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="V361">
         <v>1E-3</v>
@@ -40446,7 +40581,7 @@
         <v>5</v>
       </c>
       <c r="U362">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="V362">
         <v>1E-3</v>
@@ -40550,7 +40685,7 @@
         <v>4</v>
       </c>
       <c r="U363">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="V363">
         <v>1E-3</v>
@@ -40654,7 +40789,7 @@
         <v>6</v>
       </c>
       <c r="U364">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="V364">
         <v>1E-3</v>
@@ -40758,7 +40893,7 @@
         <v>3</v>
       </c>
       <c r="U365">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="V365">
         <v>1E-3</v>
@@ -40862,7 +40997,7 @@
         <v>4</v>
       </c>
       <c r="U366">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="V366">
         <v>1E-3</v>
@@ -40966,7 +41101,7 @@
         <v>7</v>
       </c>
       <c r="U367">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="V367">
         <v>1E-3</v>
@@ -41070,7 +41205,7 @@
         <v>5</v>
       </c>
       <c r="U368">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="V368">
         <v>1E-3</v>
@@ -41174,7 +41309,7 @@
         <v>1</v>
       </c>
       <c r="U369">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="V369">
         <v>1E-3</v>
@@ -41278,7 +41413,7 @@
         <v>3</v>
       </c>
       <c r="U370">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="V370">
         <v>1E-3</v>
@@ -41382,7 +41517,7 @@
         <v>4</v>
       </c>
       <c r="U371">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="V371">
         <v>1E-3</v>
@@ -41431,6 +41566,2335 @@
       </c>
       <c r="AM371" t="s">
         <v>651</v>
+      </c>
+    </row>
+    <row r="372" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A372" t="s">
+        <v>678</v>
+      </c>
+      <c r="B372">
+        <v>113000000000000</v>
+      </c>
+      <c r="C372">
+        <v>113000000000000</v>
+      </c>
+      <c r="D372">
+        <v>113000000000000</v>
+      </c>
+      <c r="E372">
+        <v>113000000000000</v>
+      </c>
+      <c r="F372">
+        <v>113000000000000</v>
+      </c>
+      <c r="G372">
+        <v>113000000000000</v>
+      </c>
+      <c r="H372">
+        <v>113000000000000</v>
+      </c>
+      <c r="I372">
+        <v>113000000000000</v>
+      </c>
+      <c r="J372">
+        <v>8.6333333333333293</v>
+      </c>
+      <c r="K372">
+        <v>8.6333333333333293</v>
+      </c>
+      <c r="L372">
+        <v>8.6333333333333293</v>
+      </c>
+      <c r="M372">
+        <v>8.6333333333333293</v>
+      </c>
+      <c r="Q372">
+        <v>1</v>
+      </c>
+      <c r="R372">
+        <v>1</v>
+      </c>
+      <c r="S372">
+        <v>99999</v>
+      </c>
+      <c r="T372" t="s">
+        <v>3</v>
+      </c>
+      <c r="U372">
+        <v>42</v>
+      </c>
+      <c r="V372">
+        <v>1E-3</v>
+      </c>
+      <c r="W372">
+        <v>300000000</v>
+      </c>
+      <c r="X372">
+        <v>0</v>
+      </c>
+      <c r="Y372" t="s">
+        <v>701</v>
+      </c>
+      <c r="Z372" t="s">
+        <v>701</v>
+      </c>
+      <c r="AA372">
+        <v>113000000000000</v>
+      </c>
+      <c r="AB372">
+        <v>113000000000000</v>
+      </c>
+      <c r="AC372">
+        <v>113000000000000</v>
+      </c>
+      <c r="AD372">
+        <v>1</v>
+      </c>
+      <c r="AE372">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AF372">
+        <v>5.7</v>
+      </c>
+      <c r="AG372">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AH372">
+        <v>4.8</v>
+      </c>
+      <c r="AI372">
+        <v>7.7</v>
+      </c>
+      <c r="AJ372">
+        <v>1</v>
+      </c>
+      <c r="AM372" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="373" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A373" t="s">
+        <v>679</v>
+      </c>
+      <c r="B373">
+        <v>120000000000000</v>
+      </c>
+      <c r="C373">
+        <v>120000000000000</v>
+      </c>
+      <c r="D373">
+        <v>120000000000000</v>
+      </c>
+      <c r="E373">
+        <v>120000000000000</v>
+      </c>
+      <c r="F373">
+        <v>120000000000000</v>
+      </c>
+      <c r="G373">
+        <v>120000000000000</v>
+      </c>
+      <c r="H373">
+        <v>120000000000000</v>
+      </c>
+      <c r="I373">
+        <v>120000000000000</v>
+      </c>
+      <c r="J373">
+        <v>9.0333333333333297</v>
+      </c>
+      <c r="K373">
+        <v>9.0333333333333297</v>
+      </c>
+      <c r="L373">
+        <v>9.0333333333333297</v>
+      </c>
+      <c r="M373">
+        <v>9.0333333333333297</v>
+      </c>
+      <c r="Q373">
+        <v>1</v>
+      </c>
+      <c r="R373">
+        <v>1</v>
+      </c>
+      <c r="S373">
+        <v>99999</v>
+      </c>
+      <c r="T373" t="s">
+        <v>1</v>
+      </c>
+      <c r="U373">
+        <v>42</v>
+      </c>
+      <c r="V373">
+        <v>1E-3</v>
+      </c>
+      <c r="W373">
+        <v>310000000</v>
+      </c>
+      <c r="X373">
+        <v>0</v>
+      </c>
+      <c r="Y373" t="s">
+        <v>702</v>
+      </c>
+      <c r="Z373" t="s">
+        <v>702</v>
+      </c>
+      <c r="AA373">
+        <v>120000000000000</v>
+      </c>
+      <c r="AB373">
+        <v>120000000000000</v>
+      </c>
+      <c r="AC373">
+        <v>120000000000000</v>
+      </c>
+      <c r="AD373">
+        <v>1</v>
+      </c>
+      <c r="AE373">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AF373">
+        <v>6</v>
+      </c>
+      <c r="AG373">
+        <v>4.8</v>
+      </c>
+      <c r="AH373">
+        <v>5</v>
+      </c>
+      <c r="AI373">
+        <v>8.1</v>
+      </c>
+      <c r="AJ373">
+        <v>1</v>
+      </c>
+      <c r="AM373" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="374" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A374" t="s">
+        <v>680</v>
+      </c>
+      <c r="B374">
+        <v>127000000000000</v>
+      </c>
+      <c r="C374">
+        <v>127000000000000</v>
+      </c>
+      <c r="D374">
+        <v>127000000000000</v>
+      </c>
+      <c r="E374">
+        <v>127000000000000</v>
+      </c>
+      <c r="F374">
+        <v>127000000000000</v>
+      </c>
+      <c r="G374">
+        <v>127000000000000</v>
+      </c>
+      <c r="H374">
+        <v>127000000000000</v>
+      </c>
+      <c r="I374">
+        <v>127000000000000</v>
+      </c>
+      <c r="J374">
+        <v>9.43333333333333</v>
+      </c>
+      <c r="K374">
+        <v>9.43333333333333</v>
+      </c>
+      <c r="L374">
+        <v>9.43333333333333</v>
+      </c>
+      <c r="M374">
+        <v>9.43333333333333</v>
+      </c>
+      <c r="Q374">
+        <v>1</v>
+      </c>
+      <c r="R374">
+        <v>1</v>
+      </c>
+      <c r="S374">
+        <v>99999</v>
+      </c>
+      <c r="T374" t="s">
+        <v>1</v>
+      </c>
+      <c r="U374">
+        <v>42</v>
+      </c>
+      <c r="V374">
+        <v>1E-3</v>
+      </c>
+      <c r="W374">
+        <v>320000000</v>
+      </c>
+      <c r="X374">
+        <v>0</v>
+      </c>
+      <c r="Y374" t="s">
+        <v>703</v>
+      </c>
+      <c r="Z374" t="s">
+        <v>703</v>
+      </c>
+      <c r="AA374">
+        <v>127000000000000</v>
+      </c>
+      <c r="AB374">
+        <v>127000000000000</v>
+      </c>
+      <c r="AC374">
+        <v>127000000000000</v>
+      </c>
+      <c r="AD374">
+        <v>1</v>
+      </c>
+      <c r="AE374">
+        <v>4.8</v>
+      </c>
+      <c r="AF374">
+        <v>6.3</v>
+      </c>
+      <c r="AG374">
+        <v>5</v>
+      </c>
+      <c r="AH374">
+        <v>5.2</v>
+      </c>
+      <c r="AI374">
+        <v>8.5</v>
+      </c>
+      <c r="AJ374">
+        <v>1</v>
+      </c>
+      <c r="AM374" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="375" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A375" t="s">
+        <v>681</v>
+      </c>
+      <c r="B375">
+        <v>134000000000000</v>
+      </c>
+      <c r="C375">
+        <v>134000000000000</v>
+      </c>
+      <c r="D375">
+        <v>134000000000000</v>
+      </c>
+      <c r="E375">
+        <v>134000000000000</v>
+      </c>
+      <c r="F375">
+        <v>134000000000000</v>
+      </c>
+      <c r="G375">
+        <v>134000000000000</v>
+      </c>
+      <c r="H375">
+        <v>134000000000000</v>
+      </c>
+      <c r="I375">
+        <v>134000000000000</v>
+      </c>
+      <c r="J375">
+        <v>9.8333333333333197</v>
+      </c>
+      <c r="K375">
+        <v>9.8333333333333197</v>
+      </c>
+      <c r="L375">
+        <v>9.8333333333333197</v>
+      </c>
+      <c r="M375">
+        <v>9.8333333333333197</v>
+      </c>
+      <c r="Q375">
+        <v>1</v>
+      </c>
+      <c r="R375">
+        <v>1</v>
+      </c>
+      <c r="S375">
+        <v>99999</v>
+      </c>
+      <c r="T375" t="s">
+        <v>3</v>
+      </c>
+      <c r="U375">
+        <v>42</v>
+      </c>
+      <c r="V375">
+        <v>1E-3</v>
+      </c>
+      <c r="W375">
+        <v>330000000</v>
+      </c>
+      <c r="X375">
+        <v>0</v>
+      </c>
+      <c r="Y375" t="s">
+        <v>704</v>
+      </c>
+      <c r="Z375" t="s">
+        <v>704</v>
+      </c>
+      <c r="AA375">
+        <v>134000000000000</v>
+      </c>
+      <c r="AB375">
+        <v>134000000000000</v>
+      </c>
+      <c r="AC375">
+        <v>134000000000000</v>
+      </c>
+      <c r="AD375">
+        <v>1</v>
+      </c>
+      <c r="AE375">
+        <v>5</v>
+      </c>
+      <c r="AF375">
+        <v>6.6</v>
+      </c>
+      <c r="AG375">
+        <v>5.2</v>
+      </c>
+      <c r="AH375">
+        <v>5.4</v>
+      </c>
+      <c r="AI375">
+        <v>8.9</v>
+      </c>
+      <c r="AJ375">
+        <v>1</v>
+      </c>
+      <c r="AM375" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="376" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>682</v>
+      </c>
+      <c r="B376">
+        <v>141000000000000</v>
+      </c>
+      <c r="C376">
+        <v>141000000000000</v>
+      </c>
+      <c r="D376">
+        <v>141000000000000</v>
+      </c>
+      <c r="E376">
+        <v>141000000000000</v>
+      </c>
+      <c r="F376">
+        <v>141000000000000</v>
+      </c>
+      <c r="G376">
+        <v>141000000000000</v>
+      </c>
+      <c r="H376">
+        <v>141000000000000</v>
+      </c>
+      <c r="I376">
+        <v>141000000000000</v>
+      </c>
+      <c r="J376">
+        <v>10.233333333333301</v>
+      </c>
+      <c r="K376">
+        <v>10.233333333333301</v>
+      </c>
+      <c r="L376">
+        <v>10.233333333333301</v>
+      </c>
+      <c r="M376">
+        <v>10.233333333333301</v>
+      </c>
+      <c r="Q376">
+        <v>1</v>
+      </c>
+      <c r="R376">
+        <v>1</v>
+      </c>
+      <c r="S376">
+        <v>99999</v>
+      </c>
+      <c r="T376" t="s">
+        <v>7</v>
+      </c>
+      <c r="U376">
+        <v>42</v>
+      </c>
+      <c r="V376">
+        <v>1E-3</v>
+      </c>
+      <c r="W376">
+        <v>340000000</v>
+      </c>
+      <c r="X376">
+        <v>0</v>
+      </c>
+      <c r="Y376" t="s">
+        <v>705</v>
+      </c>
+      <c r="Z376" t="s">
+        <v>705</v>
+      </c>
+      <c r="AA376">
+        <v>141000000000000</v>
+      </c>
+      <c r="AB376">
+        <v>141000000000000</v>
+      </c>
+      <c r="AC376">
+        <v>141000000000000</v>
+      </c>
+      <c r="AD376">
+        <v>1</v>
+      </c>
+      <c r="AE376">
+        <v>5.2</v>
+      </c>
+      <c r="AF376">
+        <v>6.9</v>
+      </c>
+      <c r="AG376">
+        <v>5.4</v>
+      </c>
+      <c r="AH376">
+        <v>5.6</v>
+      </c>
+      <c r="AI376">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AJ376">
+        <v>1</v>
+      </c>
+      <c r="AM376" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="377" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
+        <v>683</v>
+      </c>
+      <c r="B377">
+        <v>148000000000000</v>
+      </c>
+      <c r="C377">
+        <v>148000000000000</v>
+      </c>
+      <c r="D377">
+        <v>148000000000000</v>
+      </c>
+      <c r="E377">
+        <v>148000000000000</v>
+      </c>
+      <c r="F377">
+        <v>148000000000000</v>
+      </c>
+      <c r="G377">
+        <v>148000000000000</v>
+      </c>
+      <c r="H377">
+        <v>148000000000000</v>
+      </c>
+      <c r="I377">
+        <v>148000000000000</v>
+      </c>
+      <c r="J377">
+        <v>10.633333333333301</v>
+      </c>
+      <c r="K377">
+        <v>10.633333333333301</v>
+      </c>
+      <c r="L377">
+        <v>10.633333333333301</v>
+      </c>
+      <c r="M377">
+        <v>10.633333333333301</v>
+      </c>
+      <c r="Q377">
+        <v>1</v>
+      </c>
+      <c r="R377">
+        <v>1</v>
+      </c>
+      <c r="S377">
+        <v>99999</v>
+      </c>
+      <c r="T377" t="s">
+        <v>5</v>
+      </c>
+      <c r="U377">
+        <v>42</v>
+      </c>
+      <c r="V377">
+        <v>1E-3</v>
+      </c>
+      <c r="W377">
+        <v>350000000</v>
+      </c>
+      <c r="X377">
+        <v>0</v>
+      </c>
+      <c r="Y377" t="s">
+        <v>706</v>
+      </c>
+      <c r="Z377" t="s">
+        <v>706</v>
+      </c>
+      <c r="AA377">
+        <v>148000000000000</v>
+      </c>
+      <c r="AB377">
+        <v>148000000000000</v>
+      </c>
+      <c r="AC377">
+        <v>148000000000000</v>
+      </c>
+      <c r="AD377">
+        <v>1</v>
+      </c>
+      <c r="AE377">
+        <v>5.4</v>
+      </c>
+      <c r="AF377">
+        <v>7.2</v>
+      </c>
+      <c r="AG377">
+        <v>5.6</v>
+      </c>
+      <c r="AH377">
+        <v>5.8</v>
+      </c>
+      <c r="AI377">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AJ377">
+        <v>1</v>
+      </c>
+      <c r="AM377" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="378" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
+        <v>684</v>
+      </c>
+      <c r="B378">
+        <v>155000000000000</v>
+      </c>
+      <c r="C378">
+        <v>155000000000000</v>
+      </c>
+      <c r="D378">
+        <v>155000000000000</v>
+      </c>
+      <c r="E378">
+        <v>155000000000000</v>
+      </c>
+      <c r="F378">
+        <v>155000000000000</v>
+      </c>
+      <c r="G378">
+        <v>155000000000000</v>
+      </c>
+      <c r="H378">
+        <v>155000000000000</v>
+      </c>
+      <c r="I378">
+        <v>155000000000000</v>
+      </c>
+      <c r="J378">
+        <v>11.033333333333299</v>
+      </c>
+      <c r="K378">
+        <v>11.033333333333299</v>
+      </c>
+      <c r="L378">
+        <v>11.033333333333299</v>
+      </c>
+      <c r="M378">
+        <v>11.033333333333299</v>
+      </c>
+      <c r="Q378">
+        <v>1</v>
+      </c>
+      <c r="R378">
+        <v>1</v>
+      </c>
+      <c r="S378">
+        <v>99999</v>
+      </c>
+      <c r="T378" t="s">
+        <v>4</v>
+      </c>
+      <c r="U378">
+        <v>42</v>
+      </c>
+      <c r="V378">
+        <v>1E-3</v>
+      </c>
+      <c r="W378">
+        <v>360000000</v>
+      </c>
+      <c r="X378">
+        <v>0</v>
+      </c>
+      <c r="Y378" t="s">
+        <v>707</v>
+      </c>
+      <c r="Z378" t="s">
+        <v>707</v>
+      </c>
+      <c r="AA378">
+        <v>155000000000000</v>
+      </c>
+      <c r="AB378">
+        <v>155000000000000</v>
+      </c>
+      <c r="AC378">
+        <v>155000000000000</v>
+      </c>
+      <c r="AD378">
+        <v>1</v>
+      </c>
+      <c r="AE378">
+        <v>5.6</v>
+      </c>
+      <c r="AF378">
+        <v>7.5</v>
+      </c>
+      <c r="AG378">
+        <v>5.8</v>
+      </c>
+      <c r="AH378">
+        <v>6</v>
+      </c>
+      <c r="AI378">
+        <v>10.1</v>
+      </c>
+      <c r="AJ378">
+        <v>1</v>
+      </c>
+      <c r="AM378" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="379" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
+        <v>685</v>
+      </c>
+      <c r="B379">
+        <v>162000000000000</v>
+      </c>
+      <c r="C379">
+        <v>162000000000000</v>
+      </c>
+      <c r="D379">
+        <v>162000000000000</v>
+      </c>
+      <c r="E379">
+        <v>162000000000000</v>
+      </c>
+      <c r="F379">
+        <v>162000000000000</v>
+      </c>
+      <c r="G379">
+        <v>162000000000000</v>
+      </c>
+      <c r="H379">
+        <v>162000000000000</v>
+      </c>
+      <c r="I379">
+        <v>162000000000000</v>
+      </c>
+      <c r="J379">
+        <v>11.4333333333333</v>
+      </c>
+      <c r="K379">
+        <v>11.4333333333333</v>
+      </c>
+      <c r="L379">
+        <v>11.4333333333333</v>
+      </c>
+      <c r="M379">
+        <v>11.4333333333333</v>
+      </c>
+      <c r="Q379">
+        <v>1</v>
+      </c>
+      <c r="R379">
+        <v>1</v>
+      </c>
+      <c r="S379">
+        <v>99999</v>
+      </c>
+      <c r="T379" t="s">
+        <v>6</v>
+      </c>
+      <c r="U379">
+        <v>44</v>
+      </c>
+      <c r="V379">
+        <v>1E-3</v>
+      </c>
+      <c r="W379">
+        <v>370000000</v>
+      </c>
+      <c r="X379">
+        <v>0</v>
+      </c>
+      <c r="Y379" t="s">
+        <v>708</v>
+      </c>
+      <c r="Z379" t="s">
+        <v>708</v>
+      </c>
+      <c r="AA379">
+        <v>162000000000000</v>
+      </c>
+      <c r="AB379">
+        <v>162000000000000</v>
+      </c>
+      <c r="AC379">
+        <v>162000000000000</v>
+      </c>
+      <c r="AD379">
+        <v>1</v>
+      </c>
+      <c r="AE379">
+        <v>5.8</v>
+      </c>
+      <c r="AF379">
+        <v>7.8</v>
+      </c>
+      <c r="AG379">
+        <v>6</v>
+      </c>
+      <c r="AH379">
+        <v>6.2</v>
+      </c>
+      <c r="AI379">
+        <v>10.5</v>
+      </c>
+      <c r="AJ379">
+        <v>1</v>
+      </c>
+      <c r="AM379" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="380" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>686</v>
+      </c>
+      <c r="B380">
+        <v>169000000000000</v>
+      </c>
+      <c r="C380">
+        <v>169000000000000</v>
+      </c>
+      <c r="D380">
+        <v>169000000000000</v>
+      </c>
+      <c r="E380">
+        <v>169000000000000</v>
+      </c>
+      <c r="F380">
+        <v>169000000000000</v>
+      </c>
+      <c r="G380">
+        <v>169000000000000</v>
+      </c>
+      <c r="H380">
+        <v>169000000000000</v>
+      </c>
+      <c r="I380">
+        <v>169000000000000</v>
+      </c>
+      <c r="J380">
+        <v>11.8333333333333</v>
+      </c>
+      <c r="K380">
+        <v>11.8333333333333</v>
+      </c>
+      <c r="L380">
+        <v>11.8333333333333</v>
+      </c>
+      <c r="M380">
+        <v>11.8333333333333</v>
+      </c>
+      <c r="Q380">
+        <v>1</v>
+      </c>
+      <c r="R380">
+        <v>1</v>
+      </c>
+      <c r="S380">
+        <v>99999</v>
+      </c>
+      <c r="T380" t="s">
+        <v>3</v>
+      </c>
+      <c r="U380">
+        <v>45</v>
+      </c>
+      <c r="V380">
+        <v>1E-3</v>
+      </c>
+      <c r="W380">
+        <v>380000000</v>
+      </c>
+      <c r="X380">
+        <v>0</v>
+      </c>
+      <c r="Y380" t="s">
+        <v>709</v>
+      </c>
+      <c r="Z380" t="s">
+        <v>709</v>
+      </c>
+      <c r="AA380">
+        <v>169000000000000</v>
+      </c>
+      <c r="AB380">
+        <v>169000000000000</v>
+      </c>
+      <c r="AC380">
+        <v>169000000000000</v>
+      </c>
+      <c r="AD380">
+        <v>1</v>
+      </c>
+      <c r="AE380">
+        <v>6</v>
+      </c>
+      <c r="AF380">
+        <v>8.1</v>
+      </c>
+      <c r="AG380">
+        <v>6.2</v>
+      </c>
+      <c r="AH380">
+        <v>6.4</v>
+      </c>
+      <c r="AI380">
+        <v>10.9</v>
+      </c>
+      <c r="AJ380">
+        <v>1</v>
+      </c>
+      <c r="AM380" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="381" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A381" t="s">
+        <v>687</v>
+      </c>
+      <c r="B381">
+        <v>176000000000000</v>
+      </c>
+      <c r="C381">
+        <v>176000000000000</v>
+      </c>
+      <c r="D381">
+        <v>176000000000000</v>
+      </c>
+      <c r="E381">
+        <v>176000000000000</v>
+      </c>
+      <c r="F381">
+        <v>176000000000000</v>
+      </c>
+      <c r="G381">
+        <v>176000000000000</v>
+      </c>
+      <c r="H381">
+        <v>176000000000000</v>
+      </c>
+      <c r="I381">
+        <v>176000000000000</v>
+      </c>
+      <c r="J381">
+        <v>12.233333333333301</v>
+      </c>
+      <c r="K381">
+        <v>12.233333333333301</v>
+      </c>
+      <c r="L381">
+        <v>12.233333333333301</v>
+      </c>
+      <c r="M381">
+        <v>12.233333333333301</v>
+      </c>
+      <c r="Q381">
+        <v>1</v>
+      </c>
+      <c r="R381">
+        <v>1</v>
+      </c>
+      <c r="S381">
+        <v>99999</v>
+      </c>
+      <c r="T381" t="s">
+        <v>4</v>
+      </c>
+      <c r="U381">
+        <v>45</v>
+      </c>
+      <c r="V381">
+        <v>1E-3</v>
+      </c>
+      <c r="W381">
+        <v>390000000</v>
+      </c>
+      <c r="X381">
+        <v>0</v>
+      </c>
+      <c r="Y381" t="s">
+        <v>710</v>
+      </c>
+      <c r="Z381" t="s">
+        <v>710</v>
+      </c>
+      <c r="AA381">
+        <v>176000000000000</v>
+      </c>
+      <c r="AB381">
+        <v>176000000000000</v>
+      </c>
+      <c r="AC381">
+        <v>176000000000000</v>
+      </c>
+      <c r="AD381">
+        <v>1</v>
+      </c>
+      <c r="AE381">
+        <v>6.2</v>
+      </c>
+      <c r="AF381">
+        <v>8.4</v>
+      </c>
+      <c r="AG381">
+        <v>6.4</v>
+      </c>
+      <c r="AH381">
+        <v>6.6</v>
+      </c>
+      <c r="AI381">
+        <v>11.3</v>
+      </c>
+      <c r="AJ381">
+        <v>1</v>
+      </c>
+      <c r="AM381" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="382" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A382" t="s">
+        <v>688</v>
+      </c>
+      <c r="B382">
+        <v>183000000000000</v>
+      </c>
+      <c r="C382">
+        <v>183000000000000</v>
+      </c>
+      <c r="D382">
+        <v>183000000000000</v>
+      </c>
+      <c r="E382">
+        <v>183000000000000</v>
+      </c>
+      <c r="F382">
+        <v>183000000000000</v>
+      </c>
+      <c r="G382">
+        <v>183000000000000</v>
+      </c>
+      <c r="H382">
+        <v>183000000000000</v>
+      </c>
+      <c r="I382">
+        <v>183000000000000</v>
+      </c>
+      <c r="J382">
+        <v>12.633333333333301</v>
+      </c>
+      <c r="K382">
+        <v>12.633333333333301</v>
+      </c>
+      <c r="L382">
+        <v>12.633333333333301</v>
+      </c>
+      <c r="M382">
+        <v>12.633333333333301</v>
+      </c>
+      <c r="Q382">
+        <v>1</v>
+      </c>
+      <c r="R382">
+        <v>1</v>
+      </c>
+      <c r="S382">
+        <v>99999</v>
+      </c>
+      <c r="T382" t="s">
+        <v>7</v>
+      </c>
+      <c r="U382">
+        <v>45</v>
+      </c>
+      <c r="V382">
+        <v>1E-3</v>
+      </c>
+      <c r="W382">
+        <v>400000000</v>
+      </c>
+      <c r="X382">
+        <v>0</v>
+      </c>
+      <c r="Y382" t="s">
+        <v>711</v>
+      </c>
+      <c r="Z382" t="s">
+        <v>711</v>
+      </c>
+      <c r="AA382">
+        <v>183000000000000</v>
+      </c>
+      <c r="AB382">
+        <v>183000000000000</v>
+      </c>
+      <c r="AC382">
+        <v>183000000000000</v>
+      </c>
+      <c r="AD382">
+        <v>1</v>
+      </c>
+      <c r="AE382">
+        <v>6.4</v>
+      </c>
+      <c r="AF382">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AG382">
+        <v>6.6</v>
+      </c>
+      <c r="AH382">
+        <v>6.8</v>
+      </c>
+      <c r="AI382">
+        <v>11.7</v>
+      </c>
+      <c r="AJ382">
+        <v>1</v>
+      </c>
+      <c r="AM382" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="383" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A383" t="s">
+        <v>689</v>
+      </c>
+      <c r="B383">
+        <v>190000000000000</v>
+      </c>
+      <c r="C383">
+        <v>190000000000000</v>
+      </c>
+      <c r="D383">
+        <v>190000000000000</v>
+      </c>
+      <c r="E383">
+        <v>190000000000000</v>
+      </c>
+      <c r="F383">
+        <v>190000000000000</v>
+      </c>
+      <c r="G383">
+        <v>190000000000000</v>
+      </c>
+      <c r="H383">
+        <v>190000000000000</v>
+      </c>
+      <c r="I383">
+        <v>190000000000000</v>
+      </c>
+      <c r="J383">
+        <v>13.033333333333299</v>
+      </c>
+      <c r="K383">
+        <v>13.033333333333299</v>
+      </c>
+      <c r="L383">
+        <v>13.033333333333299</v>
+      </c>
+      <c r="M383">
+        <v>13.033333333333299</v>
+      </c>
+      <c r="Q383">
+        <v>1</v>
+      </c>
+      <c r="R383">
+        <v>1</v>
+      </c>
+      <c r="S383">
+        <v>99999</v>
+      </c>
+      <c r="T383" t="s">
+        <v>5</v>
+      </c>
+      <c r="U383">
+        <v>46</v>
+      </c>
+      <c r="V383">
+        <v>1E-3</v>
+      </c>
+      <c r="W383">
+        <v>410000000</v>
+      </c>
+      <c r="X383">
+        <v>0</v>
+      </c>
+      <c r="Y383" t="s">
+        <v>712</v>
+      </c>
+      <c r="Z383" t="s">
+        <v>712</v>
+      </c>
+      <c r="AA383">
+        <v>190000000000000</v>
+      </c>
+      <c r="AB383">
+        <v>190000000000000</v>
+      </c>
+      <c r="AC383">
+        <v>190000000000000</v>
+      </c>
+      <c r="AD383">
+        <v>1</v>
+      </c>
+      <c r="AE383">
+        <v>6.6</v>
+      </c>
+      <c r="AF383">
+        <v>9</v>
+      </c>
+      <c r="AG383">
+        <v>6.8</v>
+      </c>
+      <c r="AH383">
+        <v>7</v>
+      </c>
+      <c r="AI383">
+        <v>12.1</v>
+      </c>
+      <c r="AJ383">
+        <v>1</v>
+      </c>
+      <c r="AM383" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="384" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
+        <v>690</v>
+      </c>
+      <c r="B384">
+        <v>197000000000000</v>
+      </c>
+      <c r="C384">
+        <v>197000000000000</v>
+      </c>
+      <c r="D384">
+        <v>197000000000000</v>
+      </c>
+      <c r="E384">
+        <v>197000000000000</v>
+      </c>
+      <c r="F384">
+        <v>197000000000000</v>
+      </c>
+      <c r="G384">
+        <v>197000000000000</v>
+      </c>
+      <c r="H384">
+        <v>197000000000000</v>
+      </c>
+      <c r="I384">
+        <v>197000000000000</v>
+      </c>
+      <c r="J384">
+        <v>13.4333333333333</v>
+      </c>
+      <c r="K384">
+        <v>13.4333333333333</v>
+      </c>
+      <c r="L384">
+        <v>13.4333333333333</v>
+      </c>
+      <c r="M384">
+        <v>13.4333333333333</v>
+      </c>
+      <c r="Q384">
+        <v>1</v>
+      </c>
+      <c r="R384">
+        <v>1</v>
+      </c>
+      <c r="S384">
+        <v>99999</v>
+      </c>
+      <c r="T384" t="s">
+        <v>1</v>
+      </c>
+      <c r="U384">
+        <v>46</v>
+      </c>
+      <c r="V384">
+        <v>1E-3</v>
+      </c>
+      <c r="W384">
+        <v>420000000</v>
+      </c>
+      <c r="X384">
+        <v>0</v>
+      </c>
+      <c r="Y384" t="s">
+        <v>713</v>
+      </c>
+      <c r="Z384" t="s">
+        <v>713</v>
+      </c>
+      <c r="AA384">
+        <v>197000000000000</v>
+      </c>
+      <c r="AB384">
+        <v>197000000000000</v>
+      </c>
+      <c r="AC384">
+        <v>197000000000000</v>
+      </c>
+      <c r="AD384">
+        <v>1</v>
+      </c>
+      <c r="AE384">
+        <v>6.8</v>
+      </c>
+      <c r="AF384">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AG384">
+        <v>7</v>
+      </c>
+      <c r="AH384">
+        <v>7.2</v>
+      </c>
+      <c r="AI384">
+        <v>12.5</v>
+      </c>
+      <c r="AJ384">
+        <v>1</v>
+      </c>
+      <c r="AM384" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="385" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>691</v>
+      </c>
+      <c r="B385">
+        <v>204000000000000</v>
+      </c>
+      <c r="C385">
+        <v>204000000000000</v>
+      </c>
+      <c r="D385">
+        <v>204000000000000</v>
+      </c>
+      <c r="E385">
+        <v>204000000000000</v>
+      </c>
+      <c r="F385">
+        <v>204000000000000</v>
+      </c>
+      <c r="G385">
+        <v>204000000000000</v>
+      </c>
+      <c r="H385">
+        <v>204000000000000</v>
+      </c>
+      <c r="I385">
+        <v>204000000000000</v>
+      </c>
+      <c r="J385">
+        <v>13.8333333333333</v>
+      </c>
+      <c r="K385">
+        <v>13.8333333333333</v>
+      </c>
+      <c r="L385">
+        <v>13.8333333333333</v>
+      </c>
+      <c r="M385">
+        <v>13.8333333333333</v>
+      </c>
+      <c r="Q385">
+        <v>1</v>
+      </c>
+      <c r="R385">
+        <v>1</v>
+      </c>
+      <c r="S385">
+        <v>99999</v>
+      </c>
+      <c r="T385" t="s">
+        <v>3</v>
+      </c>
+      <c r="U385">
+        <v>46</v>
+      </c>
+      <c r="V385">
+        <v>1E-3</v>
+      </c>
+      <c r="W385">
+        <v>430000000</v>
+      </c>
+      <c r="X385">
+        <v>0</v>
+      </c>
+      <c r="Y385" t="s">
+        <v>714</v>
+      </c>
+      <c r="Z385" t="s">
+        <v>714</v>
+      </c>
+      <c r="AA385">
+        <v>204000000000000</v>
+      </c>
+      <c r="AB385">
+        <v>204000000000000</v>
+      </c>
+      <c r="AC385">
+        <v>204000000000000</v>
+      </c>
+      <c r="AD385">
+        <v>1</v>
+      </c>
+      <c r="AE385">
+        <v>6.9999999999999902</v>
+      </c>
+      <c r="AF385">
+        <v>9.6</v>
+      </c>
+      <c r="AG385">
+        <v>7.2</v>
+      </c>
+      <c r="AH385">
+        <v>7.3999999999999897</v>
+      </c>
+      <c r="AI385">
+        <v>12.9</v>
+      </c>
+      <c r="AJ385">
+        <v>1</v>
+      </c>
+      <c r="AM385" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="386" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>692</v>
+      </c>
+      <c r="B386">
+        <v>211000000000000</v>
+      </c>
+      <c r="C386">
+        <v>211000000000000</v>
+      </c>
+      <c r="D386">
+        <v>211000000000000</v>
+      </c>
+      <c r="E386">
+        <v>211000000000000</v>
+      </c>
+      <c r="F386">
+        <v>211000000000000</v>
+      </c>
+      <c r="G386">
+        <v>211000000000000</v>
+      </c>
+      <c r="H386">
+        <v>211000000000000</v>
+      </c>
+      <c r="I386">
+        <v>211000000000000</v>
+      </c>
+      <c r="J386">
+        <v>14.233333333333301</v>
+      </c>
+      <c r="K386">
+        <v>14.233333333333301</v>
+      </c>
+      <c r="L386">
+        <v>14.233333333333301</v>
+      </c>
+      <c r="M386">
+        <v>14.233333333333301</v>
+      </c>
+      <c r="Q386">
+        <v>1</v>
+      </c>
+      <c r="R386">
+        <v>1</v>
+      </c>
+      <c r="S386">
+        <v>99999</v>
+      </c>
+      <c r="T386" t="s">
+        <v>4</v>
+      </c>
+      <c r="U386">
+        <v>47</v>
+      </c>
+      <c r="V386">
+        <v>1E-3</v>
+      </c>
+      <c r="W386">
+        <v>440000000</v>
+      </c>
+      <c r="X386">
+        <v>0</v>
+      </c>
+      <c r="Y386" t="s">
+        <v>715</v>
+      </c>
+      <c r="Z386" t="s">
+        <v>715</v>
+      </c>
+      <c r="AA386">
+        <v>211000000000000</v>
+      </c>
+      <c r="AB386">
+        <v>211000000000000</v>
+      </c>
+      <c r="AC386">
+        <v>211000000000000</v>
+      </c>
+      <c r="AD386">
+        <v>1</v>
+      </c>
+      <c r="AE386">
+        <v>7.1999999999999904</v>
+      </c>
+      <c r="AF386">
+        <v>9.9000000000000092</v>
+      </c>
+      <c r="AG386">
+        <v>7.4</v>
+      </c>
+      <c r="AH386">
+        <v>7.5999999999999899</v>
+      </c>
+      <c r="AI386">
+        <v>13.3</v>
+      </c>
+      <c r="AJ386">
+        <v>1</v>
+      </c>
+      <c r="AM386" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="387" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
+        <v>693</v>
+      </c>
+      <c r="B387">
+        <v>218000000000000</v>
+      </c>
+      <c r="C387">
+        <v>218000000000000</v>
+      </c>
+      <c r="D387">
+        <v>218000000000000</v>
+      </c>
+      <c r="E387">
+        <v>218000000000000</v>
+      </c>
+      <c r="F387">
+        <v>218000000000000</v>
+      </c>
+      <c r="G387">
+        <v>218000000000000</v>
+      </c>
+      <c r="H387">
+        <v>218000000000000</v>
+      </c>
+      <c r="I387">
+        <v>218000000000000</v>
+      </c>
+      <c r="J387">
+        <v>14.633333333333301</v>
+      </c>
+      <c r="K387">
+        <v>14.633333333333301</v>
+      </c>
+      <c r="L387">
+        <v>14.633333333333301</v>
+      </c>
+      <c r="M387">
+        <v>14.633333333333301</v>
+      </c>
+      <c r="Q387">
+        <v>1</v>
+      </c>
+      <c r="R387">
+        <v>1</v>
+      </c>
+      <c r="S387">
+        <v>99999</v>
+      </c>
+      <c r="T387" t="s">
+        <v>3</v>
+      </c>
+      <c r="U387">
+        <v>47</v>
+      </c>
+      <c r="V387">
+        <v>1E-3</v>
+      </c>
+      <c r="W387">
+        <v>450000000</v>
+      </c>
+      <c r="X387">
+        <v>0</v>
+      </c>
+      <c r="Y387" t="s">
+        <v>716</v>
+      </c>
+      <c r="Z387" t="s">
+        <v>716</v>
+      </c>
+      <c r="AA387">
+        <v>218000000000000</v>
+      </c>
+      <c r="AB387">
+        <v>218000000000000</v>
+      </c>
+      <c r="AC387">
+        <v>218000000000000</v>
+      </c>
+      <c r="AD387">
+        <v>1</v>
+      </c>
+      <c r="AE387">
+        <v>7.3999999999999897</v>
+      </c>
+      <c r="AF387">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AG387">
+        <v>7.6</v>
+      </c>
+      <c r="AH387">
+        <v>7.7999999999999901</v>
+      </c>
+      <c r="AI387">
+        <v>13.7</v>
+      </c>
+      <c r="AJ387">
+        <v>1</v>
+      </c>
+      <c r="AM387" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="388" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>694</v>
+      </c>
+      <c r="B388">
+        <v>225000000000000</v>
+      </c>
+      <c r="C388">
+        <v>225000000000000</v>
+      </c>
+      <c r="D388">
+        <v>225000000000000</v>
+      </c>
+      <c r="E388">
+        <v>225000000000000</v>
+      </c>
+      <c r="F388">
+        <v>225000000000000</v>
+      </c>
+      <c r="G388">
+        <v>225000000000000</v>
+      </c>
+      <c r="H388">
+        <v>225000000000000</v>
+      </c>
+      <c r="I388">
+        <v>225000000000000</v>
+      </c>
+      <c r="J388">
+        <v>15.033333333333299</v>
+      </c>
+      <c r="K388">
+        <v>15.033333333333299</v>
+      </c>
+      <c r="L388">
+        <v>15.033333333333299</v>
+      </c>
+      <c r="M388">
+        <v>15.033333333333299</v>
+      </c>
+      <c r="Q388">
+        <v>1</v>
+      </c>
+      <c r="R388">
+        <v>1</v>
+      </c>
+      <c r="S388">
+        <v>99999</v>
+      </c>
+      <c r="T388" t="s">
+        <v>1</v>
+      </c>
+      <c r="U388">
+        <v>47</v>
+      </c>
+      <c r="V388">
+        <v>1E-3</v>
+      </c>
+      <c r="W388">
+        <v>460000000</v>
+      </c>
+      <c r="X388">
+        <v>0</v>
+      </c>
+      <c r="Y388" t="s">
+        <v>717</v>
+      </c>
+      <c r="Z388" t="s">
+        <v>717</v>
+      </c>
+      <c r="AA388">
+        <v>225000000000000</v>
+      </c>
+      <c r="AB388">
+        <v>225000000000000</v>
+      </c>
+      <c r="AC388">
+        <v>225000000000000</v>
+      </c>
+      <c r="AD388">
+        <v>1</v>
+      </c>
+      <c r="AE388">
+        <v>7.5999999999999899</v>
+      </c>
+      <c r="AF388">
+        <v>10.5</v>
+      </c>
+      <c r="AG388">
+        <v>7.8</v>
+      </c>
+      <c r="AH388">
+        <v>7.9999999999999902</v>
+      </c>
+      <c r="AI388">
+        <v>14.1</v>
+      </c>
+      <c r="AJ388">
+        <v>1</v>
+      </c>
+      <c r="AM388" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="389" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>695</v>
+      </c>
+      <c r="B389">
+        <v>232000000000000</v>
+      </c>
+      <c r="C389">
+        <v>232000000000000</v>
+      </c>
+      <c r="D389">
+        <v>232000000000000</v>
+      </c>
+      <c r="E389">
+        <v>232000000000000</v>
+      </c>
+      <c r="F389">
+        <v>232000000000000</v>
+      </c>
+      <c r="G389">
+        <v>232000000000000</v>
+      </c>
+      <c r="H389">
+        <v>232000000000000</v>
+      </c>
+      <c r="I389">
+        <v>232000000000000</v>
+      </c>
+      <c r="J389">
+        <v>15.4333333333333</v>
+      </c>
+      <c r="K389">
+        <v>15.4333333333333</v>
+      </c>
+      <c r="L389">
+        <v>15.4333333333333</v>
+      </c>
+      <c r="M389">
+        <v>15.4333333333333</v>
+      </c>
+      <c r="Q389">
+        <v>1</v>
+      </c>
+      <c r="R389">
+        <v>1</v>
+      </c>
+      <c r="S389">
+        <v>99999</v>
+      </c>
+      <c r="T389" t="s">
+        <v>1</v>
+      </c>
+      <c r="U389">
+        <v>48</v>
+      </c>
+      <c r="V389">
+        <v>1E-3</v>
+      </c>
+      <c r="W389">
+        <v>470000000</v>
+      </c>
+      <c r="X389">
+        <v>0</v>
+      </c>
+      <c r="Y389" t="s">
+        <v>718</v>
+      </c>
+      <c r="Z389" t="s">
+        <v>718</v>
+      </c>
+      <c r="AA389">
+        <v>232000000000000</v>
+      </c>
+      <c r="AB389">
+        <v>232000000000000</v>
+      </c>
+      <c r="AC389">
+        <v>232000000000000</v>
+      </c>
+      <c r="AD389">
+        <v>1</v>
+      </c>
+      <c r="AE389">
+        <v>7.7999999999999901</v>
+      </c>
+      <c r="AF389">
+        <v>10.8</v>
+      </c>
+      <c r="AG389">
+        <v>8</v>
+      </c>
+      <c r="AH389">
+        <v>8.1999999999999904</v>
+      </c>
+      <c r="AI389">
+        <v>14.5</v>
+      </c>
+      <c r="AJ389">
+        <v>1</v>
+      </c>
+      <c r="AM389" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="390" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>696</v>
+      </c>
+      <c r="B390">
+        <v>239000000000000</v>
+      </c>
+      <c r="C390">
+        <v>239000000000000</v>
+      </c>
+      <c r="D390">
+        <v>239000000000000</v>
+      </c>
+      <c r="E390">
+        <v>239000000000000</v>
+      </c>
+      <c r="F390">
+        <v>239000000000000</v>
+      </c>
+      <c r="G390">
+        <v>239000000000000</v>
+      </c>
+      <c r="H390">
+        <v>239000000000000</v>
+      </c>
+      <c r="I390">
+        <v>239000000000000</v>
+      </c>
+      <c r="J390">
+        <v>15.8333333333333</v>
+      </c>
+      <c r="K390">
+        <v>15.8333333333333</v>
+      </c>
+      <c r="L390">
+        <v>15.8333333333333</v>
+      </c>
+      <c r="M390">
+        <v>15.8333333333333</v>
+      </c>
+      <c r="Q390">
+        <v>1</v>
+      </c>
+      <c r="R390">
+        <v>1</v>
+      </c>
+      <c r="S390">
+        <v>99999</v>
+      </c>
+      <c r="T390" t="s">
+        <v>3</v>
+      </c>
+      <c r="U390">
+        <v>48</v>
+      </c>
+      <c r="V390">
+        <v>1E-3</v>
+      </c>
+      <c r="W390">
+        <v>480000000</v>
+      </c>
+      <c r="X390">
+        <v>0</v>
+      </c>
+      <c r="Y390" t="s">
+        <v>719</v>
+      </c>
+      <c r="Z390" t="s">
+        <v>719</v>
+      </c>
+      <c r="AA390">
+        <v>239000000000000</v>
+      </c>
+      <c r="AB390">
+        <v>239000000000000</v>
+      </c>
+      <c r="AC390">
+        <v>239000000000000</v>
+      </c>
+      <c r="AD390">
+        <v>1</v>
+      </c>
+      <c r="AE390">
+        <v>7.9999999999999902</v>
+      </c>
+      <c r="AF390">
+        <v>11.1</v>
+      </c>
+      <c r="AG390">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AH390">
+        <v>8.3999999999999897</v>
+      </c>
+      <c r="AI390">
+        <v>14.9</v>
+      </c>
+      <c r="AJ390">
+        <v>1</v>
+      </c>
+      <c r="AM390" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="391" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>697</v>
+      </c>
+      <c r="B391">
+        <v>246000000000000</v>
+      </c>
+      <c r="C391">
+        <v>246000000000000</v>
+      </c>
+      <c r="D391">
+        <v>246000000000000</v>
+      </c>
+      <c r="E391">
+        <v>246000000000000</v>
+      </c>
+      <c r="F391">
+        <v>246000000000000</v>
+      </c>
+      <c r="G391">
+        <v>246000000000000</v>
+      </c>
+      <c r="H391">
+        <v>246000000000000</v>
+      </c>
+      <c r="I391">
+        <v>246000000000000</v>
+      </c>
+      <c r="J391">
+        <v>16.233333333333299</v>
+      </c>
+      <c r="K391">
+        <v>16.233333333333299</v>
+      </c>
+      <c r="L391">
+        <v>16.233333333333299</v>
+      </c>
+      <c r="M391">
+        <v>16.233333333333299</v>
+      </c>
+      <c r="Q391">
+        <v>1</v>
+      </c>
+      <c r="R391">
+        <v>1</v>
+      </c>
+      <c r="S391">
+        <v>99999</v>
+      </c>
+      <c r="T391" t="s">
+        <v>7</v>
+      </c>
+      <c r="U391">
+        <v>49</v>
+      </c>
+      <c r="V391">
+        <v>1E-3</v>
+      </c>
+      <c r="W391">
+        <v>490000000</v>
+      </c>
+      <c r="X391">
+        <v>0</v>
+      </c>
+      <c r="Y391" t="s">
+        <v>720</v>
+      </c>
+      <c r="Z391" t="s">
+        <v>720</v>
+      </c>
+      <c r="AA391">
+        <v>246000000000000</v>
+      </c>
+      <c r="AB391">
+        <v>246000000000000</v>
+      </c>
+      <c r="AC391">
+        <v>246000000000000</v>
+      </c>
+      <c r="AD391">
+        <v>1</v>
+      </c>
+      <c r="AE391">
+        <v>8.1999999999999904</v>
+      </c>
+      <c r="AF391">
+        <v>11.4</v>
+      </c>
+      <c r="AG391">
+        <v>8.4</v>
+      </c>
+      <c r="AH391">
+        <v>8.5999999999999908</v>
+      </c>
+      <c r="AI391">
+        <v>15.3</v>
+      </c>
+      <c r="AJ391">
+        <v>1</v>
+      </c>
+      <c r="AM391" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="392" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>698</v>
+      </c>
+      <c r="B392">
+        <v>253000000000000</v>
+      </c>
+      <c r="C392">
+        <v>253000000000000</v>
+      </c>
+      <c r="D392">
+        <v>253000000000000</v>
+      </c>
+      <c r="E392">
+        <v>253000000000000</v>
+      </c>
+      <c r="F392">
+        <v>253000000000000</v>
+      </c>
+      <c r="G392">
+        <v>253000000000000</v>
+      </c>
+      <c r="H392">
+        <v>253000000000000</v>
+      </c>
+      <c r="I392">
+        <v>253000000000000</v>
+      </c>
+      <c r="J392">
+        <v>16.633333333333301</v>
+      </c>
+      <c r="K392">
+        <v>16.633333333333301</v>
+      </c>
+      <c r="L392">
+        <v>16.633333333333301</v>
+      </c>
+      <c r="M392">
+        <v>16.633333333333301</v>
+      </c>
+      <c r="Q392">
+        <v>1</v>
+      </c>
+      <c r="R392">
+        <v>1</v>
+      </c>
+      <c r="S392">
+        <v>99999</v>
+      </c>
+      <c r="T392" t="s">
+        <v>5</v>
+      </c>
+      <c r="U392">
+        <v>49</v>
+      </c>
+      <c r="V392">
+        <v>1E-3</v>
+      </c>
+      <c r="W392">
+        <v>500000000</v>
+      </c>
+      <c r="X392">
+        <v>0</v>
+      </c>
+      <c r="Y392" t="s">
+        <v>721</v>
+      </c>
+      <c r="Z392" t="s">
+        <v>721</v>
+      </c>
+      <c r="AA392">
+        <v>253000000000000</v>
+      </c>
+      <c r="AB392">
+        <v>253000000000000</v>
+      </c>
+      <c r="AC392">
+        <v>253000000000000</v>
+      </c>
+      <c r="AD392">
+        <v>1</v>
+      </c>
+      <c r="AE392">
+        <v>8.3999999999999897</v>
+      </c>
+      <c r="AF392">
+        <v>11.7</v>
+      </c>
+      <c r="AG392">
+        <v>8.6</v>
+      </c>
+      <c r="AH392">
+        <v>8.7999999999999901</v>
+      </c>
+      <c r="AI392">
+        <v>15.7</v>
+      </c>
+      <c r="AJ392">
+        <v>1</v>
+      </c>
+      <c r="AM392" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="393" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
+        <v>699</v>
+      </c>
+      <c r="B393">
+        <v>260000000000000</v>
+      </c>
+      <c r="C393">
+        <v>260000000000000</v>
+      </c>
+      <c r="D393">
+        <v>260000000000000</v>
+      </c>
+      <c r="E393">
+        <v>260000000000000</v>
+      </c>
+      <c r="F393">
+        <v>260000000000000</v>
+      </c>
+      <c r="G393">
+        <v>260000000000000</v>
+      </c>
+      <c r="H393">
+        <v>260000000000000</v>
+      </c>
+      <c r="I393">
+        <v>260000000000000</v>
+      </c>
+      <c r="J393">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="K393">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="L393">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="M393">
+        <v>17.033333333333299</v>
+      </c>
+      <c r="Q393">
+        <v>1</v>
+      </c>
+      <c r="R393">
+        <v>1</v>
+      </c>
+      <c r="S393">
+        <v>99999</v>
+      </c>
+      <c r="T393" t="s">
+        <v>4</v>
+      </c>
+      <c r="U393">
+        <v>50</v>
+      </c>
+      <c r="V393">
+        <v>1E-3</v>
+      </c>
+      <c r="W393">
+        <v>510000000</v>
+      </c>
+      <c r="X393">
+        <v>0</v>
+      </c>
+      <c r="Y393" t="s">
+        <v>722</v>
+      </c>
+      <c r="Z393" t="s">
+        <v>722</v>
+      </c>
+      <c r="AA393">
+        <v>253000000000000</v>
+      </c>
+      <c r="AB393">
+        <v>253000000000000</v>
+      </c>
+      <c r="AC393">
+        <v>253000000000000</v>
+      </c>
+      <c r="AD393">
+        <v>1</v>
+      </c>
+      <c r="AE393">
+        <v>8.3999999999999897</v>
+      </c>
+      <c r="AF393">
+        <v>11.7</v>
+      </c>
+      <c r="AG393">
+        <v>8.6</v>
+      </c>
+      <c r="AH393">
+        <v>8.7999999999999901</v>
+      </c>
+      <c r="AI393">
+        <v>15.7</v>
+      </c>
+      <c r="AJ393">
+        <v>1</v>
+      </c>
+      <c r="AM393" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="394" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>700</v>
+      </c>
+      <c r="B394">
+        <v>267000000000000</v>
+      </c>
+      <c r="C394">
+        <v>267000000000000</v>
+      </c>
+      <c r="D394">
+        <v>267000000000000</v>
+      </c>
+      <c r="E394">
+        <v>267000000000000</v>
+      </c>
+      <c r="F394">
+        <v>267000000000000</v>
+      </c>
+      <c r="G394">
+        <v>267000000000000</v>
+      </c>
+      <c r="H394">
+        <v>267000000000000</v>
+      </c>
+      <c r="I394">
+        <v>267000000000000</v>
+      </c>
+      <c r="J394">
+        <v>17.433333333333302</v>
+      </c>
+      <c r="K394">
+        <v>17.433333333333302</v>
+      </c>
+      <c r="L394">
+        <v>17.433333333333302</v>
+      </c>
+      <c r="M394">
+        <v>17.433333333333302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of tweaks and fixes for the release of 1.1.10
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA9B339-6CBA-7F40-9CF4-CF7A4C02BBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D288035-3649-3946-9B10-B6C0950FC8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="724">
   <si>
     <t>name</t>
   </si>
@@ -2200,6 +2200,9 @@
   </si>
   <si>
     <t>308476637656600-312476476445500</t>
+  </si>
+  <si>
+    <t>320476637656600-325476476445500</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
-      <selection activeCell="T393" sqref="T393"/>
+    <sheetView tabSelected="1" topLeftCell="O360" workbookViewId="0">
+      <selection activeCell="Z394" sqref="Z394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43896,6 +43899,69 @@
       <c r="M394">
         <v>17.433333333333302</v>
       </c>
+      <c r="Q394">
+        <v>1</v>
+      </c>
+      <c r="R394">
+        <v>1</v>
+      </c>
+      <c r="S394">
+        <v>99999</v>
+      </c>
+      <c r="T394" t="s">
+        <v>4</v>
+      </c>
+      <c r="U394">
+        <v>55</v>
+      </c>
+      <c r="V394">
+        <v>1E-3</v>
+      </c>
+      <c r="W394">
+        <v>520000000</v>
+      </c>
+      <c r="X394">
+        <v>0</v>
+      </c>
+      <c r="Y394" t="s">
+        <v>723</v>
+      </c>
+      <c r="Z394" t="s">
+        <v>723</v>
+      </c>
+      <c r="AA394">
+        <v>253000000000000</v>
+      </c>
+      <c r="AB394">
+        <v>253000000000000</v>
+      </c>
+      <c r="AC394">
+        <v>253000000000000</v>
+      </c>
+      <c r="AD394">
+        <v>1</v>
+      </c>
+      <c r="AE394">
+        <v>8.3999999999999897</v>
+      </c>
+      <c r="AF394">
+        <v>11.7</v>
+      </c>
+      <c r="AG394">
+        <v>8.6</v>
+      </c>
+      <c r="AH394">
+        <v>8.7999999999999901</v>
+      </c>
+      <c r="AI394">
+        <v>15.7</v>
+      </c>
+      <c r="AJ394">
+        <v>1</v>
+      </c>
+      <c r="AM394" t="s">
+        <v>651</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Updated monsters - fixed attacker timer
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="741">
   <si>
     <t>name</t>
   </si>
@@ -2226,6 +2226,18 @@
   </si>
   <si>
     <t>640476637656600-685476476445500</t>
+  </si>
+  <si>
+    <t>Haunted Aboration</t>
+  </si>
+  <si>
+    <t>25000000000000-30000000000000</t>
+  </si>
+  <si>
+    <t>8500000000-12600000000</t>
+  </si>
+  <si>
+    <t>Magicians Enchanted Copper Coin</t>
   </si>
 </sst>
 </file>
@@ -2561,7 +2573,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AM401"/>
+  <dimension ref="A1:AM402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -2605,7 +2617,7 @@
     <col min="34" max="34" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="35" max="35" width="26" bestFit="true" customWidth="true" style="0"/>
     <col min="36" max="36" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="37" max="37" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="37" max="37" width="37" bestFit="true" customWidth="true" style="0"/>
     <col min="38" max="38" width="26" bestFit="true" customWidth="true" style="0"/>
     <col min="39" max="39" width="15" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -44717,6 +44729,125 @@
       </c>
       <c r="AM401" t="s">
         <v>652</v>
+      </c>
+    </row>
+    <row r="402" spans="1:39">
+      <c r="A402" t="s">
+        <v>737</v>
+      </c>
+      <c r="B402">
+        <v>2000000000000</v>
+      </c>
+      <c r="C402">
+        <v>2000000000000</v>
+      </c>
+      <c r="D402">
+        <v>2000000000000</v>
+      </c>
+      <c r="E402">
+        <v>2000000000000</v>
+      </c>
+      <c r="F402">
+        <v>2000000000000</v>
+      </c>
+      <c r="G402">
+        <v>2000000000000</v>
+      </c>
+      <c r="H402">
+        <v>2000000000000</v>
+      </c>
+      <c r="I402">
+        <v>2000000000000</v>
+      </c>
+      <c r="J402">
+        <v>2</v>
+      </c>
+      <c r="K402">
+        <v>2</v>
+      </c>
+      <c r="L402">
+        <v>2</v>
+      </c>
+      <c r="M402">
+        <v>2</v>
+      </c>
+      <c r="N402">
+        <v>1</v>
+      </c>
+      <c r="O402">
+        <v>2000000000</v>
+      </c>
+      <c r="P402">
+        <v>10000</v>
+      </c>
+      <c r="Q402">
+        <v>1</v>
+      </c>
+      <c r="R402">
+        <v>1</v>
+      </c>
+      <c r="S402">
+        <v>9999</v>
+      </c>
+      <c r="T402" t="s">
+        <v>3</v>
+      </c>
+      <c r="U402">
+        <v>100</v>
+      </c>
+      <c r="V402">
+        <v>0.01</v>
+      </c>
+      <c r="W402">
+        <v>2000000000</v>
+      </c>
+      <c r="X402">
+        <v>400</v>
+      </c>
+      <c r="Y402" t="s">
+        <v>738</v>
+      </c>
+      <c r="Z402" t="s">
+        <v>739</v>
+      </c>
+      <c r="AA402">
+        <v>1000000000</v>
+      </c>
+      <c r="AB402">
+        <v>1000000000</v>
+      </c>
+      <c r="AC402">
+        <v>2000000000000</v>
+      </c>
+      <c r="AD402">
+        <v>1.6</v>
+      </c>
+      <c r="AE402">
+        <v>2</v>
+      </c>
+      <c r="AF402">
+        <v>2</v>
+      </c>
+      <c r="AG402">
+        <v>2</v>
+      </c>
+      <c r="AH402">
+        <v>1.6</v>
+      </c>
+      <c r="AI402">
+        <v>1.6</v>
+      </c>
+      <c r="AJ402">
+        <v>1</v>
+      </c>
+      <c r="AK402" t="s">
+        <v>740</v>
+      </c>
+      <c r="AL402">
+        <v>1</v>
+      </c>
+      <c r="AM402" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a command to remove all artifacts.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279E0D68-63B5-1E44-82BE-2DFE33ECF704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58716D2C-A29A-DB44-B707-A01CD16E5F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K372" workbookViewId="0">
-      <selection activeCell="AL30" sqref="AL30"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AO12" sqref="AO12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3119,12 +3119,8 @@
       <c r="AN12" s="1">
         <v>1</v>
       </c>
-      <c r="AO12" s="1">
-        <v>185</v>
-      </c>
-      <c r="AP12" s="1">
-        <v>0.15</v>
-      </c>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
       <c r="AQ12" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added a way to delete all artifacts - fixed it up.
- Updated Imports.
- We can now click on items in the set/equipped tab to view expanded
  details.
- We can view Affix info and holy info.

- What we are missing is holy stack break down.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58716D2C-A29A-DB44-B707-A01CD16E5F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F698E9-26B3-D946-8A42-7F32683E7379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AO12" sqref="AO12"/>
+    <sheetView tabSelected="1" topLeftCell="AG119" workbookViewId="0">
+      <selection activeCell="AP146" sqref="AP146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18800,12 +18800,8 @@
       <c r="AN146" s="1">
         <v>1</v>
       </c>
-      <c r="AO146" s="1">
-        <v>185</v>
-      </c>
-      <c r="AP146" s="1">
-        <v>0.2</v>
-      </c>
+      <c r="AO146" s="1"/>
+      <c r="AP146" s="1"/>
       <c r="AQ146" s="1">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Minor changes and fixes.
Ready to implement conjuring.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E94860-14E1-0F4D-BB81-0D39E3E4F1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E93AC88-C380-E846-AC95-885CE0CC08CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2048,11 +2048,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2359,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="V333" sqref="V333:V375"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W341" sqref="W341:W375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2600,7 +2601,7 @@
       <c r="V2">
         <v>2</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="4">
         <v>0.01</v>
       </c>
       <c r="X2">
@@ -2704,8 +2705,8 @@
       <c r="V3">
         <v>3</v>
       </c>
-      <c r="W3">
-        <v>0.02</v>
+      <c r="W3" s="4">
+        <v>1.8448275862068958E-2</v>
       </c>
       <c r="X3">
         <v>8</v>
@@ -2811,8 +2812,8 @@
       <c r="V4">
         <v>3</v>
       </c>
-      <c r="W4">
-        <v>0.03</v>
+      <c r="W4" s="4">
+        <v>2.6896551724137921E-2</v>
       </c>
       <c r="X4">
         <v>12</v>
@@ -2912,8 +2913,8 @@
       <c r="V5">
         <v>4</v>
       </c>
-      <c r="W5">
-        <v>0.03</v>
+      <c r="W5" s="4">
+        <v>3.5344827586206877E-2</v>
       </c>
       <c r="X5">
         <v>20</v>
@@ -3013,8 +3014,8 @@
       <c r="V6">
         <v>5</v>
       </c>
-      <c r="W6">
-        <v>0.03</v>
+      <c r="W6" s="4">
+        <v>4.379310344827584E-2</v>
       </c>
       <c r="X6">
         <v>60</v>
@@ -3120,8 +3121,8 @@
       <c r="V7">
         <v>6</v>
       </c>
-      <c r="W7">
-        <v>0.05</v>
+      <c r="W7" s="4">
+        <v>5.2241379310344803E-2</v>
       </c>
       <c r="X7">
         <v>150</v>
@@ -3227,8 +3228,8 @@
       <c r="V8">
         <v>7</v>
       </c>
-      <c r="W8">
-        <v>0.1</v>
+      <c r="W8" s="4">
+        <v>6.0689655172413759E-2</v>
       </c>
       <c r="X8">
         <v>300</v>
@@ -3334,8 +3335,8 @@
       <c r="V9">
         <v>7</v>
       </c>
-      <c r="W9">
-        <v>0.05</v>
+      <c r="W9" s="4">
+        <v>6.9137931034482708E-2</v>
       </c>
       <c r="X9">
         <v>400</v>
@@ -3435,8 +3436,8 @@
       <c r="V10">
         <v>8</v>
       </c>
-      <c r="W10">
-        <v>0.09</v>
+      <c r="W10" s="4">
+        <v>7.7586206896551671E-2</v>
       </c>
       <c r="X10">
         <v>800</v>
@@ -3542,8 +3543,8 @@
       <c r="V11">
         <v>9</v>
       </c>
-      <c r="W11">
-        <v>0.05</v>
+      <c r="W11" s="4">
+        <v>8.6034482758620634E-2</v>
       </c>
       <c r="X11">
         <v>1000</v>
@@ -3649,8 +3650,8 @@
       <c r="V12">
         <v>10</v>
       </c>
-      <c r="W12">
-        <v>0.05</v>
+      <c r="W12" s="4">
+        <v>9.4482758620689597E-2</v>
       </c>
       <c r="X12">
         <v>1200</v>
@@ -3750,8 +3751,8 @@
       <c r="V13">
         <v>10</v>
       </c>
-      <c r="W13">
-        <v>0.1</v>
+      <c r="W13" s="4">
+        <v>0.10293103448275855</v>
       </c>
       <c r="X13">
         <v>1800</v>
@@ -3851,8 +3852,8 @@
       <c r="V14">
         <v>11</v>
       </c>
-      <c r="W14">
-        <v>0.01</v>
+      <c r="W14" s="4">
+        <v>0.11137931034482751</v>
       </c>
       <c r="X14">
         <v>2500</v>
@@ -3952,8 +3953,8 @@
       <c r="V15">
         <v>12</v>
       </c>
-      <c r="W15">
-        <v>0.01</v>
+      <c r="W15" s="4">
+        <v>0.11982758620689647</v>
       </c>
       <c r="X15">
         <v>3000</v>
@@ -4059,8 +4060,8 @@
       <c r="V16">
         <v>13</v>
       </c>
-      <c r="W16">
-        <v>0.04</v>
+      <c r="W16" s="4">
+        <v>0.12827586206896543</v>
       </c>
       <c r="X16">
         <v>6000</v>
@@ -4166,8 +4167,8 @@
       <c r="V17">
         <v>13</v>
       </c>
-      <c r="W17">
-        <v>0.05</v>
+      <c r="W17" s="4">
+        <v>0.13672413793103441</v>
       </c>
       <c r="X17">
         <v>9000</v>
@@ -4267,8 +4268,8 @@
       <c r="V18">
         <v>14</v>
       </c>
-      <c r="W18">
-        <v>0.05</v>
+      <c r="W18" s="4">
+        <v>0.14517241379310336</v>
       </c>
       <c r="X18">
         <v>9793</v>
@@ -4368,8 +4369,8 @@
       <c r="V19">
         <v>15</v>
       </c>
-      <c r="W19">
-        <v>0.02</v>
+      <c r="W19" s="4">
+        <v>0.15362068965517231</v>
       </c>
       <c r="X19">
         <v>11425</v>
@@ -4469,8 +4470,8 @@
       <c r="V20">
         <v>16</v>
       </c>
-      <c r="W20">
-        <v>0.04</v>
+      <c r="W20" s="4">
+        <v>0.16206896551724129</v>
       </c>
       <c r="X20">
         <v>13056</v>
@@ -4570,8 +4571,8 @@
       <c r="V21">
         <v>16</v>
       </c>
-      <c r="W21">
-        <v>0.08</v>
+      <c r="W21" s="4">
+        <v>0.17051724137931024</v>
       </c>
       <c r="X21">
         <v>14688</v>
@@ -4671,8 +4672,8 @@
       <c r="V22">
         <v>17</v>
       </c>
-      <c r="W22">
-        <v>0.01</v>
+      <c r="W22" s="4">
+        <v>0.17896551724137921</v>
       </c>
       <c r="X22">
         <v>16319</v>
@@ -4778,8 +4779,8 @@
       <c r="V23">
         <v>18</v>
       </c>
-      <c r="W23">
-        <v>0.04</v>
+      <c r="W23" s="4">
+        <v>0.18741379310344816</v>
       </c>
       <c r="X23">
         <v>17950</v>
@@ -4879,8 +4880,8 @@
       <c r="V24">
         <v>19</v>
       </c>
-      <c r="W24">
-        <v>0.02</v>
+      <c r="W24" s="4">
+        <v>0.19586206896551711</v>
       </c>
       <c r="X24">
         <v>19582</v>
@@ -4980,8 +4981,8 @@
       <c r="V25">
         <v>19</v>
       </c>
-      <c r="W25">
-        <v>0.05</v>
+      <c r="W25" s="4">
+        <v>0.20431034482758609</v>
       </c>
       <c r="X25">
         <v>21213</v>
@@ -5081,8 +5082,8 @@
       <c r="V26">
         <v>20</v>
       </c>
-      <c r="W26">
-        <v>0.01</v>
+      <c r="W26" s="4">
+        <v>0.21275862068965504</v>
       </c>
       <c r="X26">
         <v>22845</v>
@@ -5182,8 +5183,8 @@
       <c r="V27">
         <v>21</v>
       </c>
-      <c r="W27">
-        <v>0.02</v>
+      <c r="W27" s="4">
+        <v>0.22120689655172399</v>
       </c>
       <c r="X27">
         <v>24476</v>
@@ -5289,8 +5290,8 @@
       <c r="V28">
         <v>22</v>
       </c>
-      <c r="W28">
-        <v>0.04</v>
+      <c r="W28" s="4">
+        <v>0.22965517241379296</v>
       </c>
       <c r="X28">
         <v>26108</v>
@@ -5390,8 +5391,8 @@
       <c r="V29">
         <v>22</v>
       </c>
-      <c r="W29">
-        <v>0.01</v>
+      <c r="W29" s="4">
+        <v>0.23810344827586191</v>
       </c>
       <c r="X29">
         <v>27739</v>
@@ -5497,8 +5498,8 @@
       <c r="V30">
         <v>23</v>
       </c>
-      <c r="W30">
-        <v>0.01</v>
+      <c r="W30" s="4">
+        <v>0.24655172413793086</v>
       </c>
       <c r="X30">
         <v>29370</v>
@@ -5601,8 +5602,8 @@
       <c r="V31">
         <v>24</v>
       </c>
-      <c r="W31">
-        <v>0.01</v>
+      <c r="W31" s="4">
+        <v>0.25499999999999984</v>
       </c>
       <c r="X31">
         <v>31002</v>
@@ -5705,8 +5706,8 @@
       <c r="V32">
         <v>25</v>
       </c>
-      <c r="W32">
-        <v>0.04</v>
+      <c r="W32" s="4">
+        <v>0.26344827586206881</v>
       </c>
       <c r="X32">
         <v>32633</v>
@@ -5809,8 +5810,8 @@
       <c r="V33">
         <v>25</v>
       </c>
-      <c r="W33">
-        <v>0.05</v>
+      <c r="W33" s="4">
+        <v>0.27189655172413774</v>
       </c>
       <c r="X33">
         <v>34265</v>
@@ -5913,8 +5914,8 @@
       <c r="V34">
         <v>26</v>
       </c>
-      <c r="W34">
-        <v>0.05</v>
+      <c r="W34" s="4">
+        <v>0.28034482758620671</v>
       </c>
       <c r="X34">
         <v>35896</v>
@@ -6017,8 +6018,8 @@
       <c r="V35">
         <v>27</v>
       </c>
-      <c r="W35">
-        <v>0.02</v>
+      <c r="W35" s="4">
+        <v>0.28879310344827569</v>
       </c>
       <c r="X35">
         <v>37528</v>
@@ -6121,8 +6122,8 @@
       <c r="V36">
         <v>28</v>
       </c>
-      <c r="W36">
-        <v>0.04</v>
+      <c r="W36" s="4">
+        <v>0.29724137931034461</v>
       </c>
       <c r="X36">
         <v>39159</v>
@@ -6225,8 +6226,8 @@
       <c r="V37">
         <v>28</v>
       </c>
-      <c r="W37">
-        <v>0.08</v>
+      <c r="W37" s="4">
+        <v>0.30568965517241359</v>
       </c>
       <c r="X37">
         <v>40790</v>
@@ -6329,8 +6330,8 @@
       <c r="V38">
         <v>29</v>
       </c>
-      <c r="W38">
-        <v>0.01</v>
+      <c r="W38" s="4">
+        <v>0.31413793103448256</v>
       </c>
       <c r="X38">
         <v>42422</v>
@@ -6433,8 +6434,8 @@
       <c r="V39">
         <v>30</v>
       </c>
-      <c r="W39">
-        <v>0.04</v>
+      <c r="W39" s="4">
+        <v>0.32258620689655149</v>
       </c>
       <c r="X39">
         <v>44053</v>
@@ -6537,8 +6538,8 @@
       <c r="V40">
         <v>31</v>
       </c>
-      <c r="W40">
-        <v>0.02</v>
+      <c r="W40" s="4">
+        <v>0.33103448275862046</v>
       </c>
       <c r="X40">
         <v>45685</v>
@@ -6641,8 +6642,8 @@
       <c r="V41">
         <v>31</v>
       </c>
-      <c r="W41">
-        <v>0.05</v>
+      <c r="W41" s="4">
+        <v>0.33948275862068944</v>
       </c>
       <c r="X41">
         <v>47316</v>
@@ -6745,8 +6746,8 @@
       <c r="V42">
         <v>32</v>
       </c>
-      <c r="W42">
-        <v>0.01</v>
+      <c r="W42" s="4">
+        <v>0.34793103448275842</v>
       </c>
       <c r="X42">
         <v>48948</v>
@@ -6849,8 +6850,8 @@
       <c r="V43">
         <v>33</v>
       </c>
-      <c r="W43">
-        <v>0.02</v>
+      <c r="W43" s="4">
+        <v>0.35637931034482734</v>
       </c>
       <c r="X43">
         <v>50579</v>
@@ -6953,8 +6954,8 @@
       <c r="V44">
         <v>34</v>
       </c>
-      <c r="W44">
-        <v>0.04</v>
+      <c r="W44" s="4">
+        <v>0.36482758620689631</v>
       </c>
       <c r="X44">
         <v>52210</v>
@@ -7057,8 +7058,8 @@
       <c r="V45">
         <v>34</v>
       </c>
-      <c r="W45">
-        <v>0.01</v>
+      <c r="W45" s="4">
+        <v>0.37327586206896529</v>
       </c>
       <c r="X45">
         <v>53842</v>
@@ -7161,8 +7162,8 @@
       <c r="V46">
         <v>35</v>
       </c>
-      <c r="W46">
-        <v>0.01</v>
+      <c r="W46" s="4">
+        <v>0.38172413793103421</v>
       </c>
       <c r="X46">
         <v>55473</v>
@@ -7265,8 +7266,8 @@
       <c r="V47">
         <v>36</v>
       </c>
-      <c r="W47">
-        <v>0.01</v>
+      <c r="W47" s="4">
+        <v>0.39017241379310319</v>
       </c>
       <c r="X47">
         <v>57105</v>
@@ -7369,8 +7370,8 @@
       <c r="V48">
         <v>37</v>
       </c>
-      <c r="W48">
-        <v>0.04</v>
+      <c r="W48" s="4">
+        <v>0.39862068965517217</v>
       </c>
       <c r="X48">
         <v>58736</v>
@@ -7473,8 +7474,8 @@
       <c r="V49">
         <v>37</v>
       </c>
-      <c r="W49">
-        <v>0.05</v>
+      <c r="W49" s="4">
+        <v>0.40706896551724109</v>
       </c>
       <c r="X49">
         <v>60368</v>
@@ -7577,8 +7578,8 @@
       <c r="V50">
         <v>38</v>
       </c>
-      <c r="W50">
-        <v>0.05</v>
+      <c r="W50" s="4">
+        <v>0.41551724137931006</v>
       </c>
       <c r="X50">
         <v>61999</v>
@@ -7681,8 +7682,8 @@
       <c r="V51">
         <v>39</v>
       </c>
-      <c r="W51">
-        <v>0.02</v>
+      <c r="W51" s="4">
+        <v>0.42396551724137904</v>
       </c>
       <c r="X51">
         <v>63630</v>
@@ -7785,8 +7786,8 @@
       <c r="V52">
         <v>40</v>
       </c>
-      <c r="W52">
-        <v>0.04</v>
+      <c r="W52" s="4">
+        <v>0.43241379310344796</v>
       </c>
       <c r="X52">
         <v>65262</v>
@@ -7889,8 +7890,8 @@
       <c r="V53">
         <v>40</v>
       </c>
-      <c r="W53">
-        <v>0.01</v>
+      <c r="W53" s="4">
+        <v>0.44086206896551694</v>
       </c>
       <c r="X53">
         <v>66893</v>
@@ -7993,8 +7994,8 @@
       <c r="V54">
         <v>41</v>
       </c>
-      <c r="W54">
-        <v>0.04</v>
+      <c r="W54" s="4">
+        <v>0.44931034482758592</v>
       </c>
       <c r="X54">
         <v>68525</v>
@@ -8097,8 +8098,8 @@
       <c r="V55">
         <v>42</v>
       </c>
-      <c r="W55">
-        <v>0.02</v>
+      <c r="W55" s="4">
+        <v>0.45775862068965484</v>
       </c>
       <c r="X55">
         <v>70156</v>
@@ -8201,8 +8202,8 @@
       <c r="V56">
         <v>43</v>
       </c>
-      <c r="W56">
-        <v>0.05</v>
+      <c r="W56" s="4">
+        <v>0.46620689655172382</v>
       </c>
       <c r="X56">
         <v>71788</v>
@@ -8305,8 +8306,8 @@
       <c r="V57">
         <v>43</v>
       </c>
-      <c r="W57">
-        <v>0.01</v>
+      <c r="W57" s="4">
+        <v>0.47465517241379279</v>
       </c>
       <c r="X57">
         <v>73419</v>
@@ -8409,8 +8410,8 @@
       <c r="V58">
         <v>44</v>
       </c>
-      <c r="W58">
-        <v>0.02</v>
+      <c r="W58" s="4">
+        <v>0.48310344827586171</v>
       </c>
       <c r="X58">
         <v>75050</v>
@@ -8513,8 +8514,8 @@
       <c r="V59">
         <v>45</v>
       </c>
-      <c r="W59">
-        <v>0.04</v>
+      <c r="W59" s="4">
+        <v>0.49155172413793069</v>
       </c>
       <c r="X59">
         <v>76682</v>
@@ -8617,8 +8618,8 @@
       <c r="V60">
         <v>46</v>
       </c>
-      <c r="W60">
-        <v>0.01</v>
+      <c r="W60" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X60">
         <v>78313</v>
@@ -9345,7 +9346,7 @@
       <c r="V67">
         <v>2</v>
       </c>
-      <c r="W67">
+      <c r="W67" s="4">
         <v>0.01</v>
       </c>
       <c r="X67">
@@ -9440,8 +9441,8 @@
       <c r="V68">
         <v>3</v>
       </c>
-      <c r="W68">
-        <v>0.02</v>
+      <c r="W68" s="4">
+        <v>1.8448275862068958E-2</v>
       </c>
       <c r="X68">
         <v>25</v>
@@ -9541,8 +9542,8 @@
       <c r="V69">
         <v>3</v>
       </c>
-      <c r="W69">
-        <v>0.03</v>
+      <c r="W69" s="4">
+        <v>2.6896551724137921E-2</v>
       </c>
       <c r="X69">
         <v>50</v>
@@ -9642,8 +9643,8 @@
       <c r="V70">
         <v>4</v>
       </c>
-      <c r="W70">
-        <v>0.03</v>
+      <c r="W70" s="4">
+        <v>3.5344827586206877E-2</v>
       </c>
       <c r="X70">
         <v>30</v>
@@ -9743,8 +9744,8 @@
       <c r="V71">
         <v>5</v>
       </c>
-      <c r="W71">
-        <v>0.03</v>
+      <c r="W71" s="4">
+        <v>4.379310344827584E-2</v>
       </c>
       <c r="X71">
         <v>40</v>
@@ -9844,8 +9845,8 @@
       <c r="V72">
         <v>5</v>
       </c>
-      <c r="W72">
-        <v>0.05</v>
+      <c r="W72" s="4">
+        <v>5.2241379310344803E-2</v>
       </c>
       <c r="X72">
         <v>75</v>
@@ -9945,8 +9946,8 @@
       <c r="V73">
         <v>6</v>
       </c>
-      <c r="W73">
-        <v>0.1</v>
+      <c r="W73" s="4">
+        <v>6.0689655172413759E-2</v>
       </c>
       <c r="X73">
         <v>80</v>
@@ -10046,8 +10047,8 @@
       <c r="V74">
         <v>7</v>
       </c>
-      <c r="W74">
-        <v>0.05</v>
+      <c r="W74" s="4">
+        <v>6.9137931034482708E-2</v>
       </c>
       <c r="X74">
         <v>95</v>
@@ -10147,8 +10148,8 @@
       <c r="V75">
         <v>7</v>
       </c>
-      <c r="W75">
-        <v>0.09</v>
+      <c r="W75" s="4">
+        <v>7.7586206896551671E-2</v>
       </c>
       <c r="X75">
         <v>100</v>
@@ -10248,8 +10249,8 @@
       <c r="V76">
         <v>8</v>
       </c>
-      <c r="W76">
-        <v>0.05</v>
+      <c r="W76" s="4">
+        <v>8.6034482758620634E-2</v>
       </c>
       <c r="X76">
         <v>250</v>
@@ -10349,8 +10350,8 @@
       <c r="V77">
         <v>9</v>
       </c>
-      <c r="W77">
-        <v>0.05</v>
+      <c r="W77" s="4">
+        <v>9.4482758620689597E-2</v>
       </c>
       <c r="X77">
         <v>350</v>
@@ -10450,8 +10451,8 @@
       <c r="V78">
         <v>9</v>
       </c>
-      <c r="W78">
-        <v>0.1</v>
+      <c r="W78" s="4">
+        <v>0.10293103448275855</v>
       </c>
       <c r="X78">
         <v>500</v>
@@ -10551,8 +10552,8 @@
       <c r="V79">
         <v>10</v>
       </c>
-      <c r="W79">
-        <v>0.01</v>
+      <c r="W79" s="4">
+        <v>0.11137931034482751</v>
       </c>
       <c r="X79">
         <v>750</v>
@@ -10652,8 +10653,8 @@
       <c r="V80">
         <v>11</v>
       </c>
-      <c r="W80">
-        <v>0.01</v>
+      <c r="W80" s="4">
+        <v>0.11982758620689647</v>
       </c>
       <c r="X80">
         <v>825</v>
@@ -10753,8 +10754,8 @@
       <c r="V81">
         <v>11</v>
       </c>
-      <c r="W81">
-        <v>0.05</v>
+      <c r="W81" s="4">
+        <v>0.12827586206896543</v>
       </c>
       <c r="X81">
         <v>1000</v>
@@ -10854,8 +10855,8 @@
       <c r="V82">
         <v>12</v>
       </c>
-      <c r="W82">
-        <v>0.04</v>
+      <c r="W82" s="4">
+        <v>0.13672413793103441</v>
       </c>
       <c r="X82">
         <v>1100</v>
@@ -10955,8 +10956,8 @@
       <c r="V83">
         <v>13</v>
       </c>
-      <c r="W83">
-        <v>0.05</v>
+      <c r="W83" s="4">
+        <v>0.14517241379310336</v>
       </c>
       <c r="X83">
         <v>1200</v>
@@ -11056,8 +11057,8 @@
       <c r="V84">
         <v>13</v>
       </c>
-      <c r="W84">
-        <v>0.05</v>
+      <c r="W84" s="4">
+        <v>0.15362068965517231</v>
       </c>
       <c r="X84">
         <v>1300</v>
@@ -11157,8 +11158,8 @@
       <c r="V85">
         <v>14</v>
       </c>
-      <c r="W85">
-        <v>0.02</v>
+      <c r="W85" s="4">
+        <v>0.16206896551724129</v>
       </c>
       <c r="X85">
         <v>1500</v>
@@ -11258,8 +11259,8 @@
       <c r="V86">
         <v>15</v>
       </c>
-      <c r="W86">
-        <v>0.04</v>
+      <c r="W86" s="4">
+        <v>0.17051724137931024</v>
       </c>
       <c r="X86">
         <v>1700</v>
@@ -11365,8 +11366,8 @@
       <c r="V87">
         <v>15</v>
       </c>
-      <c r="W87">
-        <v>0.08</v>
+      <c r="W87" s="4">
+        <v>0.17896551724137921</v>
       </c>
       <c r="X87">
         <v>1700</v>
@@ -11466,8 +11467,8 @@
       <c r="V88">
         <v>16</v>
       </c>
-      <c r="W88">
-        <v>0.01</v>
+      <c r="W88" s="4">
+        <v>0.18741379310344816</v>
       </c>
       <c r="X88">
         <v>2000</v>
@@ -11567,8 +11568,8 @@
       <c r="V89">
         <v>17</v>
       </c>
-      <c r="W89">
-        <v>0.04</v>
+      <c r="W89" s="4">
+        <v>0.19586206896551711</v>
       </c>
       <c r="X89">
         <v>2300</v>
@@ -11674,8 +11675,8 @@
       <c r="V90">
         <v>17</v>
       </c>
-      <c r="W90">
-        <v>0.02</v>
+      <c r="W90" s="4">
+        <v>0.20431034482758609</v>
       </c>
       <c r="X90">
         <v>2450</v>
@@ -11775,8 +11776,8 @@
       <c r="V91">
         <v>18</v>
       </c>
-      <c r="W91">
-        <v>0.05</v>
+      <c r="W91" s="4">
+        <v>0.21275862068965504</v>
       </c>
       <c r="X91">
         <v>2600</v>
@@ -11876,8 +11877,8 @@
       <c r="V92">
         <v>19</v>
       </c>
-      <c r="W92">
-        <v>0.01</v>
+      <c r="W92" s="4">
+        <v>0.22120689655172399</v>
       </c>
       <c r="X92">
         <v>3000</v>
@@ -11983,8 +11984,8 @@
       <c r="V93">
         <v>19</v>
       </c>
-      <c r="W93">
-        <v>0.02</v>
+      <c r="W93" s="4">
+        <v>0.22965517241379296</v>
       </c>
       <c r="X93">
         <v>3300</v>
@@ -12084,8 +12085,8 @@
       <c r="V94">
         <v>20</v>
       </c>
-      <c r="W94">
-        <v>0.04</v>
+      <c r="W94" s="4">
+        <v>0.23810344827586191</v>
       </c>
       <c r="X94">
         <v>3400</v>
@@ -12185,8 +12186,8 @@
       <c r="V95">
         <v>20</v>
       </c>
-      <c r="W95">
-        <v>0.01</v>
+      <c r="W95" s="4">
+        <v>0.24655172413793086</v>
       </c>
       <c r="X95">
         <v>5000</v>
@@ -12286,8 +12287,8 @@
       <c r="V96">
         <v>21</v>
       </c>
-      <c r="W96">
-        <v>0.04</v>
+      <c r="W96" s="4">
+        <v>0.25499999999999984</v>
       </c>
       <c r="X96">
         <v>4500</v>
@@ -12387,8 +12388,8 @@
       <c r="V97">
         <v>22</v>
       </c>
-      <c r="W97">
-        <v>0.03</v>
+      <c r="W97" s="4">
+        <v>0.26344827586206881</v>
       </c>
       <c r="X97">
         <v>4700</v>
@@ -12488,8 +12489,8 @@
       <c r="V98">
         <v>23</v>
       </c>
-      <c r="W98">
-        <v>0.03</v>
+      <c r="W98" s="4">
+        <v>0.27189655172413774</v>
       </c>
       <c r="X98">
         <v>5000</v>
@@ -12589,8 +12590,8 @@
       <c r="V99">
         <v>23</v>
       </c>
-      <c r="W99">
-        <v>0.05</v>
+      <c r="W99" s="4">
+        <v>0.28034482758620671</v>
       </c>
       <c r="X99">
         <v>5250</v>
@@ -12690,8 +12691,8 @@
       <c r="V100">
         <v>24</v>
       </c>
-      <c r="W100">
-        <v>0.06</v>
+      <c r="W100" s="4">
+        <v>0.28879310344827569</v>
       </c>
       <c r="X100">
         <v>6000</v>
@@ -12797,8 +12798,8 @@
       <c r="V101">
         <v>25</v>
       </c>
-      <c r="W101">
-        <v>0.01</v>
+      <c r="W101" s="4">
+        <v>0.29724137931034461</v>
       </c>
       <c r="X101">
         <v>10000</v>
@@ -12901,8 +12902,8 @@
       <c r="V102">
         <v>25</v>
       </c>
-      <c r="W102">
-        <v>0.01</v>
+      <c r="W102" s="4">
+        <v>0.30568965517241359</v>
       </c>
       <c r="X102">
         <v>15000</v>
@@ -13005,8 +13006,8 @@
       <c r="V103">
         <v>26</v>
       </c>
-      <c r="W103">
-        <v>0.04</v>
+      <c r="W103" s="4">
+        <v>0.31413793103448256</v>
       </c>
       <c r="X103">
         <v>20000</v>
@@ -13109,8 +13110,8 @@
       <c r="V104">
         <v>27</v>
       </c>
-      <c r="W104">
-        <v>0.05</v>
+      <c r="W104" s="4">
+        <v>0.32258620689655149</v>
       </c>
       <c r="X104">
         <v>30000</v>
@@ -13213,8 +13214,8 @@
       <c r="V105">
         <v>27</v>
       </c>
-      <c r="W105">
-        <v>0.05</v>
+      <c r="W105" s="4">
+        <v>0.33103448275862046</v>
       </c>
       <c r="X105">
         <v>35000</v>
@@ -13317,8 +13318,8 @@
       <c r="V106">
         <v>28</v>
       </c>
-      <c r="W106">
-        <v>0.02</v>
+      <c r="W106" s="4">
+        <v>0.33948275862068944</v>
       </c>
       <c r="X106">
         <v>40000</v>
@@ -13421,8 +13422,8 @@
       <c r="V107">
         <v>29</v>
       </c>
-      <c r="W107">
-        <v>0.04</v>
+      <c r="W107" s="4">
+        <v>0.34793103448275842</v>
       </c>
       <c r="X107">
         <v>45000</v>
@@ -13525,8 +13526,8 @@
       <c r="V108">
         <v>29</v>
       </c>
-      <c r="W108">
-        <v>0.08</v>
+      <c r="W108" s="4">
+        <v>0.35637931034482734</v>
       </c>
       <c r="X108">
         <v>50000</v>
@@ -13629,8 +13630,8 @@
       <c r="V109">
         <v>30</v>
       </c>
-      <c r="W109">
-        <v>0.01</v>
+      <c r="W109" s="4">
+        <v>0.36482758620689631</v>
       </c>
       <c r="X109">
         <v>58000</v>
@@ -13733,8 +13734,8 @@
       <c r="V110">
         <v>31</v>
       </c>
-      <c r="W110">
-        <v>0.04</v>
+      <c r="W110" s="4">
+        <v>0.37327586206896529</v>
       </c>
       <c r="X110">
         <v>60000</v>
@@ -13837,8 +13838,8 @@
       <c r="V111">
         <v>31</v>
       </c>
-      <c r="W111">
-        <v>0.02</v>
+      <c r="W111" s="4">
+        <v>0.38172413793103421</v>
       </c>
       <c r="X111">
         <v>65000</v>
@@ -13941,8 +13942,8 @@
       <c r="V112">
         <v>32</v>
       </c>
-      <c r="W112">
-        <v>0.05</v>
+      <c r="W112" s="4">
+        <v>0.39017241379310319</v>
       </c>
       <c r="X112">
         <v>70000</v>
@@ -14045,8 +14046,8 @@
       <c r="V113">
         <v>33</v>
       </c>
-      <c r="W113">
-        <v>0.01</v>
+      <c r="W113" s="4">
+        <v>0.39862068965517217</v>
       </c>
       <c r="X113">
         <v>75000</v>
@@ -14149,8 +14150,8 @@
       <c r="V114">
         <v>33</v>
       </c>
-      <c r="W114">
-        <v>0.02</v>
+      <c r="W114" s="4">
+        <v>0.40706896551724109</v>
       </c>
       <c r="X114">
         <v>90000</v>
@@ -14253,8 +14254,8 @@
       <c r="V115">
         <v>34</v>
       </c>
-      <c r="W115">
-        <v>0.04</v>
+      <c r="W115" s="4">
+        <v>0.41551724137931006</v>
       </c>
       <c r="X115">
         <v>95000</v>
@@ -14357,8 +14358,8 @@
       <c r="V116">
         <v>35</v>
       </c>
-      <c r="W116">
-        <v>0.01</v>
+      <c r="W116" s="4">
+        <v>0.42396551724137904</v>
       </c>
       <c r="X116">
         <v>100000</v>
@@ -14461,8 +14462,8 @@
       <c r="V117">
         <v>35</v>
       </c>
-      <c r="W117">
-        <v>0.01</v>
+      <c r="W117" s="4">
+        <v>0.43241379310344796</v>
       </c>
       <c r="X117">
         <v>100000</v>
@@ -14565,8 +14566,8 @@
       <c r="V118">
         <v>36</v>
       </c>
-      <c r="W118">
-        <v>0.01</v>
+      <c r="W118" s="4">
+        <v>0.44086206896551694</v>
       </c>
       <c r="X118">
         <v>100000</v>
@@ -14669,8 +14670,8 @@
       <c r="V119">
         <v>37</v>
       </c>
-      <c r="W119">
-        <v>0.04</v>
+      <c r="W119" s="4">
+        <v>0.44931034482758592</v>
       </c>
       <c r="X119">
         <v>100000</v>
@@ -14773,8 +14774,8 @@
       <c r="V120">
         <v>37</v>
       </c>
-      <c r="W120">
-        <v>0.05</v>
+      <c r="W120" s="4">
+        <v>0.45775862068965484</v>
       </c>
       <c r="X120">
         <v>100000</v>
@@ -14877,8 +14878,8 @@
       <c r="V121">
         <v>38</v>
       </c>
-      <c r="W121">
-        <v>0.05</v>
+      <c r="W121" s="4">
+        <v>0.46620689655172382</v>
       </c>
       <c r="X121">
         <v>100000</v>
@@ -14981,8 +14982,8 @@
       <c r="V122">
         <v>39</v>
       </c>
-      <c r="W122">
-        <v>0.02</v>
+      <c r="W122" s="4">
+        <v>0.47465517241379279</v>
       </c>
       <c r="X122">
         <v>100000</v>
@@ -15085,8 +15086,8 @@
       <c r="V123">
         <v>39</v>
       </c>
-      <c r="W123">
-        <v>0.04</v>
+      <c r="W123" s="4">
+        <v>0.48310344827586171</v>
       </c>
       <c r="X123">
         <v>100000</v>
@@ -15189,8 +15190,8 @@
       <c r="V124">
         <v>40</v>
       </c>
-      <c r="W124">
-        <v>0.08</v>
+      <c r="W124" s="4">
+        <v>0.49155172413793069</v>
       </c>
       <c r="X124">
         <v>100000</v>
@@ -15293,8 +15294,8 @@
       <c r="V125">
         <v>50</v>
       </c>
-      <c r="W125">
-        <v>0.01</v>
+      <c r="W125" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X125">
         <v>100000</v>
@@ -16850,7 +16851,7 @@
       <c r="V140">
         <v>2</v>
       </c>
-      <c r="W140">
+      <c r="W140" s="4">
         <v>0.01</v>
       </c>
       <c r="X140">
@@ -16945,8 +16946,8 @@
       <c r="V141">
         <v>3</v>
       </c>
-      <c r="W141">
-        <v>0.02</v>
+      <c r="W141" s="4">
+        <v>1.8448275862068958E-2</v>
       </c>
       <c r="X141">
         <v>25</v>
@@ -17046,8 +17047,8 @@
       <c r="V142">
         <v>3</v>
       </c>
-      <c r="W142">
-        <v>0.03</v>
+      <c r="W142" s="4">
+        <v>2.6896551724137921E-2</v>
       </c>
       <c r="X142">
         <v>50</v>
@@ -17147,8 +17148,8 @@
       <c r="V143">
         <v>4</v>
       </c>
-      <c r="W143">
-        <v>0.03</v>
+      <c r="W143" s="4">
+        <v>3.5344827586206877E-2</v>
       </c>
       <c r="X143">
         <v>30</v>
@@ -17248,8 +17249,8 @@
       <c r="V144">
         <v>5</v>
       </c>
-      <c r="W144">
-        <v>0.03</v>
+      <c r="W144" s="4">
+        <v>4.379310344827584E-2</v>
       </c>
       <c r="X144">
         <v>40</v>
@@ -17349,8 +17350,8 @@
       <c r="V145">
         <v>5</v>
       </c>
-      <c r="W145">
-        <v>0.05</v>
+      <c r="W145" s="4">
+        <v>5.2241379310344803E-2</v>
       </c>
       <c r="X145">
         <v>75</v>
@@ -17450,8 +17451,8 @@
       <c r="V146">
         <v>6</v>
       </c>
-      <c r="W146">
-        <v>0.1</v>
+      <c r="W146" s="4">
+        <v>6.0689655172413759E-2</v>
       </c>
       <c r="X146">
         <v>80</v>
@@ -17551,8 +17552,8 @@
       <c r="V147">
         <v>7</v>
       </c>
-      <c r="W147">
-        <v>0.05</v>
+      <c r="W147" s="4">
+        <v>6.9137931034482708E-2</v>
       </c>
       <c r="X147">
         <v>95</v>
@@ -17652,8 +17653,8 @@
       <c r="V148">
         <v>7</v>
       </c>
-      <c r="W148">
-        <v>0.09</v>
+      <c r="W148" s="4">
+        <v>7.7586206896551671E-2</v>
       </c>
       <c r="X148">
         <v>100</v>
@@ -17759,8 +17760,8 @@
       <c r="V149">
         <v>8</v>
       </c>
-      <c r="W149">
-        <v>0.05</v>
+      <c r="W149" s="4">
+        <v>8.6034482758620634E-2</v>
       </c>
       <c r="X149">
         <v>250</v>
@@ -17860,8 +17861,8 @@
       <c r="V150">
         <v>9</v>
       </c>
-      <c r="W150">
-        <v>0.05</v>
+      <c r="W150" s="4">
+        <v>9.4482758620689597E-2</v>
       </c>
       <c r="X150">
         <v>350</v>
@@ -17967,8 +17968,8 @@
       <c r="V151">
         <v>10</v>
       </c>
-      <c r="W151">
-        <v>0.1</v>
+      <c r="W151" s="4">
+        <v>0.10293103448275855</v>
       </c>
       <c r="X151">
         <v>500</v>
@@ -18068,8 +18069,8 @@
       <c r="V152">
         <v>10</v>
       </c>
-      <c r="W152">
-        <v>0.01</v>
+      <c r="W152" s="4">
+        <v>0.11137931034482751</v>
       </c>
       <c r="X152">
         <v>750</v>
@@ -18169,8 +18170,8 @@
       <c r="V153">
         <v>11</v>
       </c>
-      <c r="W153">
-        <v>0.01</v>
+      <c r="W153" s="4">
+        <v>0.11982758620689647</v>
       </c>
       <c r="X153">
         <v>825</v>
@@ -18270,8 +18271,8 @@
       <c r="V154">
         <v>12</v>
       </c>
-      <c r="W154">
-        <v>0.05</v>
+      <c r="W154" s="4">
+        <v>0.12827586206896543</v>
       </c>
       <c r="X154">
         <v>1000</v>
@@ -18371,8 +18372,8 @@
       <c r="V155">
         <v>12</v>
       </c>
-      <c r="W155">
-        <v>0.04</v>
+      <c r="W155" s="4">
+        <v>0.13672413793103441</v>
       </c>
       <c r="X155">
         <v>1100</v>
@@ -18472,8 +18473,8 @@
       <c r="V156">
         <v>13</v>
       </c>
-      <c r="W156">
-        <v>0.05</v>
+      <c r="W156" s="4">
+        <v>0.14517241379310336</v>
       </c>
       <c r="X156">
         <v>1200</v>
@@ -18573,8 +18574,8 @@
       <c r="V157">
         <v>14</v>
       </c>
-      <c r="W157">
-        <v>0.02</v>
+      <c r="W157" s="4">
+        <v>0.15362068965517231</v>
       </c>
       <c r="X157">
         <v>1500</v>
@@ -18674,8 +18675,8 @@
       <c r="V158">
         <v>14</v>
       </c>
-      <c r="W158">
-        <v>0.04</v>
+      <c r="W158" s="4">
+        <v>0.16206896551724129</v>
       </c>
       <c r="X158">
         <v>1700</v>
@@ -18775,8 +18776,8 @@
       <c r="V159">
         <v>15</v>
       </c>
-      <c r="W159">
-        <v>0.08</v>
+      <c r="W159" s="4">
+        <v>0.17051724137931024</v>
       </c>
       <c r="X159">
         <v>1700</v>
@@ -18876,8 +18877,8 @@
       <c r="V160">
         <v>16</v>
       </c>
-      <c r="W160">
-        <v>0.01</v>
+      <c r="W160" s="4">
+        <v>0.17896551724137921</v>
       </c>
       <c r="X160">
         <v>2000</v>
@@ -18977,8 +18978,8 @@
       <c r="V161">
         <v>16</v>
       </c>
-      <c r="W161">
-        <v>0.04</v>
+      <c r="W161" s="4">
+        <v>0.18741379310344816</v>
       </c>
       <c r="X161">
         <v>2300</v>
@@ -19078,8 +19079,8 @@
       <c r="V162">
         <v>17</v>
       </c>
-      <c r="W162">
-        <v>0.02</v>
+      <c r="W162" s="4">
+        <v>0.19586206896551711</v>
       </c>
       <c r="X162">
         <v>2450</v>
@@ -19179,8 +19180,8 @@
       <c r="V163">
         <v>18</v>
       </c>
-      <c r="W163">
-        <v>0.05</v>
+      <c r="W163" s="4">
+        <v>0.20431034482758609</v>
       </c>
       <c r="X163">
         <v>2600</v>
@@ -19280,8 +19281,8 @@
       <c r="V164">
         <v>18</v>
       </c>
-      <c r="W164">
-        <v>0.01</v>
+      <c r="W164" s="4">
+        <v>0.21275862068965504</v>
       </c>
       <c r="X164">
         <v>3000</v>
@@ -19387,8 +19388,8 @@
       <c r="V165">
         <v>19</v>
       </c>
-      <c r="W165">
-        <v>0.02</v>
+      <c r="W165" s="4">
+        <v>0.22120689655172399</v>
       </c>
       <c r="X165">
         <v>3300</v>
@@ -19488,8 +19489,8 @@
       <c r="V166">
         <v>20</v>
       </c>
-      <c r="W166">
-        <v>0.04</v>
+      <c r="W166" s="4">
+        <v>0.22965517241379296</v>
       </c>
       <c r="X166">
         <v>3400</v>
@@ -19595,8 +19596,8 @@
       <c r="V167">
         <v>20</v>
       </c>
-      <c r="W167">
-        <v>0.01</v>
+      <c r="W167" s="4">
+        <v>0.23810344827586191</v>
       </c>
       <c r="X167">
         <v>5000</v>
@@ -19696,8 +19697,8 @@
       <c r="V168">
         <v>21</v>
       </c>
-      <c r="W168">
-        <v>0.04</v>
+      <c r="W168" s="4">
+        <v>0.24655172413793086</v>
       </c>
       <c r="X168">
         <v>4500</v>
@@ -19797,8 +19798,8 @@
       <c r="V169">
         <v>22</v>
       </c>
-      <c r="W169">
-        <v>0.03</v>
+      <c r="W169" s="4">
+        <v>0.25499999999999984</v>
       </c>
       <c r="X169">
         <v>4700</v>
@@ -19898,8 +19899,8 @@
       <c r="V170">
         <v>23</v>
       </c>
-      <c r="W170">
-        <v>0.03</v>
+      <c r="W170" s="4">
+        <v>0.26344827586206881</v>
       </c>
       <c r="X170">
         <v>5000</v>
@@ -19999,8 +20000,8 @@
       <c r="V171">
         <v>23</v>
       </c>
-      <c r="W171">
-        <v>0.05</v>
+      <c r="W171" s="4">
+        <v>0.27189655172413774</v>
       </c>
       <c r="X171">
         <v>5250</v>
@@ -20100,8 +20101,8 @@
       <c r="V172">
         <v>24</v>
       </c>
-      <c r="W172">
-        <v>0.06</v>
+      <c r="W172" s="4">
+        <v>0.28034482758620671</v>
       </c>
       <c r="X172">
         <v>6000</v>
@@ -20201,8 +20202,8 @@
       <c r="V173">
         <v>25</v>
       </c>
-      <c r="W173">
-        <v>0.01</v>
+      <c r="W173" s="4">
+        <v>0.28879310344827569</v>
       </c>
       <c r="X173">
         <v>10000</v>
@@ -20305,8 +20306,8 @@
       <c r="V174">
         <v>25</v>
       </c>
-      <c r="W174">
-        <v>0.01</v>
+      <c r="W174" s="4">
+        <v>0.29724137931034461</v>
       </c>
       <c r="X174">
         <v>15000</v>
@@ -20409,8 +20410,8 @@
       <c r="V175">
         <v>26</v>
       </c>
-      <c r="W175">
-        <v>0.04</v>
+      <c r="W175" s="4">
+        <v>0.30568965517241359</v>
       </c>
       <c r="X175">
         <v>20000</v>
@@ -20513,8 +20514,8 @@
       <c r="V176">
         <v>27</v>
       </c>
-      <c r="W176">
-        <v>0.05</v>
+      <c r="W176" s="4">
+        <v>0.31413793103448256</v>
       </c>
       <c r="X176">
         <v>30000</v>
@@ -20617,8 +20618,8 @@
       <c r="V177">
         <v>27</v>
       </c>
-      <c r="W177">
-        <v>0.05</v>
+      <c r="W177" s="4">
+        <v>0.32258620689655149</v>
       </c>
       <c r="X177">
         <v>35000</v>
@@ -20727,8 +20728,8 @@
       <c r="V178">
         <v>28</v>
       </c>
-      <c r="W178">
-        <v>0.02</v>
+      <c r="W178" s="4">
+        <v>0.33103448275862046</v>
       </c>
       <c r="X178">
         <v>40000</v>
@@ -20831,8 +20832,8 @@
       <c r="V179">
         <v>29</v>
       </c>
-      <c r="W179">
-        <v>0.04</v>
+      <c r="W179" s="4">
+        <v>0.33948275862068944</v>
       </c>
       <c r="X179">
         <v>45000</v>
@@ -20935,8 +20936,8 @@
       <c r="V180">
         <v>29</v>
       </c>
-      <c r="W180">
-        <v>0.08</v>
+      <c r="W180" s="4">
+        <v>0.34793103448275842</v>
       </c>
       <c r="X180">
         <v>50000</v>
@@ -21039,8 +21040,8 @@
       <c r="V181">
         <v>30</v>
       </c>
-      <c r="W181">
-        <v>0.01</v>
+      <c r="W181" s="4">
+        <v>0.35637931034482734</v>
       </c>
       <c r="X181">
         <v>58000</v>
@@ -21143,8 +21144,8 @@
       <c r="V182">
         <v>31</v>
       </c>
-      <c r="W182">
-        <v>0.04</v>
+      <c r="W182" s="4">
+        <v>0.36482758620689631</v>
       </c>
       <c r="X182">
         <v>60000</v>
@@ -21247,8 +21248,8 @@
       <c r="V183">
         <v>31</v>
       </c>
-      <c r="W183">
-        <v>0.02</v>
+      <c r="W183" s="4">
+        <v>0.37327586206896529</v>
       </c>
       <c r="X183">
         <v>65000</v>
@@ -21351,8 +21352,8 @@
       <c r="V184">
         <v>32</v>
       </c>
-      <c r="W184">
-        <v>0.05</v>
+      <c r="W184" s="4">
+        <v>0.38172413793103421</v>
       </c>
       <c r="X184">
         <v>70000</v>
@@ -21455,8 +21456,8 @@
       <c r="V185">
         <v>33</v>
       </c>
-      <c r="W185">
-        <v>0.01</v>
+      <c r="W185" s="4">
+        <v>0.39017241379310319</v>
       </c>
       <c r="X185">
         <v>75000</v>
@@ -21559,8 +21560,8 @@
       <c r="V186">
         <v>34</v>
       </c>
-      <c r="W186">
-        <v>0.02</v>
+      <c r="W186" s="4">
+        <v>0.39862068965517217</v>
       </c>
       <c r="X186">
         <v>90000</v>
@@ -21663,8 +21664,8 @@
       <c r="V187">
         <v>34</v>
       </c>
-      <c r="W187">
-        <v>0.04</v>
+      <c r="W187" s="4">
+        <v>0.40706896551724109</v>
       </c>
       <c r="X187">
         <v>95000</v>
@@ -21767,8 +21768,8 @@
       <c r="V188">
         <v>35</v>
       </c>
-      <c r="W188">
-        <v>0.01</v>
+      <c r="W188" s="4">
+        <v>0.41551724137931006</v>
       </c>
       <c r="X188">
         <v>100000</v>
@@ -21871,8 +21872,8 @@
       <c r="V189">
         <v>36</v>
       </c>
-      <c r="W189">
-        <v>0.01</v>
+      <c r="W189" s="4">
+        <v>0.42396551724137904</v>
       </c>
       <c r="X189">
         <v>100000</v>
@@ -21975,8 +21976,8 @@
       <c r="V190">
         <v>36</v>
       </c>
-      <c r="W190">
-        <v>0.01</v>
+      <c r="W190" s="4">
+        <v>0.43241379310344796</v>
       </c>
       <c r="X190">
         <v>100000</v>
@@ -22079,8 +22080,8 @@
       <c r="V191">
         <v>37</v>
       </c>
-      <c r="W191">
-        <v>0.04</v>
+      <c r="W191" s="4">
+        <v>0.44086206896551694</v>
       </c>
       <c r="X191">
         <v>100000</v>
@@ -22183,8 +22184,8 @@
       <c r="V192">
         <v>38</v>
       </c>
-      <c r="W192">
-        <v>0.05</v>
+      <c r="W192" s="4">
+        <v>0.44931034482758592</v>
       </c>
       <c r="X192">
         <v>100000</v>
@@ -22287,8 +22288,8 @@
       <c r="V193">
         <v>38</v>
       </c>
-      <c r="W193">
-        <v>0.05</v>
+      <c r="W193" s="4">
+        <v>0.45775862068965484</v>
       </c>
       <c r="X193">
         <v>100000</v>
@@ -22391,8 +22392,8 @@
       <c r="V194">
         <v>39</v>
       </c>
-      <c r="W194">
-        <v>0.02</v>
+      <c r="W194" s="4">
+        <v>0.46620689655172382</v>
       </c>
       <c r="X194">
         <v>100000</v>
@@ -22495,8 +22496,8 @@
       <c r="V195">
         <v>40</v>
       </c>
-      <c r="W195">
-        <v>0.04</v>
+      <c r="W195" s="4">
+        <v>0.47465517241379279</v>
       </c>
       <c r="X195">
         <v>100000</v>
@@ -22599,8 +22600,8 @@
       <c r="V196">
         <v>40</v>
       </c>
-      <c r="W196">
-        <v>0.08</v>
+      <c r="W196" s="4">
+        <v>0.48310344827586171</v>
       </c>
       <c r="X196">
         <v>100000</v>
@@ -22703,8 +22704,8 @@
       <c r="V197">
         <v>41</v>
       </c>
-      <c r="W197">
-        <v>0.01</v>
+      <c r="W197" s="4">
+        <v>0.49155172413793069</v>
       </c>
       <c r="X197">
         <v>100000</v>
@@ -22807,8 +22808,8 @@
       <c r="V198">
         <v>60</v>
       </c>
-      <c r="W198">
-        <v>0.04</v>
+      <c r="W198" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X198">
         <v>100000</v>
@@ -24159,7 +24160,7 @@
       <c r="V211">
         <v>5</v>
       </c>
-      <c r="W211">
+      <c r="W211" s="4">
         <v>0.01</v>
       </c>
       <c r="X211">
@@ -24257,8 +24258,8 @@
       <c r="V212">
         <v>6.1206896551724101</v>
       </c>
-      <c r="W212">
-        <v>0.02</v>
+      <c r="W212" s="4">
+        <v>1.8448275862068958E-2</v>
       </c>
       <c r="X212">
         <v>25</v>
@@ -24358,8 +24359,8 @@
       <c r="V213">
         <v>7.2413793103448203</v>
       </c>
-      <c r="W213">
-        <v>0.03</v>
+      <c r="W213" s="4">
+        <v>2.6896551724137921E-2</v>
       </c>
       <c r="X213">
         <v>50</v>
@@ -24459,8 +24460,8 @@
       <c r="V214">
         <v>8.3620689655172296</v>
       </c>
-      <c r="W214">
-        <v>0.03</v>
+      <c r="W214" s="4">
+        <v>3.5344827586206877E-2</v>
       </c>
       <c r="X214">
         <v>30</v>
@@ -24560,8 +24561,8 @@
       <c r="V215">
         <v>9.4827586206896406</v>
       </c>
-      <c r="W215">
-        <v>0.03</v>
+      <c r="W215" s="4">
+        <v>4.379310344827584E-2</v>
       </c>
       <c r="X215">
         <v>40</v>
@@ -24661,8 +24662,8 @@
       <c r="V216">
         <v>10.60344827586205</v>
       </c>
-      <c r="W216">
-        <v>0.05</v>
+      <c r="W216" s="4">
+        <v>5.2241379310344803E-2</v>
       </c>
       <c r="X216">
         <v>75</v>
@@ -24762,8 +24763,8 @@
       <c r="V217">
         <v>11.724137931034459</v>
       </c>
-      <c r="W217">
-        <v>0.1</v>
+      <c r="W217" s="4">
+        <v>6.0689655172413759E-2</v>
       </c>
       <c r="X217">
         <v>80</v>
@@ -24863,8 +24864,8 @@
       <c r="V218">
         <v>12.844827586206868</v>
       </c>
-      <c r="W218">
-        <v>0.05</v>
+      <c r="W218" s="4">
+        <v>6.9137931034482708E-2</v>
       </c>
       <c r="X218">
         <v>95</v>
@@ -24964,8 +24965,8 @@
       <c r="V219">
         <v>13.965517241379279</v>
       </c>
-      <c r="W219">
-        <v>0.09</v>
+      <c r="W219" s="4">
+        <v>7.7586206896551671E-2</v>
       </c>
       <c r="X219">
         <v>100</v>
@@ -25065,8 +25066,8 @@
       <c r="V220">
         <v>15.086206896551689</v>
       </c>
-      <c r="W220">
-        <v>0.05</v>
+      <c r="W220" s="4">
+        <v>8.6034482758620634E-2</v>
       </c>
       <c r="X220">
         <v>250</v>
@@ -25166,8 +25167,8 @@
       <c r="V221">
         <v>16.2068965517241</v>
       </c>
-      <c r="W221">
-        <v>0.05</v>
+      <c r="W221" s="4">
+        <v>9.4482758620689597E-2</v>
       </c>
       <c r="X221">
         <v>350</v>
@@ -25267,8 +25268,8 @@
       <c r="V222">
         <v>17.327586206896509</v>
       </c>
-      <c r="W222">
-        <v>0.1</v>
+      <c r="W222" s="4">
+        <v>0.10293103448275855</v>
       </c>
       <c r="X222">
         <v>500</v>
@@ -25368,8 +25369,8 @@
       <c r="V223">
         <v>18.448275862068918</v>
       </c>
-      <c r="W223">
-        <v>0.01</v>
+      <c r="W223" s="4">
+        <v>0.11137931034482751</v>
       </c>
       <c r="X223">
         <v>750</v>
@@ -25469,8 +25470,8 @@
       <c r="V224">
         <v>19.568965517241331</v>
       </c>
-      <c r="W224">
-        <v>0.01</v>
+      <c r="W224" s="4">
+        <v>0.11982758620689647</v>
       </c>
       <c r="X224">
         <v>825</v>
@@ -25570,8 +25571,8 @@
       <c r="V225">
         <v>20.689655172413737</v>
       </c>
-      <c r="W225">
-        <v>0.05</v>
+      <c r="W225" s="4">
+        <v>0.12827586206896543</v>
       </c>
       <c r="X225">
         <v>1000</v>
@@ -25671,8 +25672,8 @@
       <c r="V226">
         <v>21.81034482758615</v>
       </c>
-      <c r="W226">
-        <v>0.04</v>
+      <c r="W226" s="4">
+        <v>0.13672413793103441</v>
       </c>
       <c r="X226">
         <v>1100</v>
@@ -25772,8 +25773,8 @@
       <c r="V227">
         <v>22.931034482758559</v>
       </c>
-      <c r="W227">
-        <v>0.05</v>
+      <c r="W227" s="4">
+        <v>0.14517241379310336</v>
       </c>
       <c r="X227">
         <v>1200</v>
@@ -25873,8 +25874,8 @@
       <c r="V228">
         <v>24.051724137930968</v>
       </c>
-      <c r="W228">
-        <v>0.05</v>
+      <c r="W228" s="4">
+        <v>0.15362068965517231</v>
       </c>
       <c r="X228">
         <v>1300</v>
@@ -25974,8 +25975,8 @@
       <c r="V229">
         <v>25.172413793103377</v>
       </c>
-      <c r="W229">
-        <v>0.02</v>
+      <c r="W229" s="4">
+        <v>0.16206896551724129</v>
       </c>
       <c r="X229">
         <v>1500</v>
@@ -26075,8 +26076,8 @@
       <c r="V230">
         <v>26.29310344827579</v>
       </c>
-      <c r="W230">
-        <v>0.04</v>
+      <c r="W230" s="4">
+        <v>0.17051724137931024</v>
       </c>
       <c r="X230">
         <v>1700</v>
@@ -26176,8 +26177,8 @@
       <c r="V231">
         <v>27.413793103448199</v>
       </c>
-      <c r="W231">
-        <v>0.08</v>
+      <c r="W231" s="4">
+        <v>0.17896551724137921</v>
       </c>
       <c r="X231">
         <v>1700</v>
@@ -26277,8 +26278,8 @@
       <c r="V232">
         <v>28.534482758620609</v>
       </c>
-      <c r="W232">
-        <v>0.01</v>
+      <c r="W232" s="4">
+        <v>0.18741379310344816</v>
       </c>
       <c r="X232">
         <v>2000</v>
@@ -26378,8 +26379,8 @@
       <c r="V233">
         <v>29.655172413793018</v>
       </c>
-      <c r="W233">
-        <v>0.04</v>
+      <c r="W233" s="4">
+        <v>0.19586206896551711</v>
       </c>
       <c r="X233">
         <v>2300</v>
@@ -26479,8 +26480,8 @@
       <c r="V234">
         <v>30.775862068965427</v>
       </c>
-      <c r="W234">
-        <v>0.02</v>
+      <c r="W234" s="4">
+        <v>0.20431034482758609</v>
       </c>
       <c r="X234">
         <v>2450</v>
@@ -26580,8 +26581,8 @@
       <c r="V235">
         <v>31.896551724137836</v>
       </c>
-      <c r="W235">
-        <v>0.05</v>
+      <c r="W235" s="4">
+        <v>0.21275862068965504</v>
       </c>
       <c r="X235">
         <v>2600</v>
@@ -26681,8 +26682,8 @@
       <c r="V236">
         <v>33.017241379310249</v>
       </c>
-      <c r="W236">
-        <v>0.01</v>
+      <c r="W236" s="4">
+        <v>0.22120689655172399</v>
       </c>
       <c r="X236">
         <v>3000</v>
@@ -26782,8 +26783,8 @@
       <c r="V237">
         <v>34.137931034482662</v>
       </c>
-      <c r="W237">
-        <v>0.02</v>
+      <c r="W237" s="4">
+        <v>0.22965517241379296</v>
       </c>
       <c r="X237">
         <v>3300</v>
@@ -26883,8 +26884,8 @@
       <c r="V238">
         <v>35.258620689655068</v>
       </c>
-      <c r="W238">
-        <v>0.04</v>
+      <c r="W238" s="4">
+        <v>0.23810344827586191</v>
       </c>
       <c r="X238">
         <v>3400</v>
@@ -26984,8 +26985,8 @@
       <c r="V239">
         <v>36.379310344827474</v>
       </c>
-      <c r="W239">
-        <v>0.01</v>
+      <c r="W239" s="4">
+        <v>0.24655172413793086</v>
       </c>
       <c r="X239">
         <v>5000</v>
@@ -27085,8 +27086,8 @@
       <c r="V240">
         <v>37.499999999999886</v>
       </c>
-      <c r="W240">
-        <v>0.04</v>
+      <c r="W240" s="4">
+        <v>0.25499999999999984</v>
       </c>
       <c r="X240">
         <v>4500</v>
@@ -27186,8 +27187,8 @@
       <c r="V241">
         <v>38.620689655172299</v>
       </c>
-      <c r="W241">
-        <v>0.03</v>
+      <c r="W241" s="4">
+        <v>0.26344827586206881</v>
       </c>
       <c r="X241">
         <v>4700</v>
@@ -27287,8 +27288,8 @@
       <c r="V242">
         <v>39.741379310344705</v>
       </c>
-      <c r="W242">
-        <v>0.03</v>
+      <c r="W242" s="4">
+        <v>0.27189655172413774</v>
       </c>
       <c r="X242">
         <v>5000</v>
@@ -27388,8 +27389,8 @@
       <c r="V243">
         <v>40.862068965517118</v>
       </c>
-      <c r="W243">
-        <v>0.05</v>
+      <c r="W243" s="4">
+        <v>0.28034482758620671</v>
       </c>
       <c r="X243">
         <v>5250</v>
@@ -27489,8 +27490,8 @@
       <c r="V244">
         <v>41.98275862068953</v>
       </c>
-      <c r="W244">
-        <v>0.06</v>
+      <c r="W244" s="4">
+        <v>0.28879310344827569</v>
       </c>
       <c r="X244">
         <v>6000</v>
@@ -27590,8 +27591,8 @@
       <c r="V245">
         <v>43.103448275861936</v>
       </c>
-      <c r="W245">
-        <v>0.01</v>
+      <c r="W245" s="4">
+        <v>0.29724137931034461</v>
       </c>
       <c r="X245">
         <v>10000</v>
@@ -27694,8 +27695,8 @@
       <c r="V246">
         <v>44.224137931034349</v>
       </c>
-      <c r="W246">
-        <v>0.01</v>
+      <c r="W246" s="4">
+        <v>0.30568965517241359</v>
       </c>
       <c r="X246">
         <v>15000</v>
@@ -27798,8 +27799,8 @@
       <c r="V247">
         <v>45.344827586206755</v>
       </c>
-      <c r="W247">
-        <v>0.04</v>
+      <c r="W247" s="4">
+        <v>0.31413793103448256</v>
       </c>
       <c r="X247">
         <v>20000</v>
@@ -27902,8 +27903,8 @@
       <c r="V248">
         <v>46.465517241379168</v>
       </c>
-      <c r="W248">
-        <v>0.05</v>
+      <c r="W248" s="4">
+        <v>0.32258620689655149</v>
       </c>
       <c r="X248">
         <v>30000</v>
@@ -28006,8 +28007,8 @@
       <c r="V249">
         <v>47.58620689655158</v>
       </c>
-      <c r="W249">
-        <v>0.05</v>
+      <c r="W249" s="4">
+        <v>0.33103448275862046</v>
       </c>
       <c r="X249">
         <v>35000</v>
@@ -28110,8 +28111,8 @@
       <c r="V250">
         <v>48.706896551723986</v>
       </c>
-      <c r="W250">
-        <v>0.02</v>
+      <c r="W250" s="4">
+        <v>0.33948275862068944</v>
       </c>
       <c r="X250">
         <v>40000</v>
@@ -28214,8 +28215,8 @@
       <c r="V251">
         <v>49.827586206896399</v>
       </c>
-      <c r="W251">
-        <v>0.04</v>
+      <c r="W251" s="4">
+        <v>0.34793103448275842</v>
       </c>
       <c r="X251">
         <v>45000</v>
@@ -28318,8 +28319,8 @@
       <c r="V252">
         <v>50.948275862068805</v>
       </c>
-      <c r="W252">
-        <v>0.08</v>
+      <c r="W252" s="4">
+        <v>0.35637931034482734</v>
       </c>
       <c r="X252">
         <v>50000</v>
@@ -28422,8 +28423,8 @@
       <c r="V253">
         <v>52.068965517241217</v>
       </c>
-      <c r="W253">
-        <v>0.01</v>
+      <c r="W253" s="4">
+        <v>0.36482758620689631</v>
       </c>
       <c r="X253">
         <v>58000</v>
@@ -28526,8 +28527,8 @@
       <c r="V254">
         <v>53.18965517241363</v>
       </c>
-      <c r="W254">
-        <v>0.04</v>
+      <c r="W254" s="4">
+        <v>0.37327586206896529</v>
       </c>
       <c r="X254">
         <v>60000</v>
@@ -28630,8 +28631,8 @@
       <c r="V255">
         <v>54.310344827586036</v>
       </c>
-      <c r="W255">
-        <v>0.02</v>
+      <c r="W255" s="4">
+        <v>0.38172413793103421</v>
       </c>
       <c r="X255">
         <v>65000</v>
@@ -28734,8 +28735,8 @@
       <c r="V256">
         <v>55.431034482758449</v>
       </c>
-      <c r="W256">
-        <v>0.05</v>
+      <c r="W256" s="4">
+        <v>0.39017241379310319</v>
       </c>
       <c r="X256">
         <v>70000</v>
@@ -28838,8 +28839,8 @@
       <c r="V257">
         <v>56.551724137930854</v>
       </c>
-      <c r="W257">
-        <v>0.01</v>
+      <c r="W257" s="4">
+        <v>0.39862068965517217</v>
       </c>
       <c r="X257">
         <v>75000</v>
@@ -28942,8 +28943,8 @@
       <c r="V258">
         <v>57.672413793103267</v>
       </c>
-      <c r="W258">
-        <v>0.02</v>
+      <c r="W258" s="4">
+        <v>0.40706896551724109</v>
       </c>
       <c r="X258">
         <v>90000</v>
@@ -29046,8 +29047,8 @@
       <c r="V259">
         <v>58.793103448275673</v>
       </c>
-      <c r="W259">
-        <v>0.04</v>
+      <c r="W259" s="4">
+        <v>0.41551724137931006</v>
       </c>
       <c r="X259">
         <v>95000</v>
@@ -29150,8 +29151,8 @@
       <c r="V260">
         <v>59.913793103448086</v>
       </c>
-      <c r="W260">
-        <v>0.01</v>
+      <c r="W260" s="4">
+        <v>0.42396551724137904</v>
       </c>
       <c r="X260">
         <v>100000</v>
@@ -29254,8 +29255,8 @@
       <c r="V261">
         <v>61.034482758620499</v>
       </c>
-      <c r="W261">
-        <v>0.01</v>
+      <c r="W261" s="4">
+        <v>0.43241379310344796</v>
       </c>
       <c r="X261">
         <v>100000</v>
@@ -29358,8 +29359,8 @@
       <c r="V262">
         <v>62.155172413792904</v>
       </c>
-      <c r="W262">
-        <v>0.01</v>
+      <c r="W262" s="4">
+        <v>0.44086206896551694</v>
       </c>
       <c r="X262">
         <v>100000</v>
@@ -29462,8 +29463,8 @@
       <c r="V263">
         <v>63.275862068965317</v>
       </c>
-      <c r="W263">
-        <v>0.04</v>
+      <c r="W263" s="4">
+        <v>0.44931034482758592</v>
       </c>
       <c r="X263">
         <v>100000</v>
@@ -29566,8 +29567,8 @@
       <c r="V264">
         <v>64.396551724137723</v>
       </c>
-      <c r="W264">
-        <v>0.05</v>
+      <c r="W264" s="4">
+        <v>0.45775862068965484</v>
       </c>
       <c r="X264">
         <v>100000</v>
@@ -29670,8 +29671,8 @@
       <c r="V265">
         <v>65.517241379310136</v>
       </c>
-      <c r="W265">
-        <v>0.05</v>
+      <c r="W265" s="4">
+        <v>0.46620689655172382</v>
       </c>
       <c r="X265">
         <v>100000</v>
@@ -29774,8 +29775,8 @@
       <c r="V266">
         <v>66.637931034482548</v>
       </c>
-      <c r="W266">
-        <v>0.02</v>
+      <c r="W266" s="4">
+        <v>0.47465517241379279</v>
       </c>
       <c r="X266">
         <v>100000</v>
@@ -29878,8 +29879,8 @@
       <c r="V267">
         <v>67.758620689654947</v>
       </c>
-      <c r="W267">
-        <v>0.04</v>
+      <c r="W267" s="4">
+        <v>0.48310344827586171</v>
       </c>
       <c r="X267">
         <v>100000</v>
@@ -29982,8 +29983,8 @@
       <c r="V268">
         <v>68.87931034482736</v>
       </c>
-      <c r="W268">
-        <v>0.08</v>
+      <c r="W268" s="4">
+        <v>0.49155172413793069</v>
       </c>
       <c r="X268">
         <v>100000</v>
@@ -30086,8 +30087,8 @@
       <c r="V269">
         <v>69.999999999999773</v>
       </c>
-      <c r="W269">
-        <v>0.01</v>
+      <c r="W269" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X269">
         <v>100000</v>
@@ -31542,8 +31543,8 @@
       <c r="V283">
         <v>38</v>
       </c>
-      <c r="W283">
-        <v>0.05</v>
+      <c r="W283" s="4">
+        <v>0.01</v>
       </c>
       <c r="X283">
         <v>150000</v>
@@ -31646,8 +31647,8 @@
       <c r="V284">
         <v>38</v>
       </c>
-      <c r="W284">
-        <v>0.02</v>
+      <c r="W284" s="4">
+        <v>1.8448275862068958E-2</v>
       </c>
       <c r="X284">
         <v>300000</v>
@@ -31750,8 +31751,8 @@
       <c r="V285">
         <v>39</v>
       </c>
-      <c r="W285">
-        <v>0.03</v>
+      <c r="W285" s="4">
+        <v>2.6896551724137921E-2</v>
       </c>
       <c r="X285">
         <v>500000</v>
@@ -31854,8 +31855,8 @@
       <c r="V286">
         <v>39</v>
       </c>
-      <c r="W286">
-        <v>0.03</v>
+      <c r="W286" s="4">
+        <v>3.5344827586206877E-2</v>
       </c>
       <c r="X286">
         <v>650000</v>
@@ -31958,8 +31959,8 @@
       <c r="V287">
         <v>40</v>
       </c>
-      <c r="W287">
-        <v>0.03</v>
+      <c r="W287" s="4">
+        <v>4.379310344827584E-2</v>
       </c>
       <c r="X287">
         <v>750000</v>
@@ -32062,8 +32063,8 @@
       <c r="V288">
         <v>40</v>
       </c>
-      <c r="W288">
-        <v>0.05</v>
+      <c r="W288" s="4">
+        <v>5.2241379310344803E-2</v>
       </c>
       <c r="X288">
         <v>850000</v>
@@ -32166,8 +32167,8 @@
       <c r="V289">
         <v>40</v>
       </c>
-      <c r="W289">
-        <v>0.1</v>
+      <c r="W289" s="4">
+        <v>6.0689655172413759E-2</v>
       </c>
       <c r="X289">
         <v>900000</v>
@@ -32270,8 +32271,8 @@
       <c r="V290">
         <v>41</v>
       </c>
-      <c r="W290">
-        <v>0.05</v>
+      <c r="W290" s="4">
+        <v>6.9137931034482708E-2</v>
       </c>
       <c r="X290">
         <v>1000000</v>
@@ -32374,8 +32375,8 @@
       <c r="V291">
         <v>41</v>
       </c>
-      <c r="W291">
-        <v>0.09</v>
+      <c r="W291" s="4">
+        <v>7.7586206896551671E-2</v>
       </c>
       <c r="X291">
         <v>1500000</v>
@@ -32478,8 +32479,8 @@
       <c r="V292">
         <v>42</v>
       </c>
-      <c r="W292">
-        <v>0.05</v>
+      <c r="W292" s="4">
+        <v>8.6034482758620634E-2</v>
       </c>
       <c r="X292">
         <v>1800000</v>
@@ -32582,8 +32583,8 @@
       <c r="V293">
         <v>42</v>
       </c>
-      <c r="W293">
-        <v>0.05</v>
+      <c r="W293" s="4">
+        <v>9.4482758620689597E-2</v>
       </c>
       <c r="X293">
         <v>2500000</v>
@@ -32686,8 +32687,8 @@
       <c r="V294">
         <v>43</v>
       </c>
-      <c r="W294">
-        <v>0.1</v>
+      <c r="W294" s="4">
+        <v>0.10293103448275855</v>
       </c>
       <c r="X294">
         <v>2750000</v>
@@ -32790,8 +32791,8 @@
       <c r="V295">
         <v>43</v>
       </c>
-      <c r="W295">
-        <v>0.01</v>
+      <c r="W295" s="4">
+        <v>0.11137931034482751</v>
       </c>
       <c r="X295">
         <v>3000000</v>
@@ -32894,8 +32895,8 @@
       <c r="V296">
         <v>44</v>
       </c>
-      <c r="W296">
-        <v>0.01</v>
+      <c r="W296" s="4">
+        <v>0.11982758620689647</v>
       </c>
       <c r="X296">
         <v>3800000</v>
@@ -32998,8 +32999,8 @@
       <c r="V297">
         <v>44</v>
       </c>
-      <c r="W297">
-        <v>0.05</v>
+      <c r="W297" s="4">
+        <v>0.12827586206896543</v>
       </c>
       <c r="X297">
         <v>4120000</v>
@@ -33102,8 +33103,8 @@
       <c r="V298">
         <v>45</v>
       </c>
-      <c r="W298">
-        <v>0.04</v>
+      <c r="W298" s="4">
+        <v>0.13672413793103441</v>
       </c>
       <c r="X298">
         <v>4570000</v>
@@ -33206,8 +33207,8 @@
       <c r="V299">
         <v>45</v>
       </c>
-      <c r="W299">
-        <v>0.05</v>
+      <c r="W299" s="4">
+        <v>0.14517241379310336</v>
       </c>
       <c r="X299">
         <v>5020000</v>
@@ -33310,8 +33311,8 @@
       <c r="V300">
         <v>45</v>
       </c>
-      <c r="W300">
-        <v>0.05</v>
+      <c r="W300" s="4">
+        <v>0.15362068965517231</v>
       </c>
       <c r="X300">
         <v>5470000</v>
@@ -33414,8 +33415,8 @@
       <c r="V301">
         <v>46</v>
       </c>
-      <c r="W301">
-        <v>0.02</v>
+      <c r="W301" s="4">
+        <v>0.16206896551724129</v>
       </c>
       <c r="X301">
         <v>5920000</v>
@@ -33518,8 +33519,8 @@
       <c r="V302">
         <v>46</v>
       </c>
-      <c r="W302">
-        <v>0.04</v>
+      <c r="W302" s="4">
+        <v>0.17051724137931024</v>
       </c>
       <c r="X302">
         <v>6370000</v>
@@ -33622,8 +33623,8 @@
       <c r="V303">
         <v>47</v>
       </c>
-      <c r="W303">
-        <v>0.08</v>
+      <c r="W303" s="4">
+        <v>0.17896551724137921</v>
       </c>
       <c r="X303">
         <v>6820000</v>
@@ -33726,8 +33727,8 @@
       <c r="V304">
         <v>47</v>
       </c>
-      <c r="W304">
-        <v>0.01</v>
+      <c r="W304" s="4">
+        <v>0.18741379310344816</v>
       </c>
       <c r="X304">
         <v>7270000</v>
@@ -33830,8 +33831,8 @@
       <c r="V305">
         <v>48</v>
       </c>
-      <c r="W305">
-        <v>0.04</v>
+      <c r="W305" s="4">
+        <v>0.19586206896551711</v>
       </c>
       <c r="X305">
         <v>7720000</v>
@@ -33934,8 +33935,8 @@
       <c r="V306">
         <v>48</v>
       </c>
-      <c r="W306">
-        <v>0.02</v>
+      <c r="W306" s="4">
+        <v>0.20431034482758609</v>
       </c>
       <c r="X306">
         <v>8170000</v>
@@ -34038,8 +34039,8 @@
       <c r="V307">
         <v>49</v>
       </c>
-      <c r="W307">
-        <v>0.05</v>
+      <c r="W307" s="4">
+        <v>0.21275862068965504</v>
       </c>
       <c r="X307">
         <v>8620000</v>
@@ -34142,8 +34143,8 @@
       <c r="V308">
         <v>49</v>
       </c>
-      <c r="W308">
-        <v>0.01</v>
+      <c r="W308" s="4">
+        <v>0.22120689655172399</v>
       </c>
       <c r="X308">
         <v>9070000</v>
@@ -34246,8 +34247,8 @@
       <c r="V309">
         <v>50</v>
       </c>
-      <c r="W309">
-        <v>0.02</v>
+      <c r="W309" s="4">
+        <v>0.22965517241379296</v>
       </c>
       <c r="X309">
         <v>9520000</v>
@@ -34350,8 +34351,8 @@
       <c r="V310">
         <v>50</v>
       </c>
-      <c r="W310">
-        <v>0.04</v>
+      <c r="W310" s="4">
+        <v>0.23810344827586191</v>
       </c>
       <c r="X310">
         <v>9970000</v>
@@ -34454,8 +34455,8 @@
       <c r="V311">
         <v>50</v>
       </c>
-      <c r="W311">
-        <v>0.01</v>
+      <c r="W311" s="4">
+        <v>0.24655172413793086</v>
       </c>
       <c r="X311">
         <v>10420000</v>
@@ -34558,8 +34559,8 @@
       <c r="V312">
         <v>51</v>
       </c>
-      <c r="W312">
-        <v>0.04</v>
+      <c r="W312" s="4">
+        <v>0.25499999999999984</v>
       </c>
       <c r="X312">
         <v>10870000</v>
@@ -34662,8 +34663,8 @@
       <c r="V313">
         <v>51</v>
       </c>
-      <c r="W313">
-        <v>0.03</v>
+      <c r="W313" s="4">
+        <v>0.26344827586206881</v>
       </c>
       <c r="X313">
         <v>11320000</v>
@@ -34766,8 +34767,8 @@
       <c r="V314">
         <v>52</v>
       </c>
-      <c r="W314">
-        <v>0.03</v>
+      <c r="W314" s="4">
+        <v>0.27189655172413774</v>
       </c>
       <c r="X314">
         <v>11770000</v>
@@ -34870,8 +34871,8 @@
       <c r="V315">
         <v>52</v>
       </c>
-      <c r="W315">
-        <v>0.05</v>
+      <c r="W315" s="4">
+        <v>0.28034482758620671</v>
       </c>
       <c r="X315">
         <v>12220000</v>
@@ -34974,8 +34975,8 @@
       <c r="V316">
         <v>53</v>
       </c>
-      <c r="W316">
-        <v>0.06</v>
+      <c r="W316" s="4">
+        <v>0.28879310344827569</v>
       </c>
       <c r="X316">
         <v>12670000</v>
@@ -35078,8 +35079,8 @@
       <c r="V317">
         <v>53</v>
       </c>
-      <c r="W317">
-        <v>0.01</v>
+      <c r="W317" s="4">
+        <v>0.29724137931034461</v>
       </c>
       <c r="X317">
         <v>13120000</v>
@@ -35182,8 +35183,8 @@
       <c r="V318">
         <v>54</v>
       </c>
-      <c r="W318">
-        <v>0.01</v>
+      <c r="W318" s="4">
+        <v>0.30568965517241359</v>
       </c>
       <c r="X318">
         <v>13570000</v>
@@ -35286,8 +35287,8 @@
       <c r="V319">
         <v>54</v>
       </c>
-      <c r="W319">
-        <v>0.04</v>
+      <c r="W319" s="4">
+        <v>0.31413793103448256</v>
       </c>
       <c r="X319">
         <v>14020000</v>
@@ -35390,8 +35391,8 @@
       <c r="V320">
         <v>55</v>
       </c>
-      <c r="W320">
-        <v>0.05</v>
+      <c r="W320" s="4">
+        <v>0.32258620689655149</v>
       </c>
       <c r="X320">
         <v>14470000</v>
@@ -35494,8 +35495,8 @@
       <c r="V321">
         <v>55</v>
       </c>
-      <c r="W321">
-        <v>0.05</v>
+      <c r="W321" s="4">
+        <v>0.33103448275862046</v>
       </c>
       <c r="X321">
         <v>14920000</v>
@@ -35598,8 +35599,8 @@
       <c r="V322">
         <v>55</v>
       </c>
-      <c r="W322">
-        <v>0.02</v>
+      <c r="W322" s="4">
+        <v>0.33948275862068944</v>
       </c>
       <c r="X322">
         <v>15370000</v>
@@ -35702,8 +35703,8 @@
       <c r="V323">
         <v>56</v>
       </c>
-      <c r="W323">
-        <v>0.04</v>
+      <c r="W323" s="4">
+        <v>0.34793103448275842</v>
       </c>
       <c r="X323">
         <v>15820000</v>
@@ -35806,8 +35807,8 @@
       <c r="V324">
         <v>56</v>
       </c>
-      <c r="W324">
-        <v>0.08</v>
+      <c r="W324" s="4">
+        <v>0.35637931034482734</v>
       </c>
       <c r="X324">
         <v>16270000</v>
@@ -35910,8 +35911,8 @@
       <c r="V325">
         <v>57</v>
       </c>
-      <c r="W325">
-        <v>0.01</v>
+      <c r="W325" s="4">
+        <v>0.36482758620689631</v>
       </c>
       <c r="X325">
         <v>16720000</v>
@@ -36014,8 +36015,8 @@
       <c r="V326">
         <v>57</v>
       </c>
-      <c r="W326">
-        <v>0.04</v>
+      <c r="W326" s="4">
+        <v>0.37327586206896529</v>
       </c>
       <c r="X326">
         <v>17170000</v>
@@ -36118,8 +36119,8 @@
       <c r="V327">
         <v>58</v>
       </c>
-      <c r="W327">
-        <v>0.02</v>
+      <c r="W327" s="4">
+        <v>0.38172413793103421</v>
       </c>
       <c r="X327">
         <v>17620000</v>
@@ -36222,8 +36223,8 @@
       <c r="V328">
         <v>58</v>
       </c>
-      <c r="W328">
-        <v>0.05</v>
+      <c r="W328" s="4">
+        <v>0.39017241379310319</v>
       </c>
       <c r="X328">
         <v>18070000</v>
@@ -36326,8 +36327,8 @@
       <c r="V329">
         <v>59</v>
       </c>
-      <c r="W329">
-        <v>0.01</v>
+      <c r="W329" s="4">
+        <v>0.39862068965517217</v>
       </c>
       <c r="X329">
         <v>18520000</v>
@@ -36430,8 +36431,8 @@
       <c r="V330">
         <v>59</v>
       </c>
-      <c r="W330">
-        <v>0.02</v>
+      <c r="W330" s="4">
+        <v>0.40706896551724109</v>
       </c>
       <c r="X330">
         <v>18970000</v>
@@ -36534,8 +36535,8 @@
       <c r="V331">
         <v>60</v>
       </c>
-      <c r="W331">
-        <v>0.04</v>
+      <c r="W331" s="4">
+        <v>0.41551724137931006</v>
       </c>
       <c r="X331">
         <v>19420000</v>
@@ -36638,8 +36639,8 @@
       <c r="V332">
         <v>60</v>
       </c>
-      <c r="W332">
-        <v>0.01</v>
+      <c r="W332" s="4">
+        <v>0.42396551724137904</v>
       </c>
       <c r="X332">
         <v>19870000</v>
@@ -36745,8 +36746,8 @@
       <c r="V333">
         <v>8</v>
       </c>
-      <c r="W333">
-        <v>1E-3</v>
+      <c r="W333" s="4">
+        <v>0.43241379310344796</v>
       </c>
       <c r="X333">
         <v>100000000</v>
@@ -36852,8 +36853,8 @@
       <c r="V334">
         <v>9.9523809523809508</v>
       </c>
-      <c r="W334">
-        <v>1E-3</v>
+      <c r="W334" s="4">
+        <v>0.44086206896551694</v>
       </c>
       <c r="X334">
         <v>150000000</v>
@@ -36959,8 +36960,8 @@
       <c r="V335">
         <v>11.9047619047619</v>
       </c>
-      <c r="W335">
-        <v>1E-3</v>
+      <c r="W335" s="4">
+        <v>0.44931034482758592</v>
       </c>
       <c r="X335">
         <v>180000000</v>
@@ -37066,8 +37067,8 @@
       <c r="V336">
         <v>13.857142857142851</v>
       </c>
-      <c r="W336">
-        <v>1E-3</v>
+      <c r="W336" s="4">
+        <v>0.45775862068965484</v>
       </c>
       <c r="X336">
         <v>190000000</v>
@@ -37173,8 +37174,8 @@
       <c r="V337">
         <v>15.8095238095238</v>
       </c>
-      <c r="W337">
-        <v>1E-3</v>
+      <c r="W337" s="4">
+        <v>0.46620689655172382</v>
       </c>
       <c r="X337">
         <v>200000000</v>
@@ -37280,8 +37281,8 @@
       <c r="V338">
         <v>17.761904761904752</v>
       </c>
-      <c r="W338">
-        <v>1E-3</v>
+      <c r="W338" s="4">
+        <v>0.47465517241379279</v>
       </c>
       <c r="X338">
         <v>210000000</v>
@@ -37387,8 +37388,8 @@
       <c r="V339">
         <v>19.714285714285701</v>
       </c>
-      <c r="W339">
-        <v>1E-3</v>
+      <c r="W339" s="4">
+        <v>0.48310344827586171</v>
       </c>
       <c r="X339">
         <v>220000000</v>
@@ -37494,8 +37495,8 @@
       <c r="V340">
         <v>21.66666666666665</v>
       </c>
-      <c r="W340">
-        <v>1E-3</v>
+      <c r="W340" s="4">
+        <v>0.49155172413793069</v>
       </c>
       <c r="X340">
         <v>230000000</v>
@@ -37601,8 +37602,8 @@
       <c r="V341">
         <v>23.619047619047599</v>
       </c>
-      <c r="W341">
-        <v>1E-3</v>
+      <c r="W341" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X341">
         <v>240000000</v>
@@ -37708,8 +37709,8 @@
       <c r="V342">
         <v>25.571428571428552</v>
       </c>
-      <c r="W342">
-        <v>1E-3</v>
+      <c r="W342" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X342">
         <v>250000000</v>
@@ -37815,8 +37816,8 @@
       <c r="V343">
         <v>27.523809523809501</v>
       </c>
-      <c r="W343">
-        <v>1E-3</v>
+      <c r="W343" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X343">
         <v>260000000</v>
@@ -37922,8 +37923,8 @@
       <c r="V344">
         <v>29.47619047619045</v>
       </c>
-      <c r="W344">
-        <v>1E-3</v>
+      <c r="W344" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X344">
         <v>270000000</v>
@@ -38029,8 +38030,8 @@
       <c r="V345">
         <v>31.428571428571402</v>
       </c>
-      <c r="W345">
-        <v>1E-3</v>
+      <c r="W345" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X345">
         <v>280000000</v>
@@ -38136,8 +38137,8 @@
       <c r="V346">
         <v>33.380952380952351</v>
       </c>
-      <c r="W346">
-        <v>1E-3</v>
+      <c r="W346" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X346">
         <v>290000000</v>
@@ -38243,8 +38244,8 @@
       <c r="V347">
         <v>35.3333333333333</v>
       </c>
-      <c r="W347">
-        <v>1E-3</v>
+      <c r="W347" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X347">
         <v>300000000</v>
@@ -38350,8 +38351,8 @@
       <c r="V348">
         <v>37.285714285714249</v>
       </c>
-      <c r="W348">
-        <v>1E-3</v>
+      <c r="W348" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X348">
         <v>310000000</v>
@@ -38457,8 +38458,8 @@
       <c r="V349">
         <v>39.238095238095198</v>
       </c>
-      <c r="W349">
-        <v>1E-3</v>
+      <c r="W349" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X349">
         <v>320000000</v>
@@ -38564,8 +38565,8 @@
       <c r="V350">
         <v>41.190476190476154</v>
       </c>
-      <c r="W350">
-        <v>1E-3</v>
+      <c r="W350" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X350">
         <v>330000000</v>
@@ -38671,8 +38672,8 @@
       <c r="V351">
         <v>43.142857142857103</v>
       </c>
-      <c r="W351">
-        <v>1E-3</v>
+      <c r="W351" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X351">
         <v>340000000</v>
@@ -38778,8 +38779,8 @@
       <c r="V352">
         <v>45.095238095238052</v>
       </c>
-      <c r="W352">
-        <v>1E-3</v>
+      <c r="W352" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X352">
         <v>350000000</v>
@@ -38885,8 +38886,8 @@
       <c r="V353">
         <v>47.047619047619001</v>
       </c>
-      <c r="W353">
-        <v>1E-3</v>
+      <c r="W353" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X353">
         <v>360000000</v>
@@ -38992,8 +38993,8 @@
       <c r="V354">
         <v>48.99999999999995</v>
       </c>
-      <c r="W354">
-        <v>1E-3</v>
+      <c r="W354" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X354">
         <v>370000000</v>
@@ -39099,8 +39100,8 @@
       <c r="V355">
         <v>50.952380952380899</v>
       </c>
-      <c r="W355">
-        <v>1E-3</v>
+      <c r="W355" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X355">
         <v>380000000</v>
@@ -39206,8 +39207,8 @@
       <c r="V356">
         <v>52.904761904761855</v>
       </c>
-      <c r="W356">
-        <v>1E-3</v>
+      <c r="W356" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X356">
         <v>390000000</v>
@@ -39313,8 +39314,8 @@
       <c r="V357">
         <v>54.857142857142804</v>
       </c>
-      <c r="W357">
-        <v>1E-3</v>
+      <c r="W357" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X357">
         <v>400000000</v>
@@ -39420,8 +39421,8 @@
       <c r="V358">
         <v>56.809523809523753</v>
       </c>
-      <c r="W358">
-        <v>1E-3</v>
+      <c r="W358" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X358">
         <v>410000000</v>
@@ -39527,8 +39528,8 @@
       <c r="V359">
         <v>58.761904761904702</v>
       </c>
-      <c r="W359">
-        <v>1E-3</v>
+      <c r="W359" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X359">
         <v>420000000</v>
@@ -39634,8 +39635,8 @@
       <c r="V360">
         <v>60.714285714285651</v>
       </c>
-      <c r="W360">
-        <v>1E-3</v>
+      <c r="W360" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X360">
         <v>430000000</v>
@@ -39741,8 +39742,8 @@
       <c r="V361">
         <v>62.6666666666666</v>
       </c>
-      <c r="W361">
-        <v>1E-3</v>
+      <c r="W361" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X361">
         <v>440000000</v>
@@ -39848,8 +39849,8 @@
       <c r="V362">
         <v>64.619047619047564</v>
       </c>
-      <c r="W362">
-        <v>1E-3</v>
+      <c r="W362" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X362">
         <v>450000000</v>
@@ -39955,8 +39956,8 @@
       <c r="V363">
         <v>66.571428571428498</v>
       </c>
-      <c r="W363">
-        <v>1E-3</v>
+      <c r="W363" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X363">
         <v>470000000</v>
@@ -40062,8 +40063,8 @@
       <c r="V364">
         <v>68.523809523809462</v>
       </c>
-      <c r="W364">
-        <v>1E-3</v>
+      <c r="W364" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X364">
         <v>480000000</v>
@@ -40169,8 +40170,8 @@
       <c r="V365">
         <v>70.476190476190396</v>
       </c>
-      <c r="W365">
-        <v>1E-3</v>
+      <c r="W365" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X365">
         <v>490000000</v>
@@ -40276,8 +40277,8 @@
       <c r="V366">
         <v>72.42857142857136</v>
       </c>
-      <c r="W366">
-        <v>1E-3</v>
+      <c r="W366" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X366">
         <v>500000000</v>
@@ -40383,8 +40384,8 @@
       <c r="V367">
         <v>74.380952380952309</v>
       </c>
-      <c r="W367">
-        <v>1E-3</v>
+      <c r="W367" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X367">
         <v>510000000</v>
@@ -40490,8 +40491,8 @@
       <c r="V368">
         <v>76.333333333333258</v>
       </c>
-      <c r="W368">
-        <v>1E-3</v>
+      <c r="W368" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X368">
         <v>520000000</v>
@@ -40597,8 +40598,8 @@
       <c r="V369">
         <v>78.285714285714207</v>
       </c>
-      <c r="W369">
-        <v>1E-3</v>
+      <c r="W369" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X369">
         <v>530000000</v>
@@ -40704,8 +40705,8 @@
       <c r="V370">
         <v>80.238095238095156</v>
       </c>
-      <c r="W370">
-        <v>1E-3</v>
+      <c r="W370" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X370">
         <v>540000000</v>
@@ -40811,8 +40812,8 @@
       <c r="V371">
         <v>82.190476190476105</v>
       </c>
-      <c r="W371">
-        <v>1E-3</v>
+      <c r="W371" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X371">
         <v>550000000</v>
@@ -40918,8 +40919,8 @@
       <c r="V372">
         <v>84.142857142857054</v>
       </c>
-      <c r="W372">
-        <v>1E-3</v>
+      <c r="W372" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X372">
         <v>560000000</v>
@@ -41025,8 +41026,8 @@
       <c r="V373">
         <v>86.095238095238003</v>
       </c>
-      <c r="W373">
-        <v>1E-3</v>
+      <c r="W373" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X373">
         <v>570000000</v>
@@ -41132,8 +41133,8 @@
       <c r="V374">
         <v>88.047619047618952</v>
       </c>
-      <c r="W374">
-        <v>1E-3</v>
+      <c r="W374" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X374">
         <v>580000000</v>
@@ -41239,8 +41240,8 @@
       <c r="V375">
         <v>89.999999999999901</v>
       </c>
-      <c r="W375">
-        <v>1E-3</v>
+      <c r="W375" s="4">
+        <v>0.49999999999999967</v>
       </c>
       <c r="X375">
         <v>460000000</v>

</xml_diff>

<commit_message>
More abstractions. Now we need
- Player should be able to reduce other players resistances, such as
  spell evasion and affix damage reduction.

- Player/Monster can counter and vice versa.
</commit_message>
<xml_diff>
--- a/resources/data-imports/monsters.xlsx
+++ b/resources/data-imports/monsters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E93AC88-C380-E846-AC95-885CE0CC08CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F2F5A2-2C17-3A4A-BB12-B0BE7C2C3491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2360,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS391"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W341" sqref="W341:W375"/>
+    <sheetView tabSelected="1" topLeftCell="AG319" workbookViewId="0">
+      <selection activeCell="AN323" sqref="AN323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36681,6 +36681,18 @@
       <c r="AK332">
         <v>0.05</v>
       </c>
+      <c r="AL332">
+        <v>0.05</v>
+      </c>
+      <c r="AM332">
+        <v>0.05</v>
+      </c>
+      <c r="AN332">
+        <v>0.05</v>
+      </c>
+      <c r="AO332">
+        <v>0.05</v>
+      </c>
       <c r="AP332">
         <v>1</v>
       </c>
@@ -36771,21 +36783,33 @@
         <v>1</v>
       </c>
       <c r="AF333">
-        <v>1.6</v>
+        <v>0.08</v>
       </c>
       <c r="AG333">
-        <v>1.5</v>
+        <v>0.08</v>
       </c>
       <c r="AH333">
-        <v>1.8</v>
+        <v>0.08</v>
       </c>
       <c r="AI333">
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="AJ333">
-        <v>2.1</v>
+        <v>0.08</v>
       </c>
       <c r="AK333">
+        <v>0.08</v>
+      </c>
+      <c r="AL333">
+        <v>0.08</v>
+      </c>
+      <c r="AM333">
+        <v>0.08</v>
+      </c>
+      <c r="AN333">
+        <v>0.08</v>
+      </c>
+      <c r="AO333">
         <v>0.08</v>
       </c>
       <c r="AP333">
@@ -36878,21 +36902,33 @@
         <v>1</v>
       </c>
       <c r="AF334">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="AG334">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="AH334">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="AI334">
-        <v>2.2000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="AJ334">
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="AK334">
+        <v>0.1</v>
+      </c>
+      <c r="AL334">
+        <v>0.1</v>
+      </c>
+      <c r="AM334">
+        <v>0.1</v>
+      </c>
+      <c r="AN334">
+        <v>0.1</v>
+      </c>
+      <c r="AO334">
         <v>0.1</v>
       </c>
       <c r="AP334">
@@ -36985,21 +37021,33 @@
         <v>1</v>
       </c>
       <c r="AF335">
-        <v>2</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="AG335">
-        <v>2.1</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="AH335">
-        <v>2.2000000000000002</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="AI335">
-        <v>2.4</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="AJ335">
-        <v>2.9</v>
+        <v>0.12670000000000001</v>
       </c>
       <c r="AK335">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="AL335">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="AM335">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="AN335">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="AO335">
         <v>0.12670000000000001</v>
       </c>
       <c r="AP335">
@@ -37092,21 +37140,33 @@
         <v>1</v>
       </c>
       <c r="AF336">
-        <v>2.2000000000000002</v>
+        <v>0.1517</v>
       </c>
       <c r="AG336">
-        <v>2.4</v>
+        <v>0.1517</v>
       </c>
       <c r="AH336">
-        <v>2.4</v>
+        <v>0.1517</v>
       </c>
       <c r="AI336">
-        <v>2.6</v>
+        <v>0.1517</v>
       </c>
       <c r="AJ336">
-        <v>3.3</v>
+        <v>0.1517</v>
       </c>
       <c r="AK336">
+        <v>0.1517</v>
+      </c>
+      <c r="AL336">
+        <v>0.1517</v>
+      </c>
+      <c r="AM336">
+        <v>0.1517</v>
+      </c>
+      <c r="AN336">
+        <v>0.1517</v>
+      </c>
+      <c r="AO336">
         <v>0.1517</v>
       </c>
       <c r="AP336">
@@ -37199,21 +37259,33 @@
         <v>1</v>
       </c>
       <c r="AF337">
-        <v>2.4</v>
+        <v>0.1767</v>
       </c>
       <c r="AG337">
-        <v>2.7</v>
+        <v>0.1767</v>
       </c>
       <c r="AH337">
-        <v>2.6</v>
+        <v>0.1767</v>
       </c>
       <c r="AI337">
-        <v>2.8</v>
+        <v>0.1767</v>
       </c>
       <c r="AJ337">
-        <v>3.7</v>
+        <v>0.1767</v>
       </c>
       <c r="AK337">
+        <v>0.1767</v>
+      </c>
+      <c r="AL337">
+        <v>0.1767</v>
+      </c>
+      <c r="AM337">
+        <v>0.1767</v>
+      </c>
+      <c r="AN337">
+        <v>0.1767</v>
+      </c>
+      <c r="AO337">
         <v>0.1767</v>
       </c>
       <c r="AP337">
@@ -37306,21 +37378,33 @@
         <v>1</v>
       </c>
       <c r="AF338">
-        <v>2.6</v>
+        <v>0.20169999999999999</v>
       </c>
       <c r="AG338">
-        <v>3</v>
+        <v>0.20169999999999999</v>
       </c>
       <c r="AH338">
-        <v>2.8</v>
+        <v>0.20169999999999999</v>
       </c>
       <c r="AI338">
-        <v>3</v>
+        <v>0.20169999999999999</v>
       </c>
       <c r="AJ338">
-        <v>4.0999999999999996</v>
+        <v>0.20169999999999999</v>
       </c>
       <c r="AK338">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="AL338">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="AM338">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="AN338">
+        <v>0.20169999999999999</v>
+      </c>
+      <c r="AO338">
         <v>0.20169999999999999</v>
       </c>
       <c r="AP338">
@@ -37413,21 +37497,33 @@
         <v>1</v>
       </c>
       <c r="AF339">
-        <v>2.8</v>
+        <v>0.22670000000000001</v>
       </c>
       <c r="AG339">
-        <v>3.3</v>
+        <v>0.22670000000000001</v>
       </c>
       <c r="AH339">
-        <v>3</v>
+        <v>0.22670000000000001</v>
       </c>
       <c r="AI339">
-        <v>3.2</v>
+        <v>0.22670000000000001</v>
       </c>
       <c r="AJ339">
-        <v>4.5</v>
+        <v>0.22670000000000001</v>
       </c>
       <c r="AK339">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="AL339">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="AM339">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="AN339">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="AO339">
         <v>0.22670000000000001</v>
       </c>
       <c r="AP339">
@@ -37520,21 +37616,33 @@
         <v>1</v>
       </c>
       <c r="AF340">
-        <v>3</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="AG340">
-        <v>3.6</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="AH340">
-        <v>3.2</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="AI340">
-        <v>3.4</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="AJ340">
-        <v>4.9000000000000004</v>
+        <v>0.25169999999999998</v>
       </c>
       <c r="AK340">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="AL340">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="AM340">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="AN340">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="AO340">
         <v>0.25169999999999998</v>
       </c>
       <c r="AP340">
@@ -37627,21 +37735,33 @@
         <v>1</v>
       </c>
       <c r="AF341">
-        <v>3.2</v>
+        <v>0.2767</v>
       </c>
       <c r="AG341">
-        <v>3.9</v>
+        <v>0.2767</v>
       </c>
       <c r="AH341">
-        <v>3.4</v>
+        <v>0.2767</v>
       </c>
       <c r="AI341">
-        <v>3.6</v>
+        <v>0.2767</v>
       </c>
       <c r="AJ341">
-        <v>5.3</v>
+        <v>0.2767</v>
       </c>
       <c r="AK341">
+        <v>0.2767</v>
+      </c>
+      <c r="AL341">
+        <v>0.2767</v>
+      </c>
+      <c r="AM341">
+        <v>0.2767</v>
+      </c>
+      <c r="AN341">
+        <v>0.2767</v>
+      </c>
+      <c r="AO341">
         <v>0.2767</v>
       </c>
       <c r="AP341">
@@ -37734,21 +37854,33 @@
         <v>1</v>
       </c>
       <c r="AF342">
-        <v>3.4</v>
+        <v>0.30170000000000002</v>
       </c>
       <c r="AG342">
-        <v>4.2</v>
+        <v>0.30170000000000002</v>
       </c>
       <c r="AH342">
-        <v>3.6</v>
+        <v>0.30170000000000002</v>
       </c>
       <c r="AI342">
-        <v>3.8</v>
+        <v>0.30170000000000002</v>
       </c>
       <c r="AJ342">
-        <v>5.7</v>
+        <v>0.30170000000000002</v>
       </c>
       <c r="AK342">
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="AL342">
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="AM342">
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="AN342">
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="AO342">
         <v>0.30170000000000002</v>
       </c>
       <c r="AP342">
@@ -37841,21 +37973,33 @@
         <v>1</v>
       </c>
       <c r="AF343">
-        <v>3.6</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="AG343">
-        <v>4.5</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="AH343">
-        <v>3.8</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="AI343">
-        <v>4</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="AJ343">
-        <v>6.1</v>
+        <v>0.32669999999999999</v>
       </c>
       <c r="AK343">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="AL343">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="AM343">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="AN343">
+        <v>0.32669999999999999</v>
+      </c>
+      <c r="AO343">
         <v>0.32669999999999999</v>
       </c>
       <c r="AP343">
@@ -37948,21 +38092,33 @@
         <v>1</v>
       </c>
       <c r="AF344">
-        <v>3.8</v>
+        <v>0.35170000000000001</v>
       </c>
       <c r="AG344">
-        <v>4.8</v>
+        <v>0.35170000000000001</v>
       </c>
       <c r="AH344">
-        <v>4</v>
+        <v>0.35170000000000001</v>
       </c>
       <c r="AI344">
-        <v>4.2</v>
+        <v>0.35170000000000001</v>
       </c>
       <c r="AJ344">
-        <v>6.5</v>
+        <v>0.35170000000000001</v>
       </c>
       <c r="AK344">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="AL344">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="AM344">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="AN344">
+        <v>0.35170000000000001</v>
+      </c>
+      <c r="AO344">
         <v>0.35170000000000001</v>
       </c>
       <c r="AP344">
@@ -38055,21 +38211,33 @@
         <v>1</v>
       </c>
       <c r="AF345">
-        <v>4</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="AG345">
-        <v>5.0999999999999996</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="AH345">
-        <v>4.2</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="AI345">
-        <v>4.4000000000000004</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="AJ345">
-        <v>6.9</v>
+        <v>0.37669999999999998</v>
       </c>
       <c r="AK345">
+        <v>0.37669999999999998</v>
+      </c>
+      <c r="AL345">
+        <v>0.37669999999999998</v>
+      </c>
+      <c r="AM345">
+        <v>0.37669999999999998</v>
+      </c>
+      <c r="AN345">
+        <v>0.37669999999999998</v>
+      </c>
+      <c r="AO345">
         <v>0.37669999999999998</v>
       </c>
       <c r="AP345">
@@ -38162,21 +38330,33 @@
         <v>1</v>
       </c>
       <c r="AF346">
-        <v>4.2</v>
+        <v>0.4017</v>
       </c>
       <c r="AG346">
-        <v>5.4</v>
+        <v>0.4017</v>
       </c>
       <c r="AH346">
-        <v>4.4000000000000004</v>
+        <v>0.4017</v>
       </c>
       <c r="AI346">
-        <v>4.5999999999999996</v>
+        <v>0.4017</v>
       </c>
       <c r="AJ346">
-        <v>7.3</v>
+        <v>0.4017</v>
       </c>
       <c r="AK346">
+        <v>0.4017</v>
+      </c>
+      <c r="AL346">
+        <v>0.4017</v>
+      </c>
+      <c r="AM346">
+        <v>0.4017</v>
+      </c>
+      <c r="AN346">
+        <v>0.4017</v>
+      </c>
+      <c r="AO346">
         <v>0.4017</v>
       </c>
       <c r="AP346">
@@ -38269,21 +38449,33 @@
         <v>1</v>
       </c>
       <c r="AF347">
-        <v>4.4000000000000004</v>
+        <v>0.42670000000000002</v>
       </c>
       <c r="AG347">
-        <v>5.7</v>
+        <v>0.42670000000000002</v>
       </c>
       <c r="AH347">
-        <v>4.5999999999999996</v>
+        <v>0.42670000000000002</v>
       </c>
       <c r="AI347">
-        <v>4.8</v>
+        <v>0.42670000000000002</v>
       </c>
       <c r="AJ347">
-        <v>7.7</v>
+        <v>0.42670000000000002</v>
       </c>
       <c r="AK347">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="AL347">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="AM347">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="AN347">
+        <v>0.42670000000000002</v>
+      </c>
+      <c r="AO347">
         <v>0.42670000000000002</v>
       </c>
       <c r="AP347">
@@ -38376,21 +38568,33 @@
         <v>1</v>
       </c>
       <c r="AF348">
-        <v>4.5999999999999996</v>
+        <v>0.45169999999999999</v>
       </c>
       <c r="AG348">
-        <v>6</v>
+        <v>0.45169999999999999</v>
       </c>
       <c r="AH348">
-        <v>4.8</v>
+        <v>0.45169999999999999</v>
       </c>
       <c r="AI348">
-        <v>5</v>
+        <v>0.45169999999999999</v>
       </c>
       <c r="AJ348">
-        <v>8.1</v>
+        <v>0.45169999999999999</v>
       </c>
       <c r="AK348">
+        <v>0.45169999999999999</v>
+      </c>
+      <c r="AL348">
+        <v>0.45169999999999999</v>
+      </c>
+      <c r="AM348">
+        <v>0.45169999999999999</v>
+      </c>
+      <c r="AN348">
+        <v>0.45169999999999999</v>
+      </c>
+      <c r="AO348">
         <v>0.45169999999999999</v>
       </c>
       <c r="AP348">
@@ -38483,21 +38687,33 @@
         <v>1</v>
       </c>
       <c r="AF349">
-        <v>4.8</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="AG349">
-        <v>6.3</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="AH349">
-        <v>5</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="AI349">
-        <v>5.2</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="AJ349">
-        <v>8.5</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="AK349">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="AL349">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="AM349">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="AN349">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="AO349">
         <v>0.47670000000000001</v>
       </c>
       <c r="AP349">
@@ -38590,21 +38806,33 @@
         <v>1</v>
       </c>
       <c r="AF350">
-        <v>5</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="AG350">
-        <v>6.6</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="AH350">
-        <v>5.2</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="AI350">
-        <v>5.4</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="AJ350">
-        <v>8.9</v>
+        <v>0.50170000000000003</v>
       </c>
       <c r="AK350">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="AL350">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="AM350">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="AN350">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="AO350">
         <v>0.50170000000000003</v>
       </c>
       <c r="AP350">
@@ -38697,21 +38925,33 @@
         <v>1</v>
       </c>
       <c r="AF351">
-        <v>5.2</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="AG351">
-        <v>6.9</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="AH351">
-        <v>5.4</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="AI351">
-        <v>5.6</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="AJ351">
-        <v>9.3000000000000007</v>
+        <v>0.52669999999999995</v>
       </c>
       <c r="AK351">
+        <v>0.52669999999999995</v>
+      </c>
+      <c r="AL351">
+        <v>0.52669999999999995</v>
+      </c>
+      <c r="AM351">
+        <v>0.52669999999999995</v>
+      </c>
+      <c r="AN351">
+        <v>0.52669999999999995</v>
+      </c>
+      <c r="AO351">
         <v>0.52669999999999995</v>
       </c>
       <c r="AP351">
@@ -38804,21 +39044,33 @@
         <v>1</v>
       </c>
       <c r="AF352">
-        <v>5.4</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="AG352">
-        <v>7.2</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="AH352">
-        <v>5.6</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="AI352">
-        <v>5.8</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="AJ352">
-        <v>9.6999999999999993</v>
+        <v>0.55169999999999997</v>
       </c>
       <c r="AK352">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="AL352">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="AM352">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="AN352">
+        <v>0.55169999999999997</v>
+      </c>
+      <c r="AO352">
         <v>0.55169999999999997</v>
       </c>
       <c r="AP352">
@@ -38911,21 +39163,33 @@
         <v>1</v>
       </c>
       <c r="AF353">
-        <v>5.6</v>
+        <v>0.57669999999999999</v>
       </c>
       <c r="AG353">
-        <v>7.5</v>
+        <v>0.57669999999999999</v>
       </c>
       <c r="AH353">
-        <v>5.8</v>
+        <v>0.57669999999999999</v>
       </c>
       <c r="AI353">
-        <v>6</v>
+        <v>0.57669999999999999</v>
       </c>
       <c r="AJ353">
-        <v>10.1</v>
+        <v>0.57669999999999999</v>
       </c>
       <c r="AK353">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="AL353">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="AM353">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="AN353">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="AO353">
         <v>0.57669999999999999</v>
       </c>
       <c r="AP353">
@@ -39018,21 +39282,33 @@
         <v>1</v>
       </c>
       <c r="AF354">
-        <v>5.8</v>
+        <v>0.60170000000000001</v>
       </c>
       <c r="AG354">
-        <v>7.8</v>
+        <v>0.60170000000000001</v>
       </c>
       <c r="AH354">
-        <v>6</v>
+        <v>0.60170000000000001</v>
       </c>
       <c r="AI354">
-        <v>6.2</v>
+        <v>0.60170000000000001</v>
       </c>
       <c r="AJ354">
-        <v>10.5</v>
+        <v>0.60170000000000001</v>
       </c>
       <c r="AK354">
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="AL354">
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="AM354">
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="AN354">
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="AO354">
         <v>0.60170000000000001</v>
       </c>
       <c r="AP354">
@@ -39125,21 +39401,33 @@
         <v>1</v>
       </c>
       <c r="AF355">
-        <v>6</v>
+        <v>0.62670000000000003</v>
       </c>
       <c r="AG355">
-        <v>8.1</v>
+        <v>0.62670000000000003</v>
       </c>
       <c r="AH355">
-        <v>6.2</v>
+        <v>0.62670000000000003</v>
       </c>
       <c r="AI355">
-        <v>6.4</v>
+        <v>0.62670000000000003</v>
       </c>
       <c r="AJ355">
-        <v>10.9</v>
+        <v>0.62670000000000003</v>
       </c>
       <c r="AK355">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="AL355">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="AM355">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="AN355">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="AO355">
         <v>0.62670000000000003</v>
       </c>
       <c r="AP355">
@@ -39232,21 +39520,33 @@
         <v>1</v>
       </c>
       <c r="AF356">
-        <v>6.2</v>
+        <v>0.65169999999999995</v>
       </c>
       <c r="AG356">
-        <v>8.4</v>
+        <v>0.65169999999999995</v>
       </c>
       <c r="AH356">
-        <v>6.4</v>
+        <v>0.65169999999999995</v>
       </c>
       <c r="AI356">
-        <v>6.6</v>
+        <v>0.65169999999999995</v>
       </c>
       <c r="AJ356">
-        <v>11.3</v>
+        <v>0.65169999999999995</v>
       </c>
       <c r="AK356">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="AL356">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="AM356">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="AN356">
+        <v>0.65169999999999995</v>
+      </c>
+      <c r="AO356">
         <v>0.65169999999999995</v>
       </c>
       <c r="AP356">
@@ -39339,21 +39639,33 @@
         <v>1</v>
       </c>
       <c r="AF357">
-        <v>6.4</v>
+        <v>0.67669999999999997</v>
       </c>
       <c r="AG357">
-        <v>8.6999999999999993</v>
+        <v>0.67669999999999997</v>
       </c>
       <c r="AH357">
-        <v>6.6</v>
+        <v>0.67669999999999997</v>
       </c>
       <c r="AI357">
-        <v>6.8</v>
+        <v>0.67669999999999997</v>
       </c>
       <c r="AJ357">
-        <v>11.7</v>
+        <v>0.67669999999999997</v>
       </c>
       <c r="AK357">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="AL357">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="AM357">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="AN357">
+        <v>0.67669999999999997</v>
+      </c>
+      <c r="AO357">
         <v>0.67669999999999997</v>
       </c>
       <c r="AP357">
@@ -39446,21 +39758,33 @@
         <v>1</v>
       </c>
       <c r="AF358">
-        <v>6.6</v>
+        <v>0.70169999999999999</v>
       </c>
       <c r="AG358">
-        <v>9</v>
+        <v>0.70169999999999999</v>
       </c>
       <c r="AH358">
-        <v>6.8</v>
+        <v>0.70169999999999999</v>
       </c>
       <c r="AI358">
-        <v>7</v>
+        <v>0.70169999999999999</v>
       </c>
       <c r="AJ358">
-        <v>12.1</v>
+        <v>0.70169999999999999</v>
       </c>
       <c r="AK358">
+        <v>0.70169999999999999</v>
+      </c>
+      <c r="AL358">
+        <v>0.70169999999999999</v>
+      </c>
+      <c r="AM358">
+        <v>0.70169999999999999</v>
+      </c>
+      <c r="AN358">
+        <v>0.70169999999999999</v>
+      </c>
+      <c r="AO358">
         <v>0.70169999999999999</v>
       </c>
       <c r="AP358">
@@ -39553,21 +39877,33 @@
         <v>1</v>
       </c>
       <c r="AF359">
-        <v>6.8</v>
+        <v>0.72670000000000001</v>
       </c>
       <c r="AG359">
-        <v>9.3000000000000007</v>
+        <v>0.72670000000000001</v>
       </c>
       <c r="AH359">
-        <v>7</v>
+        <v>0.72670000000000001</v>
       </c>
       <c r="AI359">
-        <v>7.2</v>
+        <v>0.72670000000000001</v>
       </c>
       <c r="AJ359">
-        <v>12.5</v>
+        <v>0.72670000000000001</v>
       </c>
       <c r="AK359">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="AL359">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="AM359">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="AN359">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="AO359">
         <v>0.72670000000000001</v>
       </c>
       <c r="AP359">
@@ -39660,21 +39996,33 @@
         <v>1</v>
       </c>
       <c r="AF360">
-        <v>7</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="AG360">
-        <v>9.6</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="AH360">
-        <v>7.2</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="AI360">
-        <v>7.4</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="AJ360">
-        <v>12.9</v>
+        <v>0.75170000000000003</v>
       </c>
       <c r="AK360">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="AL360">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="AM360">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="AN360">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="AO360">
         <v>0.75170000000000003</v>
       </c>
       <c r="AP360">
@@ -39767,21 +40115,33 @@
         <v>1</v>
       </c>
       <c r="AF361">
-        <v>7.2</v>
+        <v>0.77669999999999995</v>
       </c>
       <c r="AG361">
-        <v>9.9</v>
+        <v>0.77669999999999995</v>
       </c>
       <c r="AH361">
-        <v>7.4</v>
+        <v>0.77669999999999995</v>
       </c>
       <c r="AI361">
-        <v>7.6</v>
+        <v>0.77669999999999995</v>
       </c>
       <c r="AJ361">
-        <v>13.3</v>
+        <v>0.77669999999999995</v>
       </c>
       <c r="AK361">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="AL361">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="AM361">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="AN361">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="AO361">
         <v>0.77669999999999995</v>
       </c>
       <c r="AP361">
@@ -39874,21 +40234,33 @@
         <v>1</v>
       </c>
       <c r="AF362">
-        <v>7.4</v>
+        <v>0.80169999999999997</v>
       </c>
       <c r="AG362">
-        <v>10.199999999999999</v>
+        <v>0.80169999999999997</v>
       </c>
       <c r="AH362">
-        <v>7.6</v>
+        <v>0.80169999999999997</v>
       </c>
       <c r="AI362">
-        <v>7.8</v>
+        <v>0.80169999999999997</v>
       </c>
       <c r="AJ362">
-        <v>13.7</v>
+        <v>0.80169999999999997</v>
       </c>
       <c r="AK362">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="AL362">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="AM362">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="AN362">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="AO362">
         <v>0.80169999999999997</v>
       </c>
       <c r="AP362">
@@ -39981,21 +40353,33 @@
         <v>1</v>
       </c>
       <c r="AF363">
-        <v>7.8</v>
+        <v>0.85170000000000001</v>
       </c>
       <c r="AG363">
-        <v>10.8</v>
+        <v>0.85170000000000001</v>
       </c>
       <c r="AH363">
-        <v>8</v>
+        <v>0.85170000000000001</v>
       </c>
       <c r="AI363">
-        <v>8.1999999999999993</v>
+        <v>0.85170000000000001</v>
       </c>
       <c r="AJ363">
-        <v>14.5</v>
+        <v>0.85170000000000001</v>
       </c>
       <c r="AK363">
+        <v>0.85170000000000001</v>
+      </c>
+      <c r="AL363">
+        <v>0.85170000000000001</v>
+      </c>
+      <c r="AM363">
+        <v>0.85170000000000001</v>
+      </c>
+      <c r="AN363">
+        <v>0.85170000000000001</v>
+      </c>
+      <c r="AO363">
         <v>0.85170000000000001</v>
       </c>
       <c r="AP363">
@@ -40088,21 +40472,33 @@
         <v>1</v>
       </c>
       <c r="AF364">
-        <v>8</v>
+        <v>0.87670000000000003</v>
       </c>
       <c r="AG364">
-        <v>11.1</v>
+        <v>0.87670000000000003</v>
       </c>
       <c r="AH364">
-        <v>8.1999999999999993</v>
+        <v>0.87670000000000003</v>
       </c>
       <c r="AI364">
-        <v>8.4</v>
+        <v>0.87670000000000003</v>
       </c>
       <c r="AJ364">
-        <v>14.9</v>
+        <v>0.87670000000000003</v>
       </c>
       <c r="AK364">
+        <v>0.87670000000000003</v>
+      </c>
+      <c r="AL364">
+        <v>0.87670000000000003</v>
+      </c>
+      <c r="AM364">
+        <v>0.87670000000000003</v>
+      </c>
+      <c r="AN364">
+        <v>0.87670000000000003</v>
+      </c>
+      <c r="AO364">
         <v>0.87670000000000003</v>
       </c>
       <c r="AP364">
@@ -40195,21 +40591,33 @@
         <v>1</v>
       </c>
       <c r="AF365">
-        <v>8.1999999999999993</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="AG365">
-        <v>11.4</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="AH365">
-        <v>8.4</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="AI365">
-        <v>8.6</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="AJ365">
-        <v>15.3</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="AK365">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="AL365">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="AM365">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="AN365">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="AO365">
         <v>0.90169999999999995</v>
       </c>
       <c r="AP365">
@@ -40302,21 +40710,33 @@
         <v>1</v>
       </c>
       <c r="AF366">
-        <v>8.4</v>
+        <v>0.92669999999999997</v>
       </c>
       <c r="AG366">
-        <v>11.7</v>
+        <v>0.92669999999999997</v>
       </c>
       <c r="AH366">
-        <v>8.6</v>
+        <v>0.92669999999999997</v>
       </c>
       <c r="AI366">
-        <v>8.8000000000000007</v>
+        <v>0.92669999999999997</v>
       </c>
       <c r="AJ366">
-        <v>15.7</v>
+        <v>0.92669999999999997</v>
       </c>
       <c r="AK366">
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="AL366">
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="AM366">
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="AN366">
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="AO366">
         <v>0.92669999999999997</v>
       </c>
       <c r="AP366">
@@ -40409,21 +40829,33 @@
         <v>1</v>
       </c>
       <c r="AF367">
-        <v>8.4</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="AG367">
-        <v>11.7</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="AH367">
-        <v>8.6</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="AI367">
-        <v>8.8000000000000007</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="AJ367">
-        <v>15.7</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="AK367">
+        <v>0.95169999999999999</v>
+      </c>
+      <c r="AL367">
+        <v>0.95169999999999999</v>
+      </c>
+      <c r="AM367">
+        <v>0.95169999999999999</v>
+      </c>
+      <c r="AN367">
+        <v>0.95169999999999999</v>
+      </c>
+      <c r="AO367">
         <v>0.95169999999999999</v>
       </c>
       <c r="AP367">
@@ -40516,21 +40948,33 @@
         <v>1</v>
       </c>
       <c r="AF368">
-        <v>8.4</v>
+        <v>0.97670000000000001</v>
       </c>
       <c r="AG368">
-        <v>11.7</v>
+        <v>0.97670000000000001</v>
       </c>
       <c r="AH368">
-        <v>8.6</v>
+        <v>0.97670000000000001</v>
       </c>
       <c r="AI368">
-        <v>8.8000000000000007</v>
+        <v>0.97670000000000001</v>
       </c>
       <c r="AJ368">
-        <v>15.7</v>
+        <v>0.97670000000000001</v>
       </c>
       <c r="AK368">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="AL368">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="AM368">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="AN368">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="AO368">
         <v>0.97670000000000001</v>
       </c>
       <c r="AP368">
@@ -40623,21 +41067,33 @@
         <v>1</v>
       </c>
       <c r="AF369">
-        <v>8.5</v>
+        <v>1.0017</v>
       </c>
       <c r="AG369">
-        <v>11.85</v>
+        <v>1.0017</v>
       </c>
       <c r="AH369">
-        <v>8.6999999999999993</v>
+        <v>1.0017</v>
       </c>
       <c r="AI369">
-        <v>8.9</v>
+        <v>1.0017</v>
       </c>
       <c r="AJ369">
-        <v>15.9</v>
+        <v>1.0017</v>
       </c>
       <c r="AK369">
+        <v>1.0017</v>
+      </c>
+      <c r="AL369">
+        <v>1.0017</v>
+      </c>
+      <c r="AM369">
+        <v>1.0017</v>
+      </c>
+      <c r="AN369">
+        <v>1.0017</v>
+      </c>
+      <c r="AO369">
         <v>1.0017</v>
       </c>
       <c r="AP369">
@@ -40730,21 +41186,33 @@
         <v>1</v>
       </c>
       <c r="AF370">
-        <v>8.56</v>
+        <v>1.0266999999999999</v>
       </c>
       <c r="AG370">
-        <v>11.94</v>
+        <v>1.0266999999999999</v>
       </c>
       <c r="AH370">
-        <v>8.76</v>
+        <v>1.0266999999999999</v>
       </c>
       <c r="AI370">
-        <v>8.9600000000000009</v>
+        <v>1.0266999999999999</v>
       </c>
       <c r="AJ370">
-        <v>16.02</v>
+        <v>1.0266999999999999</v>
       </c>
       <c r="AK370">
+        <v>1.0266999999999999</v>
+      </c>
+      <c r="AL370">
+        <v>1.0266999999999999</v>
+      </c>
+      <c r="AM370">
+        <v>1.0266999999999999</v>
+      </c>
+      <c r="AN370">
+        <v>1.0266999999999999</v>
+      </c>
+      <c r="AO370">
         <v>1.0266999999999999</v>
       </c>
       <c r="AP370">
@@ -40837,21 +41305,33 @@
         <v>1</v>
       </c>
       <c r="AF371">
-        <v>8.6199999999999992</v>
+        <v>1.0517000000000001</v>
       </c>
       <c r="AG371">
-        <v>12.03</v>
+        <v>1.0517000000000001</v>
       </c>
       <c r="AH371">
-        <v>8.82</v>
+        <v>1.0517000000000001</v>
       </c>
       <c r="AI371">
-        <v>9.02</v>
+        <v>1.0517000000000001</v>
       </c>
       <c r="AJ371">
-        <v>16.14</v>
+        <v>1.0517000000000001</v>
       </c>
       <c r="AK371">
+        <v>1.0517000000000001</v>
+      </c>
+      <c r="AL371">
+        <v>1.0517000000000001</v>
+      </c>
+      <c r="AM371">
+        <v>1.0517000000000001</v>
+      </c>
+      <c r="AN371">
+        <v>1.0517000000000001</v>
+      </c>
+      <c r="AO371">
         <v>1.0517000000000001</v>
       </c>
       <c r="AP371">
@@ -40944,21 +41424,33 @@
         <v>1</v>
       </c>
       <c r="AF372">
-        <v>8.68</v>
+        <v>1.0767</v>
       </c>
       <c r="AG372">
-        <v>12.12</v>
+        <v>1.0767</v>
       </c>
       <c r="AH372">
-        <v>8.8800000000000008</v>
+        <v>1.0767</v>
       </c>
       <c r="AI372">
-        <v>9.08</v>
+        <v>1.0767</v>
       </c>
       <c r="AJ372">
-        <v>16.260000000000002</v>
+        <v>1.0767</v>
       </c>
       <c r="AK372">
+        <v>1.0767</v>
+      </c>
+      <c r="AL372">
+        <v>1.0767</v>
+      </c>
+      <c r="AM372">
+        <v>1.0767</v>
+      </c>
+      <c r="AN372">
+        <v>1.0767</v>
+      </c>
+      <c r="AO372">
         <v>1.0767</v>
       </c>
       <c r="AP372">
@@ -41051,21 +41543,33 @@
         <v>1</v>
       </c>
       <c r="AF373">
-        <v>8.74</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="AG373">
-        <v>12.21</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="AH373">
-        <v>8.94</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="AI373">
-        <v>9.14</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="AJ373">
-        <v>16.38</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="AK373">
+        <v>1.1016999999999999</v>
+      </c>
+      <c r="AL373">
+        <v>1.1016999999999999</v>
+      </c>
+      <c r="AM373">
+        <v>1.1016999999999999</v>
+      </c>
+      <c r="AN373">
+        <v>1.1016999999999999</v>
+      </c>
+      <c r="AO373">
         <v>1.1016999999999999</v>
       </c>
       <c r="AP373">
@@ -41158,21 +41662,33 @@
         <v>1</v>
       </c>
       <c r="AF374">
-        <v>8.8000000000000007</v>
+        <v>1.1267</v>
       </c>
       <c r="AG374">
-        <v>12.3</v>
+        <v>1.1267</v>
       </c>
       <c r="AH374">
-        <v>9</v>
+        <v>1.1267</v>
       </c>
       <c r="AI374">
-        <v>9.1999999999999993</v>
+        <v>1.1267</v>
       </c>
       <c r="AJ374">
-        <v>16.5</v>
+        <v>1.1267</v>
       </c>
       <c r="AK374">
+        <v>1.1267</v>
+      </c>
+      <c r="AL374">
+        <v>1.1267</v>
+      </c>
+      <c r="AM374">
+        <v>1.1267</v>
+      </c>
+      <c r="AN374">
+        <v>1.1267</v>
+      </c>
+      <c r="AO374">
         <v>1.1267</v>
       </c>
       <c r="AP374">
@@ -41265,21 +41781,33 @@
         <v>1</v>
       </c>
       <c r="AF375">
-        <v>7.6</v>
+        <v>1.1767000000000001</v>
       </c>
       <c r="AG375">
-        <v>10.5</v>
+        <v>1.1767000000000001</v>
       </c>
       <c r="AH375">
-        <v>7.8</v>
+        <v>1.1767000000000001</v>
       </c>
       <c r="AI375">
-        <v>8</v>
+        <v>1.1767000000000001</v>
       </c>
       <c r="AJ375">
-        <v>14.1</v>
+        <v>1.1767000000000001</v>
       </c>
       <c r="AK375">
+        <v>1.1767000000000001</v>
+      </c>
+      <c r="AL375">
+        <v>1.1767000000000001</v>
+      </c>
+      <c r="AM375">
+        <v>1.1767000000000001</v>
+      </c>
+      <c r="AN375">
+        <v>1.1767000000000001</v>
+      </c>
+      <c r="AO375">
         <v>1.1767000000000001</v>
       </c>
       <c r="AP375">

</xml_diff>